<commit_message>
PROS-5498 - CCRU - KPI template update
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/FT PoS 2018.xlsx
+++ b/Projects/CCRU/Data/FT PoS 2018.xlsx
@@ -31,9 +31,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$161</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$161</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$161</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$161</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$165</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$161</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$161</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$161</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1877,12 +1878,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1943,6 +1938,12 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -2023,19 +2024,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -2094,7 +2088,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2120,10 +2114,7 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -2136,175 +2127,175 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2312,15 +2303,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -2328,131 +2319,131 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2468,23 +2459,23 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2492,79 +2483,79 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="11" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="11" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="10" fillId="11" borderId="2" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="9" fillId="11" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2576,28 +2567,27 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="SAPBEXstdItem" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -2673,20 +2663,25 @@
   </sheetPr>
   <dimension ref="A1:AQ165"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F55" activeCellId="0" sqref="F55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O167" activeCellId="0" sqref="O167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.2591093117409"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.4615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.587044534413"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.3603238866397"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.2591093117409"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.0769230769231"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.2591093117409"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="21.0607287449393"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="35" min="16" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="36" min="36" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="81.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3587,7 +3582,7 @@
       </c>
       <c r="AQ10" s="12"/>
     </row>
-    <row r="11" customFormat="false" ht="26.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="24" t="n">
         <v>10</v>
       </c>
@@ -3623,7 +3618,7 @@
         <v>74</v>
       </c>
       <c r="O11" s="31" t="n">
-        <v>5449000000729</v>
+        <v>5449000008046</v>
       </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="16"/>
@@ -3848,7 +3843,7 @@
       </c>
       <c r="AQ13" s="12"/>
     </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="n">
         <v>13</v>
       </c>
@@ -3884,7 +3879,7 @@
         <v>80</v>
       </c>
       <c r="O14" s="27" t="n">
-        <v>4607042436505</v>
+        <v>5449000000729</v>
       </c>
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
@@ -3935,7 +3930,7 @@
       </c>
       <c r="AQ14" s="12"/>
     </row>
-    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="24" t="n">
         <v>14</v>
       </c>
@@ -3971,7 +3966,7 @@
         <v>82</v>
       </c>
       <c r="O15" s="27" t="n">
-        <v>4607042436109</v>
+        <v>5449000000712</v>
       </c>
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
@@ -4022,7 +4017,7 @@
       </c>
       <c r="AQ15" s="12"/>
     </row>
-    <row r="16" customFormat="false" ht="39.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="42.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="n">
         <v>15</v>
       </c>
@@ -4058,7 +4053,7 @@
         <v>84</v>
       </c>
       <c r="O16" s="31" t="n">
-        <v>5449000000712</v>
+        <v>5449000020987</v>
       </c>
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
@@ -16720,6 +16715,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="108" t="s">
@@ -16754,6 +16752,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -16788,6 +16789,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -17020,6 +17024,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="112" t="s">

</xml_diff>

<commit_message>
CCRU - Targets upload improvement
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/FT PoS 2018.xlsx
+++ b/Projects/CCRU/Data/FT PoS 2018.xlsx
@@ -40,9 +40,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2427" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="538">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -1238,6 +1239,9 @@
   </si>
   <si>
     <t xml:space="preserve">Mixed 1 door, Mixed  1.5 door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scene type</t>
   </si>
   <si>
     <t xml:space="preserve">114
@@ -1858,7 +1862,7 @@
     <numFmt numFmtId="168" formatCode="D\-MMM"/>
     <numFmt numFmtId="169" formatCode="@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1917,6 +1921,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2062,7 +2071,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2223,6 +2232,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2239,7 +2252,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2275,7 +2288,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2287,15 +2300,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2383,19 +2396,19 @@
   </sheetPr>
   <dimension ref="A1:AQ167"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="AI116" activeCellId="0" sqref="AI116"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="AI111" activeCellId="0" sqref="AI111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="39.2753036437247"/>
-    <col collapsed="false" hidden="false" max="31" min="9" style="1" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="16.2834008097166"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="31" min="9" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="16.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="42.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11752,7 +11765,7 @@
       </c>
       <c r="AG110" s="37"/>
       <c r="AH110" s="37"/>
-      <c r="AI110" s="37" t="s">
+      <c r="AI110" s="40" t="s">
         <v>341</v>
       </c>
       <c r="AJ110" s="37" t="s">
@@ -11888,7 +11901,7 @@
       <c r="L112" s="9"/>
       <c r="M112" s="9"/>
       <c r="N112" s="12"/>
-      <c r="O112" s="40" t="s">
+      <c r="O112" s="41" t="s">
         <v>352</v>
       </c>
       <c r="P112" s="27"/>
@@ -11899,15 +11912,15 @@
       </c>
       <c r="T112" s="12"/>
       <c r="U112" s="12"/>
-      <c r="V112" s="40"/>
+      <c r="V112" s="41"/>
       <c r="W112" s="12"/>
       <c r="X112" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="Y112" s="40" t="s">
+      <c r="Y112" s="41" t="s">
         <v>352</v>
       </c>
-      <c r="Z112" s="40"/>
+      <c r="Z112" s="41"/>
       <c r="AA112" s="9"/>
       <c r="AB112" s="12"/>
       <c r="AC112" s="12"/>
@@ -12052,7 +12065,7 @@
       <c r="H114" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="I114" s="41" t="s">
+      <c r="I114" s="42" t="s">
         <v>49</v>
       </c>
       <c r="J114" s="14"/>
@@ -12060,7 +12073,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="9"/>
       <c r="N114" s="12"/>
-      <c r="O114" s="42"/>
+      <c r="O114" s="43"/>
       <c r="P114" s="27"/>
       <c r="Q114" s="27"/>
       <c r="R114" s="9" t="s">
@@ -12082,7 +12095,7 @@
       <c r="AD114" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AE114" s="41" t="s">
+      <c r="AE114" s="42" t="s">
         <v>363</v>
       </c>
       <c r="AF114" s="17" t="n">
@@ -12149,7 +12162,7 @@
       <c r="L115" s="9"/>
       <c r="M115" s="9"/>
       <c r="N115" s="12"/>
-      <c r="O115" s="42"/>
+      <c r="O115" s="43"/>
       <c r="P115" s="27"/>
       <c r="Q115" s="27"/>
       <c r="R115" s="9" t="s">
@@ -12174,7 +12187,7 @@
       <c r="AE115" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="AF115" s="43" t="n">
+      <c r="AF115" s="44" t="n">
         <v>1</v>
       </c>
       <c r="AG115" s="9" t="n">
@@ -12183,7 +12196,9 @@
       <c r="AH115" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AI115" s="37"/>
+      <c r="AI115" s="37" t="s">
+        <v>369</v>
+      </c>
       <c r="AJ115" s="37"/>
       <c r="AK115" s="9"/>
       <c r="AL115" s="9"/>
@@ -12194,7 +12209,7 @@
         <v>113</v>
       </c>
       <c r="AO115" s="13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AP115" s="33" t="s">
         <v>361</v>
@@ -12219,10 +12234,10 @@
       </c>
       <c r="F116" s="12"/>
       <c r="G116" s="9" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="H116" s="9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="I116" s="14" t="s">
         <v>54</v>
@@ -12304,10 +12319,10 @@
       </c>
       <c r="F117" s="12"/>
       <c r="G117" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H117" s="9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="I117" s="14" t="s">
         <v>54</v>
@@ -12389,10 +12404,10 @@
       </c>
       <c r="F118" s="12"/>
       <c r="G118" s="9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="H118" s="9" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="I118" s="14" t="s">
         <v>54</v>
@@ -12474,10 +12489,10 @@
       </c>
       <c r="F119" s="12"/>
       <c r="G119" s="9" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H119" s="9" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="I119" s="14" t="s">
         <v>54</v>
@@ -12559,10 +12574,10 @@
       </c>
       <c r="F120" s="12"/>
       <c r="G120" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H120" s="9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I120" s="14" t="s">
         <v>54</v>
@@ -12644,10 +12659,10 @@
       </c>
       <c r="F121" s="12"/>
       <c r="G121" s="9" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H121" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I121" s="14" t="s">
         <v>54</v>
@@ -12729,10 +12744,10 @@
       </c>
       <c r="F122" s="12"/>
       <c r="G122" s="9" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H122" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="I122" s="14" t="s">
         <v>54</v>
@@ -12814,10 +12829,10 @@
       </c>
       <c r="F123" s="12"/>
       <c r="G123" s="9" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="H123" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="I123" s="14" t="s">
         <v>54</v>
@@ -12899,10 +12914,10 @@
       </c>
       <c r="F124" s="12"/>
       <c r="G124" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="H124" s="9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I124" s="14" t="s">
         <v>54</v>
@@ -12984,10 +12999,10 @@
       </c>
       <c r="F125" s="12"/>
       <c r="G125" s="9" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H125" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="I125" s="14" t="s">
         <v>54</v>
@@ -13069,10 +13084,10 @@
       </c>
       <c r="F126" s="12"/>
       <c r="G126" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="H126" s="9" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="I126" s="14" t="s">
         <v>54</v>
@@ -13154,10 +13169,10 @@
       </c>
       <c r="F127" s="12"/>
       <c r="G127" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="H127" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="I127" s="14" t="s">
         <v>54</v>
@@ -13169,10 +13184,10 @@
       <c r="L127" s="9"/>
       <c r="M127" s="9"/>
       <c r="N127" s="12" t="s">
-        <v>394</v>
-      </c>
-      <c r="O127" s="44" t="s">
         <v>395</v>
+      </c>
+      <c r="O127" s="45" t="s">
+        <v>396</v>
       </c>
       <c r="P127" s="27"/>
       <c r="Q127" s="27"/>
@@ -13239,10 +13254,10 @@
       </c>
       <c r="F128" s="12"/>
       <c r="G128" s="9" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="H128" s="9" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="I128" s="14" t="s">
         <v>54</v>
@@ -13254,10 +13269,10 @@
       <c r="L128" s="9"/>
       <c r="M128" s="9"/>
       <c r="N128" s="12" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="O128" s="27" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P128" s="27"/>
       <c r="Q128" s="27"/>
@@ -13324,10 +13339,10 @@
       </c>
       <c r="F129" s="12"/>
       <c r="G129" s="9" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="H129" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="I129" s="14" t="s">
         <v>54</v>
@@ -13409,10 +13424,10 @@
       </c>
       <c r="F130" s="12"/>
       <c r="G130" s="9" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="H130" s="9" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="I130" s="14" t="s">
         <v>54</v>
@@ -13494,10 +13509,10 @@
       </c>
       <c r="F131" s="12"/>
       <c r="G131" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="H131" s="9" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="I131" s="14" t="s">
         <v>54</v>
@@ -13579,10 +13594,10 @@
       </c>
       <c r="F132" s="12"/>
       <c r="G132" s="9" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="H132" s="9" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>256</v>
@@ -13594,7 +13609,7 @@
       <c r="L132" s="9"/>
       <c r="M132" s="9"/>
       <c r="N132" s="12"/>
-      <c r="O132" s="42"/>
+      <c r="O132" s="43"/>
       <c r="P132" s="27"/>
       <c r="Q132" s="27"/>
       <c r="R132" s="9" t="s">
@@ -13607,7 +13622,7 @@
       <c r="W132" s="12"/>
       <c r="X132" s="9"/>
       <c r="Y132" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z132" s="12"/>
       <c r="AA132" s="9"/>
@@ -13619,7 +13634,7 @@
       <c r="AE132" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="AF132" s="43" t="n">
+      <c r="AF132" s="44" t="n">
         <v>0.5</v>
       </c>
       <c r="AG132" s="9" t="n">
@@ -13628,7 +13643,9 @@
       <c r="AH132" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AI132" s="37"/>
+      <c r="AI132" s="37" t="s">
+        <v>369</v>
+      </c>
       <c r="AJ132" s="37"/>
       <c r="AK132" s="9"/>
       <c r="AL132" s="9"/>
@@ -13639,7 +13656,7 @@
         <v>130</v>
       </c>
       <c r="AO132" s="13" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AP132" s="33" t="s">
         <v>361</v>
@@ -13664,10 +13681,10 @@
       </c>
       <c r="F133" s="12"/>
       <c r="G133" s="9" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H133" s="9" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="I133" s="14" t="s">
         <v>54</v>
@@ -13698,7 +13715,7 @@
       <c r="W133" s="12"/>
       <c r="X133" s="9"/>
       <c r="Y133" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z133" s="12"/>
       <c r="AA133" s="9"/>
@@ -13727,7 +13744,7 @@
       </c>
       <c r="AO133" s="12"/>
       <c r="AP133" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ133" s="12"/>
     </row>
@@ -13749,10 +13766,10 @@
       </c>
       <c r="F134" s="12"/>
       <c r="G134" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="H134" s="9" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="I134" s="14" t="s">
         <v>54</v>
@@ -13783,7 +13800,7 @@
       <c r="W134" s="12"/>
       <c r="X134" s="9"/>
       <c r="Y134" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z134" s="12"/>
       <c r="AA134" s="9"/>
@@ -13812,7 +13829,7 @@
       </c>
       <c r="AO134" s="12"/>
       <c r="AP134" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ134" s="12"/>
     </row>
@@ -13834,10 +13851,10 @@
       </c>
       <c r="F135" s="12"/>
       <c r="G135" s="9" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="H135" s="9" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="I135" s="14" t="s">
         <v>54</v>
@@ -13868,7 +13885,7 @@
       <c r="W135" s="12"/>
       <c r="X135" s="9"/>
       <c r="Y135" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z135" s="12"/>
       <c r="AA135" s="9"/>
@@ -13897,7 +13914,7 @@
       </c>
       <c r="AO135" s="12"/>
       <c r="AP135" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ135" s="12"/>
     </row>
@@ -13919,10 +13936,10 @@
       </c>
       <c r="F136" s="12"/>
       <c r="G136" s="9" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="H136" s="9" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="I136" s="14" t="s">
         <v>54</v>
@@ -13953,7 +13970,7 @@
       <c r="W136" s="12"/>
       <c r="X136" s="9"/>
       <c r="Y136" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z136" s="12"/>
       <c r="AA136" s="9"/>
@@ -13982,7 +13999,7 @@
       </c>
       <c r="AO136" s="12"/>
       <c r="AP136" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ136" s="12"/>
     </row>
@@ -14004,10 +14021,10 @@
       </c>
       <c r="F137" s="12"/>
       <c r="G137" s="9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="H137" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="I137" s="14" t="s">
         <v>54</v>
@@ -14038,7 +14055,7 @@
       <c r="W137" s="12"/>
       <c r="X137" s="9"/>
       <c r="Y137" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z137" s="12"/>
       <c r="AA137" s="9"/>
@@ -14067,7 +14084,7 @@
       </c>
       <c r="AO137" s="12"/>
       <c r="AP137" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ137" s="12"/>
     </row>
@@ -14089,10 +14106,10 @@
       </c>
       <c r="F138" s="12"/>
       <c r="G138" s="9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="H138" s="9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="I138" s="14" t="s">
         <v>54</v>
@@ -14123,7 +14140,7 @@
       <c r="W138" s="12"/>
       <c r="X138" s="9"/>
       <c r="Y138" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z138" s="12"/>
       <c r="AA138" s="9"/>
@@ -14152,7 +14169,7 @@
       </c>
       <c r="AO138" s="12"/>
       <c r="AP138" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ138" s="12"/>
     </row>
@@ -14174,10 +14191,10 @@
       </c>
       <c r="F139" s="12"/>
       <c r="G139" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="H139" s="9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="I139" s="14" t="s">
         <v>54</v>
@@ -14208,7 +14225,7 @@
       <c r="W139" s="12"/>
       <c r="X139" s="9"/>
       <c r="Y139" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z139" s="12"/>
       <c r="AA139" s="9"/>
@@ -14237,7 +14254,7 @@
       </c>
       <c r="AO139" s="12"/>
       <c r="AP139" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ139" s="12"/>
     </row>
@@ -14259,10 +14276,10 @@
       </c>
       <c r="F140" s="12"/>
       <c r="G140" s="9" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H140" s="9" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="I140" s="14" t="s">
         <v>54</v>
@@ -14293,7 +14310,7 @@
       <c r="W140" s="12"/>
       <c r="X140" s="9"/>
       <c r="Y140" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z140" s="12"/>
       <c r="AA140" s="9"/>
@@ -14322,7 +14339,7 @@
       </c>
       <c r="AO140" s="12"/>
       <c r="AP140" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ140" s="12"/>
     </row>
@@ -14344,10 +14361,10 @@
       </c>
       <c r="F141" s="12"/>
       <c r="G141" s="9" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="H141" s="9" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="I141" s="14" t="s">
         <v>54</v>
@@ -14378,7 +14395,7 @@
       <c r="W141" s="12"/>
       <c r="X141" s="9"/>
       <c r="Y141" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z141" s="12"/>
       <c r="AA141" s="9"/>
@@ -14407,7 +14424,7 @@
       </c>
       <c r="AO141" s="12"/>
       <c r="AP141" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ141" s="12"/>
     </row>
@@ -14429,10 +14446,10 @@
       </c>
       <c r="F142" s="12"/>
       <c r="G142" s="9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="H142" s="9" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="I142" s="14" t="s">
         <v>54</v>
@@ -14463,7 +14480,7 @@
       <c r="W142" s="12"/>
       <c r="X142" s="9"/>
       <c r="Y142" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z142" s="12"/>
       <c r="AA142" s="9"/>
@@ -14492,7 +14509,7 @@
       </c>
       <c r="AO142" s="12"/>
       <c r="AP142" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ142" s="12"/>
     </row>
@@ -14514,10 +14531,10 @@
       </c>
       <c r="F143" s="12"/>
       <c r="G143" s="9" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H143" s="9" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="I143" s="14" t="s">
         <v>54</v>
@@ -14548,7 +14565,7 @@
       <c r="W143" s="12"/>
       <c r="X143" s="9"/>
       <c r="Y143" s="37" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Z143" s="12"/>
       <c r="AA143" s="9"/>
@@ -14577,7 +14594,7 @@
       </c>
       <c r="AO143" s="12"/>
       <c r="AP143" s="33" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="AQ143" s="12"/>
     </row>
@@ -14599,10 +14616,10 @@
       </c>
       <c r="F144" s="12"/>
       <c r="G144" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="H144" s="9" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>256</v>
@@ -14614,7 +14631,7 @@
       <c r="L144" s="9"/>
       <c r="M144" s="9"/>
       <c r="N144" s="12"/>
-      <c r="O144" s="42"/>
+      <c r="O144" s="43"/>
       <c r="P144" s="27"/>
       <c r="Q144" s="27"/>
       <c r="R144" s="9" t="s">
@@ -14627,7 +14644,7 @@
       <c r="W144" s="12"/>
       <c r="X144" s="9"/>
       <c r="Y144" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z144" s="12"/>
       <c r="AA144" s="9"/>
@@ -14639,7 +14656,7 @@
       <c r="AE144" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="AF144" s="43" t="n">
+      <c r="AF144" s="44" t="n">
         <v>0.5</v>
       </c>
       <c r="AG144" s="9" t="n">
@@ -14648,7 +14665,9 @@
       <c r="AH144" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AI144" s="37"/>
+      <c r="AI144" s="37" t="s">
+        <v>369</v>
+      </c>
       <c r="AJ144" s="37"/>
       <c r="AK144" s="9"/>
       <c r="AL144" s="9"/>
@@ -14659,7 +14678,7 @@
         <v>142</v>
       </c>
       <c r="AO144" s="13" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="AP144" s="33" t="s">
         <v>361</v>
@@ -14684,10 +14703,10 @@
       </c>
       <c r="F145" s="12"/>
       <c r="G145" s="9" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="H145" s="9" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="I145" s="14" t="s">
         <v>54</v>
@@ -14718,7 +14737,7 @@
       <c r="W145" s="12"/>
       <c r="X145" s="9"/>
       <c r="Y145" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z145" s="12"/>
       <c r="AA145" s="9"/>
@@ -14747,7 +14766,7 @@
       </c>
       <c r="AO145" s="12"/>
       <c r="AP145" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ145" s="12"/>
     </row>
@@ -14769,10 +14788,10 @@
       </c>
       <c r="F146" s="12"/>
       <c r="G146" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="H146" s="9" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="I146" s="14" t="s">
         <v>54</v>
@@ -14803,7 +14822,7 @@
       <c r="W146" s="12"/>
       <c r="X146" s="9"/>
       <c r="Y146" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z146" s="12"/>
       <c r="AA146" s="9"/>
@@ -14832,7 +14851,7 @@
       </c>
       <c r="AO146" s="12"/>
       <c r="AP146" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ146" s="12"/>
     </row>
@@ -14854,10 +14873,10 @@
       </c>
       <c r="F147" s="12"/>
       <c r="G147" s="9" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="H147" s="9" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="I147" s="14" t="s">
         <v>54</v>
@@ -14888,7 +14907,7 @@
       <c r="W147" s="12"/>
       <c r="X147" s="9"/>
       <c r="Y147" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z147" s="12"/>
       <c r="AA147" s="9"/>
@@ -14917,7 +14936,7 @@
       </c>
       <c r="AO147" s="12"/>
       <c r="AP147" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ147" s="12"/>
     </row>
@@ -14939,10 +14958,10 @@
       </c>
       <c r="F148" s="12"/>
       <c r="G148" s="9" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="H148" s="9" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="I148" s="14" t="s">
         <v>54</v>
@@ -14973,7 +14992,7 @@
       <c r="W148" s="12"/>
       <c r="X148" s="9"/>
       <c r="Y148" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z148" s="12"/>
       <c r="AA148" s="9"/>
@@ -15002,7 +15021,7 @@
       </c>
       <c r="AO148" s="12"/>
       <c r="AP148" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ148" s="12"/>
     </row>
@@ -15024,10 +15043,10 @@
       </c>
       <c r="F149" s="12"/>
       <c r="G149" s="9" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H149" s="9" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="I149" s="14" t="s">
         <v>54</v>
@@ -15058,7 +15077,7 @@
       <c r="W149" s="12"/>
       <c r="X149" s="9"/>
       <c r="Y149" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z149" s="12"/>
       <c r="AA149" s="9"/>
@@ -15087,7 +15106,7 @@
       </c>
       <c r="AO149" s="12"/>
       <c r="AP149" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ149" s="12"/>
     </row>
@@ -15109,10 +15128,10 @@
       </c>
       <c r="F150" s="12"/>
       <c r="G150" s="9" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="H150" s="9" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="I150" s="14" t="s">
         <v>54</v>
@@ -15124,10 +15143,10 @@
       <c r="L150" s="9"/>
       <c r="M150" s="9"/>
       <c r="N150" s="12" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="O150" s="10" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="P150" s="27"/>
       <c r="Q150" s="27"/>
@@ -15143,7 +15162,7 @@
       <c r="W150" s="12"/>
       <c r="X150" s="9"/>
       <c r="Y150" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z150" s="12"/>
       <c r="AA150" s="9"/>
@@ -15172,7 +15191,7 @@
       </c>
       <c r="AO150" s="12"/>
       <c r="AP150" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ150" s="12"/>
     </row>
@@ -15194,10 +15213,10 @@
       </c>
       <c r="F151" s="12"/>
       <c r="G151" s="9" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="H151" s="9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="I151" s="14" t="s">
         <v>54</v>
@@ -15209,10 +15228,10 @@
       <c r="L151" s="9"/>
       <c r="M151" s="9"/>
       <c r="N151" s="12" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="O151" s="10" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="P151" s="27"/>
       <c r="Q151" s="27"/>
@@ -15228,7 +15247,7 @@
       <c r="W151" s="12"/>
       <c r="X151" s="9"/>
       <c r="Y151" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z151" s="12"/>
       <c r="AA151" s="9"/>
@@ -15257,7 +15276,7 @@
       </c>
       <c r="AO151" s="12"/>
       <c r="AP151" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ151" s="12"/>
     </row>
@@ -15279,10 +15298,10 @@
       </c>
       <c r="F152" s="12"/>
       <c r="G152" s="9" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H152" s="9" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="I152" s="14" t="s">
         <v>54</v>
@@ -15294,10 +15313,10 @@
       <c r="L152" s="9"/>
       <c r="M152" s="9"/>
       <c r="N152" s="12" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="O152" s="10" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="P152" s="27"/>
       <c r="Q152" s="27"/>
@@ -15313,7 +15332,7 @@
       <c r="W152" s="12"/>
       <c r="X152" s="9"/>
       <c r="Y152" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z152" s="12"/>
       <c r="AA152" s="9"/>
@@ -15342,7 +15361,7 @@
       </c>
       <c r="AO152" s="12"/>
       <c r="AP152" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ152" s="12"/>
     </row>
@@ -15364,10 +15383,10 @@
       </c>
       <c r="F153" s="12"/>
       <c r="G153" s="9" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="H153" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="I153" s="14" t="s">
         <v>54</v>
@@ -15398,7 +15417,7 @@
       <c r="W153" s="12"/>
       <c r="X153" s="9"/>
       <c r="Y153" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z153" s="12"/>
       <c r="AA153" s="9"/>
@@ -15427,7 +15446,7 @@
       </c>
       <c r="AO153" s="12"/>
       <c r="AP153" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ153" s="12"/>
     </row>
@@ -15449,10 +15468,10 @@
       </c>
       <c r="F154" s="12"/>
       <c r="G154" s="9" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="H154" s="9" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="I154" s="14" t="s">
         <v>54</v>
@@ -15464,10 +15483,10 @@
       <c r="L154" s="9"/>
       <c r="M154" s="9"/>
       <c r="N154" s="12" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="O154" s="10" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="P154" s="27"/>
       <c r="Q154" s="27"/>
@@ -15483,7 +15502,7 @@
       <c r="W154" s="12"/>
       <c r="X154" s="9"/>
       <c r="Y154" s="37" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="Z154" s="12"/>
       <c r="AA154" s="9"/>
@@ -15512,7 +15531,7 @@
       </c>
       <c r="AO154" s="12"/>
       <c r="AP154" s="33" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AQ154" s="12"/>
     </row>
@@ -15534,13 +15553,13 @@
       </c>
       <c r="F155" s="12"/>
       <c r="G155" s="9" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="H155" s="12" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="I155" s="14" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="J155" s="14"/>
       <c r="K155" s="9"/>
@@ -15610,67 +15629,67 @@
         <v>44</v>
       </c>
       <c r="D156" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E156" s="45" t="s">
         <v>465</v>
       </c>
-      <c r="F156" s="45" t="s">
+      <c r="E156" s="46" t="s">
         <v>466</v>
+      </c>
+      <c r="F156" s="46" t="s">
+        <v>467</v>
       </c>
       <c r="G156" s="33" t="s">
         <v>308</v>
       </c>
-      <c r="H156" s="46" t="s">
-        <v>467</v>
-      </c>
-      <c r="I156" s="47" t="s">
+      <c r="H156" s="47" t="s">
         <v>468</v>
       </c>
-      <c r="J156" s="47" t="s">
+      <c r="I156" s="48" t="s">
         <v>469</v>
       </c>
-      <c r="K156" s="47"/>
-      <c r="L156" s="47"/>
+      <c r="J156" s="48" t="s">
+        <v>470</v>
+      </c>
+      <c r="K156" s="48"/>
+      <c r="L156" s="48"/>
       <c r="M156" s="21"/>
       <c r="N156" s="21"/>
-      <c r="O156" s="47"/>
-      <c r="P156" s="47"/>
-      <c r="Q156" s="47"/>
-      <c r="R156" s="47"/>
-      <c r="S156" s="47" t="s">
-        <v>470</v>
-      </c>
-      <c r="T156" s="47"/>
-      <c r="U156" s="47"/>
-      <c r="V156" s="47"/>
-      <c r="W156" s="47"/>
-      <c r="X156" s="47"/>
-      <c r="Y156" s="47"/>
-      <c r="Z156" s="47"/>
-      <c r="AA156" s="47"/>
-      <c r="AB156" s="47"/>
-      <c r="AC156" s="47"/>
-      <c r="AD156" s="47"/>
-      <c r="AE156" s="47"/>
-      <c r="AF156" s="48" t="n">
+      <c r="O156" s="48"/>
+      <c r="P156" s="48"/>
+      <c r="Q156" s="48"/>
+      <c r="R156" s="48"/>
+      <c r="S156" s="48" t="s">
+        <v>471</v>
+      </c>
+      <c r="T156" s="48"/>
+      <c r="U156" s="48"/>
+      <c r="V156" s="48"/>
+      <c r="W156" s="48"/>
+      <c r="X156" s="48"/>
+      <c r="Y156" s="48"/>
+      <c r="Z156" s="48"/>
+      <c r="AA156" s="48"/>
+      <c r="AB156" s="48"/>
+      <c r="AC156" s="48"/>
+      <c r="AD156" s="48"/>
+      <c r="AE156" s="48"/>
+      <c r="AF156" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="AG156" s="47"/>
-      <c r="AH156" s="47"/>
-      <c r="AI156" s="47"/>
-      <c r="AJ156" s="47"/>
-      <c r="AK156" s="47"/>
-      <c r="AL156" s="47"/>
-      <c r="AM156" s="47"/>
+      <c r="AG156" s="48"/>
+      <c r="AH156" s="48"/>
+      <c r="AI156" s="48"/>
+      <c r="AJ156" s="48"/>
+      <c r="AK156" s="48"/>
+      <c r="AL156" s="48"/>
+      <c r="AM156" s="48"/>
       <c r="AN156" s="12" t="n">
         <v>154</v>
       </c>
-      <c r="AO156" s="47" t="n">
+      <c r="AO156" s="48" t="n">
         <v>101</v>
       </c>
-      <c r="AP156" s="47"/>
-      <c r="AQ156" s="47"/>
+      <c r="AP156" s="48"/>
+      <c r="AQ156" s="48"/>
     </row>
     <row r="157" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A157" s="37" t="n">
@@ -15683,65 +15702,65 @@
         <v>44</v>
       </c>
       <c r="D157" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E157" s="45" t="s">
-        <v>471</v>
-      </c>
-      <c r="F157" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E157" s="46" t="s">
         <v>472</v>
       </c>
-      <c r="G157" s="45" t="s">
+      <c r="F157" s="46" t="s">
+        <v>473</v>
+      </c>
+      <c r="G157" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="H157" s="46"/>
-      <c r="I157" s="47" t="s">
-        <v>473</v>
-      </c>
-      <c r="J157" s="47" t="s">
+      <c r="H157" s="47"/>
+      <c r="I157" s="48" t="s">
         <v>474</v>
       </c>
-      <c r="K157" s="47"/>
-      <c r="L157" s="47"/>
+      <c r="J157" s="48" t="s">
+        <v>475</v>
+      </c>
+      <c r="K157" s="48"/>
+      <c r="L157" s="48"/>
       <c r="M157" s="21"/>
       <c r="N157" s="21"/>
-      <c r="O157" s="47"/>
-      <c r="P157" s="47"/>
-      <c r="Q157" s="47"/>
-      <c r="R157" s="47"/>
-      <c r="S157" s="47" t="s">
-        <v>470</v>
-      </c>
-      <c r="T157" s="47"/>
-      <c r="U157" s="47"/>
-      <c r="V157" s="47"/>
-      <c r="W157" s="47"/>
-      <c r="X157" s="47"/>
-      <c r="Y157" s="47"/>
-      <c r="Z157" s="47"/>
-      <c r="AA157" s="47"/>
-      <c r="AB157" s="47"/>
-      <c r="AC157" s="47"/>
-      <c r="AD157" s="47"/>
-      <c r="AE157" s="47"/>
-      <c r="AF157" s="48" t="n">
+      <c r="O157" s="48"/>
+      <c r="P157" s="48"/>
+      <c r="Q157" s="48"/>
+      <c r="R157" s="48"/>
+      <c r="S157" s="48" t="s">
+        <v>471</v>
+      </c>
+      <c r="T157" s="48"/>
+      <c r="U157" s="48"/>
+      <c r="V157" s="48"/>
+      <c r="W157" s="48"/>
+      <c r="X157" s="48"/>
+      <c r="Y157" s="48"/>
+      <c r="Z157" s="48"/>
+      <c r="AA157" s="48"/>
+      <c r="AB157" s="48"/>
+      <c r="AC157" s="48"/>
+      <c r="AD157" s="48"/>
+      <c r="AE157" s="48"/>
+      <c r="AF157" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="AG157" s="47"/>
-      <c r="AH157" s="47"/>
-      <c r="AI157" s="47"/>
-      <c r="AJ157" s="47"/>
-      <c r="AK157" s="47"/>
-      <c r="AL157" s="47"/>
-      <c r="AM157" s="47"/>
+      <c r="AG157" s="48"/>
+      <c r="AH157" s="48"/>
+      <c r="AI157" s="48"/>
+      <c r="AJ157" s="48"/>
+      <c r="AK157" s="48"/>
+      <c r="AL157" s="48"/>
+      <c r="AM157" s="48"/>
       <c r="AN157" s="12" t="n">
         <v>155</v>
       </c>
       <c r="AO157" s="21" t="s">
-        <v>475</v>
-      </c>
-      <c r="AP157" s="47"/>
-      <c r="AQ157" s="47"/>
+        <v>476</v>
+      </c>
+      <c r="AP157" s="48"/>
+      <c r="AQ157" s="48"/>
     </row>
     <row r="158" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A158" s="37" t="n">
@@ -15754,67 +15773,67 @@
         <v>44</v>
       </c>
       <c r="D158" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E158" s="45" t="s">
-        <v>476</v>
-      </c>
-      <c r="F158" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E158" s="46" t="s">
         <v>477</v>
       </c>
-      <c r="G158" s="45" t="s">
+      <c r="F158" s="46" t="s">
+        <v>478</v>
+      </c>
+      <c r="G158" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="H158" s="46" t="s">
-        <v>478</v>
-      </c>
-      <c r="I158" s="47" t="s">
-        <v>468</v>
-      </c>
-      <c r="J158" s="47" t="s">
-        <v>474</v>
-      </c>
-      <c r="K158" s="47"/>
-      <c r="L158" s="47"/>
+      <c r="H158" s="47" t="s">
+        <v>479</v>
+      </c>
+      <c r="I158" s="48" t="s">
+        <v>469</v>
+      </c>
+      <c r="J158" s="48" t="s">
+        <v>475</v>
+      </c>
+      <c r="K158" s="48"/>
+      <c r="L158" s="48"/>
       <c r="M158" s="21"/>
       <c r="N158" s="21"/>
-      <c r="O158" s="47"/>
-      <c r="P158" s="47"/>
-      <c r="Q158" s="47"/>
-      <c r="R158" s="47"/>
-      <c r="S158" s="47" t="s">
-        <v>470</v>
-      </c>
-      <c r="T158" s="47"/>
-      <c r="U158" s="47"/>
-      <c r="V158" s="47"/>
-      <c r="W158" s="47"/>
-      <c r="X158" s="47"/>
-      <c r="Y158" s="47"/>
-      <c r="Z158" s="47"/>
-      <c r="AA158" s="47"/>
-      <c r="AB158" s="47"/>
-      <c r="AC158" s="47"/>
-      <c r="AD158" s="47"/>
-      <c r="AE158" s="47"/>
-      <c r="AF158" s="48" t="n">
+      <c r="O158" s="48"/>
+      <c r="P158" s="48"/>
+      <c r="Q158" s="48"/>
+      <c r="R158" s="48"/>
+      <c r="S158" s="48" t="s">
+        <v>471</v>
+      </c>
+      <c r="T158" s="48"/>
+      <c r="U158" s="48"/>
+      <c r="V158" s="48"/>
+      <c r="W158" s="48"/>
+      <c r="X158" s="48"/>
+      <c r="Y158" s="48"/>
+      <c r="Z158" s="48"/>
+      <c r="AA158" s="48"/>
+      <c r="AB158" s="48"/>
+      <c r="AC158" s="48"/>
+      <c r="AD158" s="48"/>
+      <c r="AE158" s="48"/>
+      <c r="AF158" s="49" t="n">
         <v>0</v>
       </c>
-      <c r="AG158" s="47"/>
-      <c r="AH158" s="47"/>
-      <c r="AI158" s="47"/>
-      <c r="AJ158" s="47"/>
-      <c r="AK158" s="47"/>
-      <c r="AL158" s="47"/>
-      <c r="AM158" s="47"/>
+      <c r="AG158" s="48"/>
+      <c r="AH158" s="48"/>
+      <c r="AI158" s="48"/>
+      <c r="AJ158" s="48"/>
+      <c r="AK158" s="48"/>
+      <c r="AL158" s="48"/>
+      <c r="AM158" s="48"/>
       <c r="AN158" s="12" t="n">
         <v>156</v>
       </c>
-      <c r="AO158" s="47" t="n">
+      <c r="AO158" s="48" t="n">
         <v>105</v>
       </c>
-      <c r="AP158" s="47"/>
-      <c r="AQ158" s="47"/>
+      <c r="AP158" s="48"/>
+      <c r="AQ158" s="48"/>
     </row>
     <row r="159" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A159" s="37" t="n">
@@ -15827,69 +15846,69 @@
         <v>44</v>
       </c>
       <c r="D159" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E159" s="45" t="s">
-        <v>479</v>
-      </c>
-      <c r="F159" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E159" s="46" t="s">
         <v>480</v>
       </c>
-      <c r="G159" s="45" t="s">
+      <c r="F159" s="46" t="s">
         <v>481</v>
       </c>
-      <c r="H159" s="47"/>
+      <c r="G159" s="46" t="s">
+        <v>482</v>
+      </c>
+      <c r="H159" s="48"/>
       <c r="I159" s="21" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="J159" s="21" t="s">
-        <v>474</v>
-      </c>
-      <c r="K159" s="47"/>
-      <c r="L159" s="47"/>
+        <v>475</v>
+      </c>
+      <c r="K159" s="48"/>
+      <c r="L159" s="48"/>
       <c r="M159" s="21"/>
       <c r="N159" s="21"/>
-      <c r="O159" s="47" t="s">
-        <v>483</v>
-      </c>
-      <c r="P159" s="47"/>
-      <c r="Q159" s="47"/>
-      <c r="R159" s="47"/>
-      <c r="S159" s="47" t="s">
+      <c r="O159" s="48" t="s">
         <v>484</v>
       </c>
-      <c r="T159" s="47"/>
-      <c r="U159" s="47"/>
-      <c r="V159" s="47"/>
-      <c r="W159" s="47"/>
-      <c r="X159" s="49" t="s">
+      <c r="P159" s="48"/>
+      <c r="Q159" s="48"/>
+      <c r="R159" s="48"/>
+      <c r="S159" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T159" s="48"/>
+      <c r="U159" s="48"/>
+      <c r="V159" s="48"/>
+      <c r="W159" s="48"/>
+      <c r="X159" s="50" t="s">
         <v>339</v>
       </c>
-      <c r="Y159" s="50" t="s">
-        <v>485</v>
-      </c>
-      <c r="Z159" s="47"/>
-      <c r="AA159" s="47"/>
-      <c r="AB159" s="47"/>
-      <c r="AC159" s="47"/>
-      <c r="AD159" s="47"/>
-      <c r="AE159" s="47"/>
-      <c r="AF159" s="51" t="n">
+      <c r="Y159" s="51" t="s">
+        <v>486</v>
+      </c>
+      <c r="Z159" s="48"/>
+      <c r="AA159" s="48"/>
+      <c r="AB159" s="48"/>
+      <c r="AC159" s="48"/>
+      <c r="AD159" s="48"/>
+      <c r="AE159" s="48"/>
+      <c r="AF159" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="AG159" s="47"/>
-      <c r="AH159" s="47"/>
-      <c r="AI159" s="47"/>
-      <c r="AJ159" s="47"/>
-      <c r="AK159" s="47"/>
-      <c r="AL159" s="47"/>
-      <c r="AM159" s="47"/>
+      <c r="AG159" s="48"/>
+      <c r="AH159" s="48"/>
+      <c r="AI159" s="48"/>
+      <c r="AJ159" s="48"/>
+      <c r="AK159" s="48"/>
+      <c r="AL159" s="48"/>
+      <c r="AM159" s="48"/>
       <c r="AN159" s="12" t="n">
         <v>157</v>
       </c>
-      <c r="AO159" s="47"/>
-      <c r="AP159" s="47"/>
-      <c r="AQ159" s="47"/>
+      <c r="AO159" s="48"/>
+      <c r="AP159" s="48"/>
+      <c r="AQ159" s="48"/>
     </row>
     <row r="160" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A160" s="37" t="n">
@@ -15902,67 +15921,67 @@
         <v>44</v>
       </c>
       <c r="D160" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E160" s="45" t="s">
-        <v>486</v>
-      </c>
-      <c r="F160" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E160" s="46" t="s">
         <v>487</v>
       </c>
-      <c r="G160" s="45" t="s">
+      <c r="F160" s="46" t="s">
         <v>488</v>
       </c>
-      <c r="H160" s="47"/>
+      <c r="G160" s="46" t="s">
+        <v>489</v>
+      </c>
+      <c r="H160" s="48"/>
       <c r="I160" s="21" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="J160" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="K160" s="47"/>
-      <c r="L160" s="47"/>
+        <v>491</v>
+      </c>
+      <c r="K160" s="48"/>
+      <c r="L160" s="48"/>
       <c r="M160" s="21"/>
       <c r="N160" s="21"/>
-      <c r="O160" s="47" t="s">
+      <c r="O160" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="P160" s="47"/>
-      <c r="Q160" s="47"/>
-      <c r="R160" s="47"/>
-      <c r="S160" s="47" t="s">
-        <v>484</v>
-      </c>
-      <c r="T160" s="47"/>
-      <c r="U160" s="47"/>
-      <c r="V160" s="47"/>
-      <c r="W160" s="47"/>
-      <c r="X160" s="47"/>
+      <c r="P160" s="48"/>
+      <c r="Q160" s="48"/>
+      <c r="R160" s="48"/>
+      <c r="S160" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T160" s="48"/>
+      <c r="U160" s="48"/>
+      <c r="V160" s="48"/>
+      <c r="W160" s="48"/>
+      <c r="X160" s="48"/>
       <c r="Y160" s="21" t="s">
-        <v>491</v>
-      </c>
-      <c r="Z160" s="47"/>
-      <c r="AA160" s="47"/>
-      <c r="AB160" s="47"/>
-      <c r="AC160" s="47"/>
-      <c r="AD160" s="47"/>
-      <c r="AE160" s="47"/>
-      <c r="AF160" s="51" t="n">
+        <v>492</v>
+      </c>
+      <c r="Z160" s="48"/>
+      <c r="AA160" s="48"/>
+      <c r="AB160" s="48"/>
+      <c r="AC160" s="48"/>
+      <c r="AD160" s="48"/>
+      <c r="AE160" s="48"/>
+      <c r="AF160" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="AG160" s="47"/>
-      <c r="AH160" s="47"/>
-      <c r="AI160" s="47"/>
-      <c r="AJ160" s="47"/>
-      <c r="AK160" s="47"/>
-      <c r="AL160" s="47"/>
-      <c r="AM160" s="47"/>
+      <c r="AG160" s="48"/>
+      <c r="AH160" s="48"/>
+      <c r="AI160" s="48"/>
+      <c r="AJ160" s="48"/>
+      <c r="AK160" s="48"/>
+      <c r="AL160" s="48"/>
+      <c r="AM160" s="48"/>
       <c r="AN160" s="12" t="n">
         <v>158</v>
       </c>
-      <c r="AO160" s="47"/>
-      <c r="AP160" s="47"/>
-      <c r="AQ160" s="47"/>
+      <c r="AO160" s="48"/>
+      <c r="AP160" s="48"/>
+      <c r="AQ160" s="48"/>
     </row>
     <row r="161" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A161" s="37" t="n">
@@ -15975,67 +15994,67 @@
         <v>44</v>
       </c>
       <c r="D161" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E161" s="45" t="s">
-        <v>492</v>
-      </c>
-      <c r="F161" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E161" s="46" t="s">
         <v>493</v>
       </c>
-      <c r="G161" s="45" t="s">
+      <c r="F161" s="46" t="s">
         <v>494</v>
       </c>
-      <c r="H161" s="47"/>
+      <c r="G161" s="46" t="s">
+        <v>495</v>
+      </c>
+      <c r="H161" s="48"/>
       <c r="I161" s="21" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="J161" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="K161" s="47"/>
-      <c r="L161" s="47"/>
+        <v>491</v>
+      </c>
+      <c r="K161" s="48"/>
+      <c r="L161" s="48"/>
       <c r="M161" s="21"/>
       <c r="N161" s="21"/>
-      <c r="O161" s="47" t="s">
-        <v>495</v>
-      </c>
-      <c r="P161" s="47"/>
-      <c r="Q161" s="47"/>
-      <c r="R161" s="47"/>
-      <c r="S161" s="47" t="s">
-        <v>484</v>
-      </c>
-      <c r="T161" s="47"/>
-      <c r="U161" s="47"/>
-      <c r="V161" s="47"/>
-      <c r="W161" s="47"/>
-      <c r="X161" s="47"/>
+      <c r="O161" s="48" t="s">
+        <v>496</v>
+      </c>
+      <c r="P161" s="48"/>
+      <c r="Q161" s="48"/>
+      <c r="R161" s="48"/>
+      <c r="S161" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T161" s="48"/>
+      <c r="U161" s="48"/>
+      <c r="V161" s="48"/>
+      <c r="W161" s="48"/>
+      <c r="X161" s="48"/>
       <c r="Y161" s="21" t="s">
-        <v>491</v>
-      </c>
-      <c r="Z161" s="47"/>
-      <c r="AA161" s="47"/>
-      <c r="AB161" s="47"/>
-      <c r="AC161" s="47"/>
-      <c r="AD161" s="47"/>
-      <c r="AE161" s="47"/>
-      <c r="AF161" s="51" t="n">
+        <v>492</v>
+      </c>
+      <c r="Z161" s="48"/>
+      <c r="AA161" s="48"/>
+      <c r="AB161" s="48"/>
+      <c r="AC161" s="48"/>
+      <c r="AD161" s="48"/>
+      <c r="AE161" s="48"/>
+      <c r="AF161" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="AG161" s="47"/>
-      <c r="AH161" s="47"/>
-      <c r="AI161" s="47"/>
-      <c r="AJ161" s="47"/>
-      <c r="AK161" s="47"/>
-      <c r="AL161" s="47"/>
-      <c r="AM161" s="47"/>
+      <c r="AG161" s="48"/>
+      <c r="AH161" s="48"/>
+      <c r="AI161" s="48"/>
+      <c r="AJ161" s="48"/>
+      <c r="AK161" s="48"/>
+      <c r="AL161" s="48"/>
+      <c r="AM161" s="48"/>
       <c r="AN161" s="12" t="n">
         <v>159</v>
       </c>
-      <c r="AO161" s="47"/>
-      <c r="AP161" s="47"/>
-      <c r="AQ161" s="47"/>
+      <c r="AO161" s="48"/>
+      <c r="AP161" s="48"/>
+      <c r="AQ161" s="48"/>
     </row>
     <row r="162" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A162" s="37" t="n">
@@ -16048,67 +16067,67 @@
         <v>44</v>
       </c>
       <c r="D162" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E162" s="45" t="s">
-        <v>496</v>
-      </c>
-      <c r="F162" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E162" s="46" t="s">
         <v>497</v>
       </c>
-      <c r="G162" s="45" t="s">
+      <c r="F162" s="46" t="s">
         <v>498</v>
       </c>
-      <c r="H162" s="47"/>
+      <c r="G162" s="46" t="s">
+        <v>499</v>
+      </c>
+      <c r="H162" s="48"/>
       <c r="I162" s="21" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="J162" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="K162" s="47"/>
-      <c r="L162" s="47"/>
+        <v>491</v>
+      </c>
+      <c r="K162" s="48"/>
+      <c r="L162" s="48"/>
       <c r="M162" s="21"/>
       <c r="N162" s="21"/>
-      <c r="O162" s="47" t="s">
-        <v>499</v>
-      </c>
-      <c r="P162" s="47"/>
-      <c r="Q162" s="47"/>
-      <c r="R162" s="47"/>
-      <c r="S162" s="47" t="s">
-        <v>484</v>
-      </c>
-      <c r="T162" s="47"/>
-      <c r="U162" s="47"/>
-      <c r="V162" s="47"/>
-      <c r="W162" s="47"/>
-      <c r="X162" s="47"/>
+      <c r="O162" s="48" t="s">
+        <v>500</v>
+      </c>
+      <c r="P162" s="48"/>
+      <c r="Q162" s="48"/>
+      <c r="R162" s="48"/>
+      <c r="S162" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T162" s="48"/>
+      <c r="U162" s="48"/>
+      <c r="V162" s="48"/>
+      <c r="W162" s="48"/>
+      <c r="X162" s="48"/>
       <c r="Y162" s="21" t="s">
-        <v>491</v>
-      </c>
-      <c r="Z162" s="47"/>
-      <c r="AA162" s="47"/>
-      <c r="AB162" s="47"/>
-      <c r="AC162" s="47"/>
-      <c r="AD162" s="47"/>
-      <c r="AE162" s="47"/>
-      <c r="AF162" s="51" t="n">
+        <v>492</v>
+      </c>
+      <c r="Z162" s="48"/>
+      <c r="AA162" s="48"/>
+      <c r="AB162" s="48"/>
+      <c r="AC162" s="48"/>
+      <c r="AD162" s="48"/>
+      <c r="AE162" s="48"/>
+      <c r="AF162" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="AG162" s="47"/>
-      <c r="AH162" s="47"/>
-      <c r="AI162" s="47"/>
-      <c r="AJ162" s="47"/>
-      <c r="AK162" s="47"/>
+      <c r="AG162" s="48"/>
+      <c r="AH162" s="48"/>
+      <c r="AI162" s="48"/>
+      <c r="AJ162" s="48"/>
+      <c r="AK162" s="48"/>
       <c r="AL162" s="12"/>
-      <c r="AM162" s="47"/>
+      <c r="AM162" s="48"/>
       <c r="AN162" s="12" t="n">
         <v>160</v>
       </c>
-      <c r="AO162" s="47"/>
-      <c r="AP162" s="47"/>
-      <c r="AQ162" s="47"/>
+      <c r="AO162" s="48"/>
+      <c r="AP162" s="48"/>
+      <c r="AQ162" s="48"/>
     </row>
     <row r="163" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A163" s="37" t="n">
@@ -16121,71 +16140,71 @@
         <v>44</v>
       </c>
       <c r="D163" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E163" s="45" t="s">
-        <v>500</v>
-      </c>
-      <c r="F163" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E163" s="46" t="s">
         <v>501</v>
       </c>
-      <c r="G163" s="45" t="s">
+      <c r="F163" s="46" t="s">
         <v>502</v>
       </c>
-      <c r="H163" s="47" t="s">
+      <c r="G163" s="46" t="s">
+        <v>503</v>
+      </c>
+      <c r="H163" s="48" t="s">
         <v>246</v>
       </c>
       <c r="I163" s="21" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="J163" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="K163" s="47"/>
-      <c r="L163" s="47"/>
+        <v>491</v>
+      </c>
+      <c r="K163" s="48"/>
+      <c r="L163" s="48"/>
       <c r="M163" s="21"/>
       <c r="N163" s="21"/>
       <c r="O163" s="21" t="s">
-        <v>504</v>
-      </c>
-      <c r="P163" s="47"/>
-      <c r="Q163" s="47"/>
-      <c r="R163" s="47"/>
-      <c r="S163" s="47" t="s">
-        <v>484</v>
-      </c>
-      <c r="T163" s="47"/>
-      <c r="U163" s="47"/>
-      <c r="V163" s="47"/>
-      <c r="W163" s="47"/>
-      <c r="X163" s="47"/>
+        <v>505</v>
+      </c>
+      <c r="P163" s="48"/>
+      <c r="Q163" s="48"/>
+      <c r="R163" s="48"/>
+      <c r="S163" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T163" s="48"/>
+      <c r="U163" s="48"/>
+      <c r="V163" s="48"/>
+      <c r="W163" s="48"/>
+      <c r="X163" s="48"/>
       <c r="Y163" s="21" t="s">
-        <v>505</v>
-      </c>
-      <c r="Z163" s="47"/>
-      <c r="AA163" s="47"/>
-      <c r="AB163" s="47"/>
-      <c r="AC163" s="47"/>
-      <c r="AD163" s="47"/>
-      <c r="AE163" s="47"/>
-      <c r="AF163" s="51" t="n">
+        <v>506</v>
+      </c>
+      <c r="Z163" s="48"/>
+      <c r="AA163" s="48"/>
+      <c r="AB163" s="48"/>
+      <c r="AC163" s="48"/>
+      <c r="AD163" s="48"/>
+      <c r="AE163" s="48"/>
+      <c r="AF163" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="AG163" s="47"/>
-      <c r="AH163" s="47"/>
-      <c r="AI163" s="47"/>
-      <c r="AJ163" s="47"/>
-      <c r="AK163" s="47"/>
-      <c r="AL163" s="47"/>
-      <c r="AM163" s="47"/>
+      <c r="AG163" s="48"/>
+      <c r="AH163" s="48"/>
+      <c r="AI163" s="48"/>
+      <c r="AJ163" s="48"/>
+      <c r="AK163" s="48"/>
+      <c r="AL163" s="48"/>
+      <c r="AM163" s="48"/>
       <c r="AN163" s="12" t="n">
         <v>161</v>
       </c>
-      <c r="AO163" s="47" t="n">
+      <c r="AO163" s="48" t="n">
         <v>83</v>
       </c>
-      <c r="AP163" s="47"/>
-      <c r="AQ163" s="47"/>
+      <c r="AP163" s="48"/>
+      <c r="AQ163" s="48"/>
     </row>
     <row r="164" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A164" s="37" t="n">
@@ -16198,71 +16217,71 @@
         <v>44</v>
       </c>
       <c r="D164" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E164" s="45" t="s">
-        <v>500</v>
-      </c>
-      <c r="F164" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E164" s="46" t="s">
         <v>501</v>
       </c>
-      <c r="G164" s="45" t="s">
+      <c r="F164" s="46" t="s">
         <v>502</v>
       </c>
-      <c r="H164" s="47" t="s">
+      <c r="G164" s="46" t="s">
+        <v>503</v>
+      </c>
+      <c r="H164" s="48" t="s">
         <v>274</v>
       </c>
       <c r="I164" s="21" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="J164" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="K164" s="47"/>
-      <c r="L164" s="47"/>
+        <v>491</v>
+      </c>
+      <c r="K164" s="48"/>
+      <c r="L164" s="48"/>
       <c r="M164" s="21"/>
       <c r="N164" s="21"/>
       <c r="O164" s="21" t="s">
-        <v>504</v>
-      </c>
-      <c r="P164" s="47"/>
-      <c r="Q164" s="47"/>
-      <c r="R164" s="47"/>
-      <c r="S164" s="47" t="s">
-        <v>484</v>
-      </c>
-      <c r="T164" s="47"/>
-      <c r="U164" s="47"/>
-      <c r="V164" s="47"/>
-      <c r="W164" s="47"/>
-      <c r="X164" s="47"/>
+        <v>505</v>
+      </c>
+      <c r="P164" s="48"/>
+      <c r="Q164" s="48"/>
+      <c r="R164" s="48"/>
+      <c r="S164" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T164" s="48"/>
+      <c r="U164" s="48"/>
+      <c r="V164" s="48"/>
+      <c r="W164" s="48"/>
+      <c r="X164" s="48"/>
       <c r="Y164" s="21" t="s">
-        <v>506</v>
-      </c>
-      <c r="Z164" s="47"/>
-      <c r="AA164" s="47"/>
-      <c r="AB164" s="47"/>
-      <c r="AC164" s="47"/>
-      <c r="AD164" s="47"/>
-      <c r="AE164" s="47"/>
-      <c r="AF164" s="51" t="n">
+        <v>507</v>
+      </c>
+      <c r="Z164" s="48"/>
+      <c r="AA164" s="48"/>
+      <c r="AB164" s="48"/>
+      <c r="AC164" s="48"/>
+      <c r="AD164" s="48"/>
+      <c r="AE164" s="48"/>
+      <c r="AF164" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="AG164" s="47"/>
-      <c r="AH164" s="47"/>
-      <c r="AI164" s="47"/>
-      <c r="AJ164" s="47"/>
-      <c r="AK164" s="47"/>
-      <c r="AL164" s="47"/>
-      <c r="AM164" s="47"/>
+      <c r="AG164" s="48"/>
+      <c r="AH164" s="48"/>
+      <c r="AI164" s="48"/>
+      <c r="AJ164" s="48"/>
+      <c r="AK164" s="48"/>
+      <c r="AL164" s="48"/>
+      <c r="AM164" s="48"/>
       <c r="AN164" s="12" t="n">
         <v>162</v>
       </c>
-      <c r="AO164" s="47" t="n">
+      <c r="AO164" s="48" t="n">
         <v>91</v>
       </c>
-      <c r="AP164" s="47"/>
-      <c r="AQ164" s="47"/>
+      <c r="AP164" s="48"/>
+      <c r="AQ164" s="48"/>
     </row>
     <row r="165" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A165" s="37" t="n">
@@ -16275,71 +16294,71 @@
         <v>44</v>
       </c>
       <c r="D165" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E165" s="45" t="s">
-        <v>500</v>
-      </c>
-      <c r="F165" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E165" s="46" t="s">
         <v>501</v>
       </c>
-      <c r="G165" s="45" t="s">
+      <c r="F165" s="46" t="s">
         <v>502</v>
       </c>
-      <c r="H165" s="47" t="s">
+      <c r="G165" s="46" t="s">
+        <v>503</v>
+      </c>
+      <c r="H165" s="48" t="s">
         <v>265</v>
       </c>
       <c r="I165" s="21" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="J165" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="K165" s="47"/>
-      <c r="L165" s="47"/>
+        <v>491</v>
+      </c>
+      <c r="K165" s="48"/>
+      <c r="L165" s="48"/>
       <c r="M165" s="21"/>
       <c r="N165" s="21"/>
       <c r="O165" s="21" t="s">
-        <v>504</v>
-      </c>
-      <c r="P165" s="47"/>
-      <c r="Q165" s="47"/>
-      <c r="R165" s="47"/>
-      <c r="S165" s="47" t="s">
-        <v>484</v>
-      </c>
-      <c r="T165" s="47"/>
-      <c r="U165" s="47"/>
-      <c r="V165" s="47"/>
-      <c r="W165" s="47"/>
-      <c r="X165" s="47"/>
+        <v>505</v>
+      </c>
+      <c r="P165" s="48"/>
+      <c r="Q165" s="48"/>
+      <c r="R165" s="48"/>
+      <c r="S165" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T165" s="48"/>
+      <c r="U165" s="48"/>
+      <c r="V165" s="48"/>
+      <c r="W165" s="48"/>
+      <c r="X165" s="48"/>
       <c r="Y165" s="21" t="s">
-        <v>507</v>
-      </c>
-      <c r="Z165" s="47"/>
-      <c r="AA165" s="47"/>
-      <c r="AB165" s="47"/>
-      <c r="AC165" s="47"/>
-      <c r="AD165" s="47"/>
-      <c r="AE165" s="47"/>
-      <c r="AF165" s="51" t="n">
+        <v>508</v>
+      </c>
+      <c r="Z165" s="48"/>
+      <c r="AA165" s="48"/>
+      <c r="AB165" s="48"/>
+      <c r="AC165" s="48"/>
+      <c r="AD165" s="48"/>
+      <c r="AE165" s="48"/>
+      <c r="AF165" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="AG165" s="47"/>
-      <c r="AH165" s="47"/>
-      <c r="AI165" s="47"/>
-      <c r="AJ165" s="47"/>
-      <c r="AK165" s="47"/>
-      <c r="AL165" s="47"/>
-      <c r="AM165" s="47"/>
+      <c r="AG165" s="48"/>
+      <c r="AH165" s="48"/>
+      <c r="AI165" s="48"/>
+      <c r="AJ165" s="48"/>
+      <c r="AK165" s="48"/>
+      <c r="AL165" s="48"/>
+      <c r="AM165" s="48"/>
       <c r="AN165" s="12" t="n">
         <v>163</v>
       </c>
-      <c r="AO165" s="47" t="n">
+      <c r="AO165" s="48" t="n">
         <v>88</v>
       </c>
-      <c r="AP165" s="47"/>
-      <c r="AQ165" s="47"/>
+      <c r="AP165" s="48"/>
+      <c r="AQ165" s="48"/>
     </row>
     <row r="166" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A166" s="37" t="n">
@@ -16352,71 +16371,71 @@
         <v>44</v>
       </c>
       <c r="D166" s="23" t="s">
-        <v>464</v>
-      </c>
-      <c r="E166" s="45" t="s">
-        <v>500</v>
-      </c>
-      <c r="F166" s="45" t="s">
+        <v>465</v>
+      </c>
+      <c r="E166" s="46" t="s">
         <v>501</v>
       </c>
-      <c r="G166" s="45" t="s">
+      <c r="F166" s="46" t="s">
         <v>502</v>
       </c>
-      <c r="H166" s="47" t="s">
+      <c r="G166" s="46" t="s">
+        <v>503</v>
+      </c>
+      <c r="H166" s="48" t="s">
         <v>289</v>
       </c>
       <c r="I166" s="21" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="J166" s="21" t="s">
-        <v>490</v>
-      </c>
-      <c r="K166" s="47"/>
-      <c r="L166" s="47"/>
+        <v>491</v>
+      </c>
+      <c r="K166" s="48"/>
+      <c r="L166" s="48"/>
       <c r="M166" s="21"/>
       <c r="N166" s="21"/>
       <c r="O166" s="21" t="s">
-        <v>504</v>
-      </c>
-      <c r="P166" s="47"/>
-      <c r="Q166" s="47"/>
-      <c r="R166" s="47"/>
-      <c r="S166" s="47" t="s">
-        <v>484</v>
-      </c>
-      <c r="T166" s="47"/>
-      <c r="U166" s="47"/>
-      <c r="V166" s="47"/>
-      <c r="W166" s="47"/>
-      <c r="X166" s="47"/>
+        <v>505</v>
+      </c>
+      <c r="P166" s="48"/>
+      <c r="Q166" s="48"/>
+      <c r="R166" s="48"/>
+      <c r="S166" s="48" t="s">
+        <v>485</v>
+      </c>
+      <c r="T166" s="48"/>
+      <c r="U166" s="48"/>
+      <c r="V166" s="48"/>
+      <c r="W166" s="48"/>
+      <c r="X166" s="48"/>
       <c r="Y166" s="21" t="s">
-        <v>508</v>
-      </c>
-      <c r="Z166" s="47"/>
-      <c r="AA166" s="47"/>
-      <c r="AB166" s="47"/>
-      <c r="AC166" s="47"/>
-      <c r="AD166" s="47"/>
-      <c r="AE166" s="47"/>
-      <c r="AF166" s="51" t="n">
+        <v>509</v>
+      </c>
+      <c r="Z166" s="48"/>
+      <c r="AA166" s="48"/>
+      <c r="AB166" s="48"/>
+      <c r="AC166" s="48"/>
+      <c r="AD166" s="48"/>
+      <c r="AE166" s="48"/>
+      <c r="AF166" s="52" t="n">
         <v>0</v>
       </c>
-      <c r="AG166" s="47"/>
-      <c r="AH166" s="47"/>
-      <c r="AI166" s="47"/>
-      <c r="AJ166" s="47"/>
-      <c r="AK166" s="47"/>
-      <c r="AL166" s="47"/>
-      <c r="AM166" s="47"/>
+      <c r="AG166" s="48"/>
+      <c r="AH166" s="48"/>
+      <c r="AI166" s="48"/>
+      <c r="AJ166" s="48"/>
+      <c r="AK166" s="48"/>
+      <c r="AL166" s="48"/>
+      <c r="AM166" s="48"/>
       <c r="AN166" s="12" t="n">
         <v>164</v>
       </c>
-      <c r="AO166" s="47" t="n">
+      <c r="AO166" s="48" t="n">
         <v>96</v>
       </c>
-      <c r="AP166" s="47"/>
-      <c r="AQ166" s="47"/>
+      <c r="AP166" s="48"/>
+      <c r="AQ166" s="48"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16475,14 +16494,17 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="53" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="53" t="s">
         <v>355</v>
       </c>
     </row>
@@ -16509,15 +16531,18 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
   </sheetData>
@@ -16543,19 +16568,22 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16568,7 +16596,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F3" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>10</v>
@@ -16576,180 +16604,180 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>515</v>
-      </c>
-      <c r="C7" s="53" t="s">
         <v>516</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>517</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>9</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>517</v>
-      </c>
-      <c r="H7" s="53"/>
+        <v>518</v>
+      </c>
+      <c r="H7" s="54"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="54" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>16</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>518</v>
-      </c>
-      <c r="H8" s="53"/>
+        <v>519</v>
+      </c>
+      <c r="H8" s="54"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="53"/>
+      <c r="A10" s="54"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="53" t="s">
-        <v>516</v>
+      <c r="A11" s="54" t="s">
+        <v>517</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>14</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="54" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>16</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>521</v>
-      </c>
-      <c r="E15" s="53"/>
-      <c r="H15" s="53"/>
+        <v>522</v>
+      </c>
+      <c r="E15" s="54"/>
+      <c r="H15" s="54"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="53"/>
-      <c r="H16" s="53"/>
+      <c r="E16" s="54"/>
+      <c r="H16" s="54"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="53" t="s">
-        <v>516</v>
+      <c r="A18" s="54" t="s">
+        <v>517</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C18" s="53" t="s">
-        <v>516</v>
+      <c r="C18" s="54" t="s">
+        <v>517</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="53" t="s">
+      <c r="A19" s="54" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C19" s="53" t="s">
+      <c r="C19" s="54" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>10</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="53" t="s">
-        <v>524</v>
-      </c>
-      <c r="B20" s="54" t="s">
+      <c r="A20" s="54" t="s">
         <v>525</v>
       </c>
-      <c r="C20" s="53" t="s">
-        <v>524</v>
-      </c>
-      <c r="D20" s="54" t="s">
+      <c r="B20" s="55" t="s">
         <v>526</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>525</v>
+      </c>
+      <c r="D20" s="55" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="53" t="s">
-        <v>516</v>
-      </c>
-      <c r="H25" s="55" t="s">
-        <v>529</v>
-      </c>
-      <c r="J25" s="53"/>
+      <c r="G25" s="54" t="s">
+        <v>517</v>
+      </c>
+      <c r="H25" s="56" t="s">
+        <v>530</v>
+      </c>
+      <c r="J25" s="54"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G26" s="53" t="s">
+      <c r="G26" s="54" t="s">
         <v>10</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="J26" s="53"/>
+      <c r="J26" s="54"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="53" t="s">
-        <v>516</v>
-      </c>
-      <c r="C28" s="55" t="s">
-        <v>529</v>
-      </c>
-      <c r="D28" s="53" t="s">
-        <v>516</v>
+      <c r="B28" s="54" t="s">
+        <v>517</v>
+      </c>
+      <c r="C28" s="56" t="s">
+        <v>530</v>
+      </c>
+      <c r="D28" s="54" t="s">
+        <v>517</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="53" t="s">
+      <c r="B29" s="54" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D29" s="53" t="s">
+      <c r="D29" s="54" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="0" t="n">
         <v>10</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
   </sheetData>
@@ -16775,51 +16803,54 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="57" t="s">
-        <v>533</v>
-      </c>
-      <c r="H1" s="57" t="s">
+      <c r="G1" s="58" t="s">
         <v>534</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="H1" s="58" t="s">
+        <v>535</v>
+      </c>
+      <c r="I1" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="J1" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="57" t="s">
-        <v>535</v>
-      </c>
-      <c r="L1" s="57" t="s">
+      <c r="K1" s="58" t="s">
+        <v>536</v>
+      </c>
+      <c r="L1" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="57" t="s">
+      <c r="M1" s="58" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="58" t="s">
-        <v>536</v>
+      <c r="B4" s="59" t="s">
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PROS-6346 - CCRU - KPI template logic update - hot fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/FT PoS 2018.xlsx
+++ b/Projects/CCRU/Data/FT PoS 2018.xlsx
@@ -41,9 +41,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2430" uniqueCount="539">
   <si>
     <t xml:space="preserve">Sorting</t>
   </si>
@@ -1152,7 +1153,7 @@
     <t xml:space="preserve">Cooler</t>
   </si>
   <si>
-    <t xml:space="preserve">FC 1 door, FC 1.5 door</t>
+    <t xml:space="preserve">FC 1 door, FC door 1.5 door</t>
   </si>
   <si>
     <t xml:space="preserve">filled collers target</t>
@@ -1219,6 +1220,9 @@
   </si>
   <si>
     <t xml:space="preserve">Холодильники: Мерч. Стандарты</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weighted Sum</t>
   </si>
   <si>
     <t xml:space="preserve">CONDITIONAL PROPORTIONAL</t>
@@ -2216,7 +2220,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2224,15 +2228,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2396,19 +2400,19 @@
   </sheetPr>
   <dimension ref="A1:AQ167"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="AI111" activeCellId="0" sqref="AI111"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="Q1" activeCellId="0" sqref="Q1"/>
+      <selection pane="bottomLeft" activeCell="U107" activeCellId="0" sqref="U107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="39.5263157894737"/>
-    <col collapsed="false" hidden="false" max="31" min="9" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="41.4210526315789"/>
+    <col collapsed="false" hidden="false" max="31" min="9" style="1" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="17.1376518218624"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="42.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11698,19 +11702,19 @@
       <c r="A110" s="37" t="n">
         <v>109</v>
       </c>
-      <c r="B110" s="36" t="s">
+      <c r="B110" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C110" s="36" t="s">
+      <c r="C110" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D110" s="36" t="s">
+      <c r="D110" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E110" s="36" t="s">
+      <c r="E110" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="F110" s="36"/>
+      <c r="F110" s="38"/>
       <c r="G110" s="37" t="s">
         <v>343</v>
       </c>
@@ -11728,44 +11732,44 @@
         <v>24</v>
       </c>
       <c r="M110" s="37"/>
-      <c r="N110" s="36" t="s">
+      <c r="N110" s="38" t="s">
         <v>326</v>
       </c>
-      <c r="O110" s="38" t="s">
+      <c r="O110" s="39" t="s">
         <v>327</v>
       </c>
-      <c r="P110" s="38"/>
-      <c r="Q110" s="38"/>
-      <c r="R110" s="36"/>
+      <c r="P110" s="39"/>
+      <c r="Q110" s="39"/>
+      <c r="R110" s="38"/>
       <c r="S110" s="37" t="s">
         <v>328</v>
       </c>
-      <c r="T110" s="36"/>
-      <c r="U110" s="36"/>
-      <c r="V110" s="36"/>
-      <c r="W110" s="36"/>
+      <c r="T110" s="38"/>
+      <c r="U110" s="38"/>
+      <c r="V110" s="38"/>
+      <c r="W110" s="38"/>
       <c r="X110" s="37" t="s">
         <v>339</v>
       </c>
-      <c r="Y110" s="36" t="s">
+      <c r="Y110" s="38" t="s">
         <v>340</v>
       </c>
-      <c r="Z110" s="36"/>
+      <c r="Z110" s="38"/>
       <c r="AA110" s="37"/>
-      <c r="AB110" s="36"/>
-      <c r="AC110" s="36"/>
+      <c r="AB110" s="38"/>
+      <c r="AC110" s="38"/>
       <c r="AD110" s="37" t="s">
         <v>50</v>
       </c>
       <c r="AE110" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="AF110" s="39" t="n">
+      <c r="AF110" s="40" t="n">
         <v>0</v>
       </c>
       <c r="AG110" s="37"/>
       <c r="AH110" s="37"/>
-      <c r="AI110" s="40" t="s">
+      <c r="AI110" s="37" t="s">
         <v>341</v>
       </c>
       <c r="AJ110" s="37" t="s">
@@ -11773,17 +11777,17 @@
       </c>
       <c r="AK110" s="37"/>
       <c r="AL110" s="37"/>
-      <c r="AM110" s="36" t="n">
+      <c r="AM110" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="AN110" s="36" t="n">
+      <c r="AN110" s="38" t="n">
         <v>165</v>
       </c>
-      <c r="AO110" s="36"/>
-      <c r="AP110" s="36" t="s">
+      <c r="AO110" s="38"/>
+      <c r="AP110" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="AQ110" s="36"/>
+      <c r="AQ110" s="38"/>
     </row>
     <row r="111" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="37" t="n">
@@ -12066,7 +12070,7 @@
         <v>362</v>
       </c>
       <c r="I114" s="42" t="s">
-        <v>49</v>
+        <v>363</v>
       </c>
       <c r="J114" s="14"/>
       <c r="K114" s="9"/>
@@ -12096,7 +12100,7 @@
         <v>50</v>
       </c>
       <c r="AE114" s="42" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AF114" s="17" t="n">
         <v>0.025</v>
@@ -12111,7 +12115,7 @@
         <v>336</v>
       </c>
       <c r="AJ114" s="37" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AK114" s="9"/>
       <c r="AL114" s="9"/>
@@ -12122,7 +12126,7 @@
         <v>112</v>
       </c>
       <c r="AO114" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AP114" s="33" t="s">
         <v>356</v>
@@ -12147,10 +12151,10 @@
       </c>
       <c r="F115" s="12"/>
       <c r="G115" s="9" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="H115" s="9" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>256</v>
@@ -12175,7 +12179,7 @@
       <c r="W115" s="12"/>
       <c r="X115" s="9"/>
       <c r="Y115" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z115" s="12"/>
       <c r="AA115" s="9"/>
@@ -12185,7 +12189,7 @@
         <v>50</v>
       </c>
       <c r="AE115" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AF115" s="44" t="n">
         <v>1</v>
@@ -12197,7 +12201,7 @@
         <v>1</v>
       </c>
       <c r="AI115" s="37" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AJ115" s="37"/>
       <c r="AK115" s="9"/>
@@ -12209,7 +12213,7 @@
         <v>113</v>
       </c>
       <c r="AO115" s="13" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AP115" s="33" t="s">
         <v>361</v>
@@ -12234,10 +12238,10 @@
       </c>
       <c r="F116" s="12"/>
       <c r="G116" s="9" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="H116" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="I116" s="14" t="s">
         <v>54</v>
@@ -12268,7 +12272,7 @@
       <c r="W116" s="12"/>
       <c r="X116" s="9"/>
       <c r="Y116" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z116" s="12"/>
       <c r="AA116" s="9"/>
@@ -12297,7 +12301,7 @@
       </c>
       <c r="AO116" s="12"/>
       <c r="AP116" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ116" s="12"/>
     </row>
@@ -12319,10 +12323,10 @@
       </c>
       <c r="F117" s="12"/>
       <c r="G117" s="9" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H117" s="9" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="I117" s="14" t="s">
         <v>54</v>
@@ -12353,7 +12357,7 @@
       <c r="W117" s="12"/>
       <c r="X117" s="9"/>
       <c r="Y117" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z117" s="12"/>
       <c r="AA117" s="9"/>
@@ -12382,7 +12386,7 @@
       </c>
       <c r="AO117" s="12"/>
       <c r="AP117" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ117" s="12"/>
     </row>
@@ -12404,10 +12408,10 @@
       </c>
       <c r="F118" s="12"/>
       <c r="G118" s="9" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="H118" s="9" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="I118" s="14" t="s">
         <v>54</v>
@@ -12438,7 +12442,7 @@
       <c r="W118" s="12"/>
       <c r="X118" s="9"/>
       <c r="Y118" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z118" s="12"/>
       <c r="AA118" s="9"/>
@@ -12467,7 +12471,7 @@
       </c>
       <c r="AO118" s="12"/>
       <c r="AP118" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ118" s="12"/>
     </row>
@@ -12489,10 +12493,10 @@
       </c>
       <c r="F119" s="12"/>
       <c r="G119" s="9" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="H119" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="I119" s="14" t="s">
         <v>54</v>
@@ -12523,7 +12527,7 @@
       <c r="W119" s="12"/>
       <c r="X119" s="9"/>
       <c r="Y119" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z119" s="12"/>
       <c r="AA119" s="9"/>
@@ -12552,7 +12556,7 @@
       </c>
       <c r="AO119" s="12"/>
       <c r="AP119" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ119" s="12"/>
     </row>
@@ -12574,10 +12578,10 @@
       </c>
       <c r="F120" s="12"/>
       <c r="G120" s="9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H120" s="9" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="I120" s="14" t="s">
         <v>54</v>
@@ -12608,7 +12612,7 @@
       <c r="W120" s="12"/>
       <c r="X120" s="9"/>
       <c r="Y120" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z120" s="12"/>
       <c r="AA120" s="9"/>
@@ -12637,7 +12641,7 @@
       </c>
       <c r="AO120" s="12"/>
       <c r="AP120" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ120" s="12"/>
     </row>
@@ -12659,10 +12663,10 @@
       </c>
       <c r="F121" s="12"/>
       <c r="G121" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="H121" s="9" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="I121" s="14" t="s">
         <v>54</v>
@@ -12693,7 +12697,7 @@
       <c r="W121" s="12"/>
       <c r="X121" s="9"/>
       <c r="Y121" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z121" s="12"/>
       <c r="AA121" s="9"/>
@@ -12722,7 +12726,7 @@
       </c>
       <c r="AO121" s="12"/>
       <c r="AP121" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ121" s="12"/>
     </row>
@@ -12744,10 +12748,10 @@
       </c>
       <c r="F122" s="12"/>
       <c r="G122" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="H122" s="9" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="I122" s="14" t="s">
         <v>54</v>
@@ -12778,7 +12782,7 @@
       <c r="W122" s="12"/>
       <c r="X122" s="9"/>
       <c r="Y122" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z122" s="12"/>
       <c r="AA122" s="9"/>
@@ -12807,7 +12811,7 @@
       </c>
       <c r="AO122" s="12"/>
       <c r="AP122" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ122" s="12"/>
     </row>
@@ -12829,10 +12833,10 @@
       </c>
       <c r="F123" s="12"/>
       <c r="G123" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="H123" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I123" s="14" t="s">
         <v>54</v>
@@ -12863,7 +12867,7 @@
       <c r="W123" s="12"/>
       <c r="X123" s="9"/>
       <c r="Y123" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z123" s="12"/>
       <c r="AA123" s="9"/>
@@ -12892,7 +12896,7 @@
       </c>
       <c r="AO123" s="12"/>
       <c r="AP123" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ123" s="12"/>
     </row>
@@ -12914,10 +12918,10 @@
       </c>
       <c r="F124" s="12"/>
       <c r="G124" s="9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="H124" s="9" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="I124" s="14" t="s">
         <v>54</v>
@@ -12948,7 +12952,7 @@
       <c r="W124" s="12"/>
       <c r="X124" s="9"/>
       <c r="Y124" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z124" s="12"/>
       <c r="AA124" s="9"/>
@@ -12977,7 +12981,7 @@
       </c>
       <c r="AO124" s="12"/>
       <c r="AP124" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ124" s="12"/>
     </row>
@@ -12999,10 +13003,10 @@
       </c>
       <c r="F125" s="12"/>
       <c r="G125" s="9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="H125" s="9" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="I125" s="14" t="s">
         <v>54</v>
@@ -13033,7 +13037,7 @@
       <c r="W125" s="12"/>
       <c r="X125" s="9"/>
       <c r="Y125" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z125" s="12"/>
       <c r="AA125" s="9"/>
@@ -13062,7 +13066,7 @@
       </c>
       <c r="AO125" s="12"/>
       <c r="AP125" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ125" s="12"/>
     </row>
@@ -13084,10 +13088,10 @@
       </c>
       <c r="F126" s="12"/>
       <c r="G126" s="9" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H126" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="I126" s="14" t="s">
         <v>54</v>
@@ -13118,7 +13122,7 @@
       <c r="W126" s="12"/>
       <c r="X126" s="9"/>
       <c r="Y126" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z126" s="12"/>
       <c r="AA126" s="9"/>
@@ -13147,7 +13151,7 @@
       </c>
       <c r="AO126" s="12"/>
       <c r="AP126" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ126" s="12"/>
     </row>
@@ -13169,10 +13173,10 @@
       </c>
       <c r="F127" s="12"/>
       <c r="G127" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="H127" s="9" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="I127" s="14" t="s">
         <v>54</v>
@@ -13184,10 +13188,10 @@
       <c r="L127" s="9"/>
       <c r="M127" s="9"/>
       <c r="N127" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="O127" s="45" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="P127" s="27"/>
       <c r="Q127" s="27"/>
@@ -13203,7 +13207,7 @@
       <c r="W127" s="12"/>
       <c r="X127" s="9"/>
       <c r="Y127" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z127" s="12"/>
       <c r="AA127" s="9"/>
@@ -13232,7 +13236,7 @@
       </c>
       <c r="AO127" s="12"/>
       <c r="AP127" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ127" s="12"/>
     </row>
@@ -13254,10 +13258,10 @@
       </c>
       <c r="F128" s="12"/>
       <c r="G128" s="9" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="H128" s="9" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="I128" s="14" t="s">
         <v>54</v>
@@ -13269,10 +13273,10 @@
       <c r="L128" s="9"/>
       <c r="M128" s="9"/>
       <c r="N128" s="12" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="O128" s="27" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="P128" s="27"/>
       <c r="Q128" s="27"/>
@@ -13288,7 +13292,7 @@
       <c r="W128" s="12"/>
       <c r="X128" s="9"/>
       <c r="Y128" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z128" s="12"/>
       <c r="AA128" s="9"/>
@@ -13317,7 +13321,7 @@
       </c>
       <c r="AO128" s="12"/>
       <c r="AP128" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ128" s="12"/>
     </row>
@@ -13339,10 +13343,10 @@
       </c>
       <c r="F129" s="12"/>
       <c r="G129" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="H129" s="9" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="I129" s="14" t="s">
         <v>54</v>
@@ -13373,7 +13377,7 @@
       <c r="W129" s="12"/>
       <c r="X129" s="9"/>
       <c r="Y129" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z129" s="12"/>
       <c r="AA129" s="9"/>
@@ -13402,7 +13406,7 @@
       </c>
       <c r="AO129" s="12"/>
       <c r="AP129" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ129" s="12"/>
     </row>
@@ -13424,10 +13428,10 @@
       </c>
       <c r="F130" s="12"/>
       <c r="G130" s="9" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H130" s="9" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="I130" s="14" t="s">
         <v>54</v>
@@ -13458,7 +13462,7 @@
       <c r="W130" s="12"/>
       <c r="X130" s="9"/>
       <c r="Y130" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z130" s="12"/>
       <c r="AA130" s="9"/>
@@ -13487,7 +13491,7 @@
       </c>
       <c r="AO130" s="12"/>
       <c r="AP130" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ130" s="12"/>
     </row>
@@ -13509,10 +13513,10 @@
       </c>
       <c r="F131" s="12"/>
       <c r="G131" s="9" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H131" s="9" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="I131" s="14" t="s">
         <v>54</v>
@@ -13543,7 +13547,7 @@
       <c r="W131" s="12"/>
       <c r="X131" s="9"/>
       <c r="Y131" s="37" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z131" s="12"/>
       <c r="AA131" s="9"/>
@@ -13572,7 +13576,7 @@
       </c>
       <c r="AO131" s="12"/>
       <c r="AP131" s="33" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AQ131" s="12"/>
     </row>
@@ -13594,10 +13598,10 @@
       </c>
       <c r="F132" s="12"/>
       <c r="G132" s="9" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="H132" s="9" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>256</v>
@@ -13622,7 +13626,7 @@
       <c r="W132" s="12"/>
       <c r="X132" s="9"/>
       <c r="Y132" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z132" s="12"/>
       <c r="AA132" s="9"/>
@@ -13632,7 +13636,7 @@
         <v>50</v>
       </c>
       <c r="AE132" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AF132" s="44" t="n">
         <v>0.5</v>
@@ -13644,7 +13648,7 @@
         <v>1</v>
       </c>
       <c r="AI132" s="37" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AJ132" s="37"/>
       <c r="AK132" s="9"/>
@@ -13656,7 +13660,7 @@
         <v>130</v>
       </c>
       <c r="AO132" s="13" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="AP132" s="33" t="s">
         <v>361</v>
@@ -13681,10 +13685,10 @@
       </c>
       <c r="F133" s="12"/>
       <c r="G133" s="9" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="H133" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="I133" s="14" t="s">
         <v>54</v>
@@ -13715,7 +13719,7 @@
       <c r="W133" s="12"/>
       <c r="X133" s="9"/>
       <c r="Y133" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z133" s="12"/>
       <c r="AA133" s="9"/>
@@ -13744,7 +13748,7 @@
       </c>
       <c r="AO133" s="12"/>
       <c r="AP133" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ133" s="12"/>
     </row>
@@ -13766,10 +13770,10 @@
       </c>
       <c r="F134" s="12"/>
       <c r="G134" s="9" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H134" s="9" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="I134" s="14" t="s">
         <v>54</v>
@@ -13800,7 +13804,7 @@
       <c r="W134" s="12"/>
       <c r="X134" s="9"/>
       <c r="Y134" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z134" s="12"/>
       <c r="AA134" s="9"/>
@@ -13829,7 +13833,7 @@
       </c>
       <c r="AO134" s="12"/>
       <c r="AP134" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ134" s="12"/>
     </row>
@@ -13851,10 +13855,10 @@
       </c>
       <c r="F135" s="12"/>
       <c r="G135" s="9" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="H135" s="9" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="I135" s="14" t="s">
         <v>54</v>
@@ -13885,7 +13889,7 @@
       <c r="W135" s="12"/>
       <c r="X135" s="9"/>
       <c r="Y135" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z135" s="12"/>
       <c r="AA135" s="9"/>
@@ -13914,7 +13918,7 @@
       </c>
       <c r="AO135" s="12"/>
       <c r="AP135" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ135" s="12"/>
     </row>
@@ -13936,10 +13940,10 @@
       </c>
       <c r="F136" s="12"/>
       <c r="G136" s="9" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="H136" s="9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="I136" s="14" t="s">
         <v>54</v>
@@ -13970,7 +13974,7 @@
       <c r="W136" s="12"/>
       <c r="X136" s="9"/>
       <c r="Y136" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z136" s="12"/>
       <c r="AA136" s="9"/>
@@ -13999,7 +14003,7 @@
       </c>
       <c r="AO136" s="12"/>
       <c r="AP136" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ136" s="12"/>
     </row>
@@ -14021,10 +14025,10 @@
       </c>
       <c r="F137" s="12"/>
       <c r="G137" s="9" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H137" s="9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="I137" s="14" t="s">
         <v>54</v>
@@ -14055,7 +14059,7 @@
       <c r="W137" s="12"/>
       <c r="X137" s="9"/>
       <c r="Y137" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z137" s="12"/>
       <c r="AA137" s="9"/>
@@ -14084,7 +14088,7 @@
       </c>
       <c r="AO137" s="12"/>
       <c r="AP137" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ137" s="12"/>
     </row>
@@ -14106,10 +14110,10 @@
       </c>
       <c r="F138" s="12"/>
       <c r="G138" s="9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="H138" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="I138" s="14" t="s">
         <v>54</v>
@@ -14140,7 +14144,7 @@
       <c r="W138" s="12"/>
       <c r="X138" s="9"/>
       <c r="Y138" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z138" s="12"/>
       <c r="AA138" s="9"/>
@@ -14169,7 +14173,7 @@
       </c>
       <c r="AO138" s="12"/>
       <c r="AP138" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ138" s="12"/>
     </row>
@@ -14191,10 +14195,10 @@
       </c>
       <c r="F139" s="12"/>
       <c r="G139" s="9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="H139" s="9" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="I139" s="14" t="s">
         <v>54</v>
@@ -14225,7 +14229,7 @@
       <c r="W139" s="12"/>
       <c r="X139" s="9"/>
       <c r="Y139" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z139" s="12"/>
       <c r="AA139" s="9"/>
@@ -14254,7 +14258,7 @@
       </c>
       <c r="AO139" s="12"/>
       <c r="AP139" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ139" s="12"/>
     </row>
@@ -14276,10 +14280,10 @@
       </c>
       <c r="F140" s="12"/>
       <c r="G140" s="9" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="H140" s="9" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="I140" s="14" t="s">
         <v>54</v>
@@ -14310,7 +14314,7 @@
       <c r="W140" s="12"/>
       <c r="X140" s="9"/>
       <c r="Y140" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z140" s="12"/>
       <c r="AA140" s="9"/>
@@ -14339,7 +14343,7 @@
       </c>
       <c r="AO140" s="12"/>
       <c r="AP140" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ140" s="12"/>
     </row>
@@ -14361,10 +14365,10 @@
       </c>
       <c r="F141" s="12"/>
       <c r="G141" s="9" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="H141" s="9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="I141" s="14" t="s">
         <v>54</v>
@@ -14395,7 +14399,7 @@
       <c r="W141" s="12"/>
       <c r="X141" s="9"/>
       <c r="Y141" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z141" s="12"/>
       <c r="AA141" s="9"/>
@@ -14424,7 +14428,7 @@
       </c>
       <c r="AO141" s="12"/>
       <c r="AP141" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ141" s="12"/>
     </row>
@@ -14446,10 +14450,10 @@
       </c>
       <c r="F142" s="12"/>
       <c r="G142" s="9" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H142" s="9" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="I142" s="14" t="s">
         <v>54</v>
@@ -14480,7 +14484,7 @@
       <c r="W142" s="12"/>
       <c r="X142" s="9"/>
       <c r="Y142" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z142" s="12"/>
       <c r="AA142" s="9"/>
@@ -14509,7 +14513,7 @@
       </c>
       <c r="AO142" s="12"/>
       <c r="AP142" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ142" s="12"/>
     </row>
@@ -14531,10 +14535,10 @@
       </c>
       <c r="F143" s="12"/>
       <c r="G143" s="9" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H143" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="I143" s="14" t="s">
         <v>54</v>
@@ -14565,7 +14569,7 @@
       <c r="W143" s="12"/>
       <c r="X143" s="9"/>
       <c r="Y143" s="37" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="Z143" s="12"/>
       <c r="AA143" s="9"/>
@@ -14594,7 +14598,7 @@
       </c>
       <c r="AO143" s="12"/>
       <c r="AP143" s="33" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AQ143" s="12"/>
     </row>
@@ -14616,10 +14620,10 @@
       </c>
       <c r="F144" s="12"/>
       <c r="G144" s="9" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H144" s="9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>256</v>
@@ -14644,7 +14648,7 @@
       <c r="W144" s="12"/>
       <c r="X144" s="9"/>
       <c r="Y144" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z144" s="12"/>
       <c r="AA144" s="9"/>
@@ -14654,7 +14658,7 @@
         <v>50</v>
       </c>
       <c r="AE144" s="9" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AF144" s="44" t="n">
         <v>0.5</v>
@@ -14666,7 +14670,7 @@
         <v>1</v>
       </c>
       <c r="AI144" s="37" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AJ144" s="37"/>
       <c r="AK144" s="9"/>
@@ -14678,7 +14682,7 @@
         <v>142</v>
       </c>
       <c r="AO144" s="13" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="AP144" s="33" t="s">
         <v>361</v>
@@ -14703,10 +14707,10 @@
       </c>
       <c r="F145" s="12"/>
       <c r="G145" s="9" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H145" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I145" s="14" t="s">
         <v>54</v>
@@ -14737,7 +14741,7 @@
       <c r="W145" s="12"/>
       <c r="X145" s="9"/>
       <c r="Y145" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z145" s="12"/>
       <c r="AA145" s="9"/>
@@ -14766,7 +14770,7 @@
       </c>
       <c r="AO145" s="12"/>
       <c r="AP145" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ145" s="12"/>
     </row>
@@ -14788,10 +14792,10 @@
       </c>
       <c r="F146" s="12"/>
       <c r="G146" s="9" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H146" s="9" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="I146" s="14" t="s">
         <v>54</v>
@@ -14822,7 +14826,7 @@
       <c r="W146" s="12"/>
       <c r="X146" s="9"/>
       <c r="Y146" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z146" s="12"/>
       <c r="AA146" s="9"/>
@@ -14851,7 +14855,7 @@
       </c>
       <c r="AO146" s="12"/>
       <c r="AP146" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ146" s="12"/>
     </row>
@@ -14873,10 +14877,10 @@
       </c>
       <c r="F147" s="12"/>
       <c r="G147" s="9" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H147" s="9" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="I147" s="14" t="s">
         <v>54</v>
@@ -14907,7 +14911,7 @@
       <c r="W147" s="12"/>
       <c r="X147" s="9"/>
       <c r="Y147" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z147" s="12"/>
       <c r="AA147" s="9"/>
@@ -14936,7 +14940,7 @@
       </c>
       <c r="AO147" s="12"/>
       <c r="AP147" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ147" s="12"/>
     </row>
@@ -14958,10 +14962,10 @@
       </c>
       <c r="F148" s="12"/>
       <c r="G148" s="9" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="H148" s="9" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="I148" s="14" t="s">
         <v>54</v>
@@ -14992,7 +14996,7 @@
       <c r="W148" s="12"/>
       <c r="X148" s="9"/>
       <c r="Y148" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z148" s="12"/>
       <c r="AA148" s="9"/>
@@ -15021,7 +15025,7 @@
       </c>
       <c r="AO148" s="12"/>
       <c r="AP148" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ148" s="12"/>
     </row>
@@ -15043,10 +15047,10 @@
       </c>
       <c r="F149" s="12"/>
       <c r="G149" s="9" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="H149" s="9" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="I149" s="14" t="s">
         <v>54</v>
@@ -15077,7 +15081,7 @@
       <c r="W149" s="12"/>
       <c r="X149" s="9"/>
       <c r="Y149" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z149" s="12"/>
       <c r="AA149" s="9"/>
@@ -15106,7 +15110,7 @@
       </c>
       <c r="AO149" s="12"/>
       <c r="AP149" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ149" s="12"/>
     </row>
@@ -15128,10 +15132,10 @@
       </c>
       <c r="F150" s="12"/>
       <c r="G150" s="9" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H150" s="9" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="I150" s="14" t="s">
         <v>54</v>
@@ -15143,10 +15147,10 @@
       <c r="L150" s="9"/>
       <c r="M150" s="9"/>
       <c r="N150" s="12" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="O150" s="10" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="P150" s="27"/>
       <c r="Q150" s="27"/>
@@ -15162,7 +15166,7 @@
       <c r="W150" s="12"/>
       <c r="X150" s="9"/>
       <c r="Y150" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z150" s="12"/>
       <c r="AA150" s="9"/>
@@ -15191,7 +15195,7 @@
       </c>
       <c r="AO150" s="12"/>
       <c r="AP150" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ150" s="12"/>
     </row>
@@ -15213,10 +15217,10 @@
       </c>
       <c r="F151" s="12"/>
       <c r="G151" s="9" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H151" s="9" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="I151" s="14" t="s">
         <v>54</v>
@@ -15228,10 +15232,10 @@
       <c r="L151" s="9"/>
       <c r="M151" s="9"/>
       <c r="N151" s="12" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="O151" s="10" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="P151" s="27"/>
       <c r="Q151" s="27"/>
@@ -15247,7 +15251,7 @@
       <c r="W151" s="12"/>
       <c r="X151" s="9"/>
       <c r="Y151" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z151" s="12"/>
       <c r="AA151" s="9"/>
@@ -15276,7 +15280,7 @@
       </c>
       <c r="AO151" s="12"/>
       <c r="AP151" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ151" s="12"/>
     </row>
@@ -15298,10 +15302,10 @@
       </c>
       <c r="F152" s="12"/>
       <c r="G152" s="9" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="H152" s="9" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I152" s="14" t="s">
         <v>54</v>
@@ -15313,10 +15317,10 @@
       <c r="L152" s="9"/>
       <c r="M152" s="9"/>
       <c r="N152" s="12" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="O152" s="10" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="P152" s="27"/>
       <c r="Q152" s="27"/>
@@ -15332,7 +15336,7 @@
       <c r="W152" s="12"/>
       <c r="X152" s="9"/>
       <c r="Y152" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z152" s="12"/>
       <c r="AA152" s="9"/>
@@ -15361,7 +15365,7 @@
       </c>
       <c r="AO152" s="12"/>
       <c r="AP152" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ152" s="12"/>
     </row>
@@ -15383,10 +15387,10 @@
       </c>
       <c r="F153" s="12"/>
       <c r="G153" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="H153" s="9" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="I153" s="14" t="s">
         <v>54</v>
@@ -15417,7 +15421,7 @@
       <c r="W153" s="12"/>
       <c r="X153" s="9"/>
       <c r="Y153" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z153" s="12"/>
       <c r="AA153" s="9"/>
@@ -15446,7 +15450,7 @@
       </c>
       <c r="AO153" s="12"/>
       <c r="AP153" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ153" s="12"/>
     </row>
@@ -15468,10 +15472,10 @@
       </c>
       <c r="F154" s="12"/>
       <c r="G154" s="9" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="H154" s="9" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="I154" s="14" t="s">
         <v>54</v>
@@ -15483,10 +15487,10 @@
       <c r="L154" s="9"/>
       <c r="M154" s="9"/>
       <c r="N154" s="12" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="O154" s="10" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="P154" s="27"/>
       <c r="Q154" s="27"/>
@@ -15502,7 +15506,7 @@
       <c r="W154" s="12"/>
       <c r="X154" s="9"/>
       <c r="Y154" s="37" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Z154" s="12"/>
       <c r="AA154" s="9"/>
@@ -15531,7 +15535,7 @@
       </c>
       <c r="AO154" s="12"/>
       <c r="AP154" s="33" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AQ154" s="12"/>
     </row>
@@ -15553,13 +15557,13 @@
       </c>
       <c r="F155" s="12"/>
       <c r="G155" s="9" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="H155" s="12" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="I155" s="14" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="J155" s="14"/>
       <c r="K155" s="9"/>
@@ -15629,25 +15633,25 @@
         <v>44</v>
       </c>
       <c r="D156" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E156" s="46" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="F156" s="46" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="G156" s="33" t="s">
         <v>308</v>
       </c>
       <c r="H156" s="47" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="I156" s="48" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="J156" s="48" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="K156" s="48"/>
       <c r="L156" s="48"/>
@@ -15658,7 +15662,7 @@
       <c r="Q156" s="48"/>
       <c r="R156" s="48"/>
       <c r="S156" s="48" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="T156" s="48"/>
       <c r="U156" s="48"/>
@@ -15702,23 +15706,23 @@
         <v>44</v>
       </c>
       <c r="D157" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E157" s="46" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="F157" s="46" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G157" s="46" t="s">
         <v>356</v>
       </c>
       <c r="H157" s="47"/>
       <c r="I157" s="48" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="J157" s="48" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="K157" s="48"/>
       <c r="L157" s="48"/>
@@ -15729,7 +15733,7 @@
       <c r="Q157" s="48"/>
       <c r="R157" s="48"/>
       <c r="S157" s="48" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="T157" s="48"/>
       <c r="U157" s="48"/>
@@ -15757,7 +15761,7 @@
         <v>155</v>
       </c>
       <c r="AO157" s="21" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AP157" s="48"/>
       <c r="AQ157" s="48"/>
@@ -15773,25 +15777,25 @@
         <v>44</v>
       </c>
       <c r="D158" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E158" s="46" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="F158" s="46" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="G158" s="46" t="s">
         <v>323</v>
       </c>
       <c r="H158" s="47" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="I158" s="48" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="J158" s="48" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="K158" s="48"/>
       <c r="L158" s="48"/>
@@ -15802,7 +15806,7 @@
       <c r="Q158" s="48"/>
       <c r="R158" s="48"/>
       <c r="S158" s="48" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="T158" s="48"/>
       <c r="U158" s="48"/>
@@ -15846,36 +15850,36 @@
         <v>44</v>
       </c>
       <c r="D159" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E159" s="46" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="F159" s="46" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G159" s="46" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="H159" s="48"/>
       <c r="I159" s="21" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="J159" s="21" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="K159" s="48"/>
       <c r="L159" s="48"/>
       <c r="M159" s="21"/>
       <c r="N159" s="21"/>
       <c r="O159" s="48" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="P159" s="48"/>
       <c r="Q159" s="48"/>
       <c r="R159" s="48"/>
       <c r="S159" s="48" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T159" s="48"/>
       <c r="U159" s="48"/>
@@ -15885,7 +15889,7 @@
         <v>339</v>
       </c>
       <c r="Y159" s="51" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="Z159" s="48"/>
       <c r="AA159" s="48"/>
@@ -15921,23 +15925,23 @@
         <v>44</v>
       </c>
       <c r="D160" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E160" s="46" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="F160" s="46" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="G160" s="46" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="H160" s="48"/>
       <c r="I160" s="21" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="J160" s="21" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K160" s="48"/>
       <c r="L160" s="48"/>
@@ -15950,7 +15954,7 @@
       <c r="Q160" s="48"/>
       <c r="R160" s="48"/>
       <c r="S160" s="48" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T160" s="48"/>
       <c r="U160" s="48"/>
@@ -15958,7 +15962,7 @@
       <c r="W160" s="48"/>
       <c r="X160" s="48"/>
       <c r="Y160" s="21" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="Z160" s="48"/>
       <c r="AA160" s="48"/>
@@ -15994,36 +15998,36 @@
         <v>44</v>
       </c>
       <c r="D161" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E161" s="46" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F161" s="46" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="G161" s="46" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="H161" s="48"/>
       <c r="I161" s="21" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="J161" s="21" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K161" s="48"/>
       <c r="L161" s="48"/>
       <c r="M161" s="21"/>
       <c r="N161" s="21"/>
       <c r="O161" s="48" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="P161" s="48"/>
       <c r="Q161" s="48"/>
       <c r="R161" s="48"/>
       <c r="S161" s="48" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T161" s="48"/>
       <c r="U161" s="48"/>
@@ -16031,7 +16035,7 @@
       <c r="W161" s="48"/>
       <c r="X161" s="48"/>
       <c r="Y161" s="21" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="Z161" s="48"/>
       <c r="AA161" s="48"/>
@@ -16067,36 +16071,36 @@
         <v>44</v>
       </c>
       <c r="D162" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E162" s="46" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="F162" s="46" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="G162" s="46" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="H162" s="48"/>
       <c r="I162" s="21" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="J162" s="21" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K162" s="48"/>
       <c r="L162" s="48"/>
       <c r="M162" s="21"/>
       <c r="N162" s="21"/>
       <c r="O162" s="48" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="P162" s="48"/>
       <c r="Q162" s="48"/>
       <c r="R162" s="48"/>
       <c r="S162" s="48" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T162" s="48"/>
       <c r="U162" s="48"/>
@@ -16104,7 +16108,7 @@
       <c r="W162" s="48"/>
       <c r="X162" s="48"/>
       <c r="Y162" s="21" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="Z162" s="48"/>
       <c r="AA162" s="48"/>
@@ -16140,38 +16144,38 @@
         <v>44</v>
       </c>
       <c r="D163" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E163" s="46" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F163" s="46" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G163" s="46" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="H163" s="48" t="s">
         <v>246</v>
       </c>
       <c r="I163" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="J163" s="21" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K163" s="48"/>
       <c r="L163" s="48"/>
       <c r="M163" s="21"/>
       <c r="N163" s="21"/>
       <c r="O163" s="21" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="P163" s="48"/>
       <c r="Q163" s="48"/>
       <c r="R163" s="48"/>
       <c r="S163" s="48" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T163" s="48"/>
       <c r="U163" s="48"/>
@@ -16179,7 +16183,7 @@
       <c r="W163" s="48"/>
       <c r="X163" s="48"/>
       <c r="Y163" s="21" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="Z163" s="48"/>
       <c r="AA163" s="48"/>
@@ -16217,38 +16221,38 @@
         <v>44</v>
       </c>
       <c r="D164" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E164" s="46" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F164" s="46" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G164" s="46" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="H164" s="48" t="s">
         <v>274</v>
       </c>
       <c r="I164" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="J164" s="21" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K164" s="48"/>
       <c r="L164" s="48"/>
       <c r="M164" s="21"/>
       <c r="N164" s="21"/>
       <c r="O164" s="21" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="P164" s="48"/>
       <c r="Q164" s="48"/>
       <c r="R164" s="48"/>
       <c r="S164" s="48" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T164" s="48"/>
       <c r="U164" s="48"/>
@@ -16256,7 +16260,7 @@
       <c r="W164" s="48"/>
       <c r="X164" s="48"/>
       <c r="Y164" s="21" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="Z164" s="48"/>
       <c r="AA164" s="48"/>
@@ -16294,38 +16298,38 @@
         <v>44</v>
       </c>
       <c r="D165" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E165" s="46" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F165" s="46" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G165" s="46" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="H165" s="48" t="s">
         <v>265</v>
       </c>
       <c r="I165" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="J165" s="21" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K165" s="48"/>
       <c r="L165" s="48"/>
       <c r="M165" s="21"/>
       <c r="N165" s="21"/>
       <c r="O165" s="21" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="P165" s="48"/>
       <c r="Q165" s="48"/>
       <c r="R165" s="48"/>
       <c r="S165" s="48" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T165" s="48"/>
       <c r="U165" s="48"/>
@@ -16333,7 +16337,7 @@
       <c r="W165" s="48"/>
       <c r="X165" s="48"/>
       <c r="Y165" s="21" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="Z165" s="48"/>
       <c r="AA165" s="48"/>
@@ -16371,38 +16375,38 @@
         <v>44</v>
       </c>
       <c r="D166" s="23" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E166" s="46" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="F166" s="46" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G166" s="46" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="H166" s="48" t="s">
         <v>289</v>
       </c>
       <c r="I166" s="21" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="J166" s="21" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="K166" s="48"/>
       <c r="L166" s="48"/>
       <c r="M166" s="21"/>
       <c r="N166" s="21"/>
       <c r="O166" s="21" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="P166" s="48"/>
       <c r="Q166" s="48"/>
       <c r="R166" s="48"/>
       <c r="S166" s="48" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="T166" s="48"/>
       <c r="U166" s="48"/>
@@ -16410,7 +16414,7 @@
       <c r="W166" s="48"/>
       <c r="X166" s="48"/>
       <c r="Y166" s="21" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="Z166" s="48"/>
       <c r="AA166" s="48"/>
@@ -16495,7 +16499,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16532,17 +16536,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -16569,21 +16573,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="G1" s="0" t="n">
         <v>16</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16596,7 +16600,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F3" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>10</v>
@@ -16604,16 +16608,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C7" s="54" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>9</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="H7" s="54"/>
     </row>
@@ -16625,7 +16629,7 @@
         <v>16</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="H8" s="54"/>
     </row>
@@ -16634,13 +16638,13 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="54" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>14</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16651,12 +16655,12 @@
         <v>16</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="E15" s="54"/>
       <c r="H15" s="54"/>
@@ -16667,19 +16671,19 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="54" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="C18" s="54" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>8</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16696,39 +16700,39 @@
         <v>10</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="54" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="B20" s="55" t="s">
+        <v>527</v>
+      </c>
+      <c r="C20" s="54" t="s">
         <v>526</v>
       </c>
-      <c r="C20" s="54" t="s">
-        <v>525</v>
-      </c>
       <c r="D20" s="55" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G25" s="54" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="H25" s="56" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="J25" s="54"/>
     </row>
@@ -16743,19 +16747,19 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="54" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C28" s="56" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="D28" s="54" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E28" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16772,12 +16776,12 @@
         <v>10</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -16804,7 +16808,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16827,10 +16831,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="58" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="H1" s="58" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="I1" s="58" t="s">
         <v>35</v>
@@ -16839,7 +16843,7 @@
         <v>31</v>
       </c>
       <c r="K1" s="58" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="L1" s="58" t="s">
         <v>36</v>
@@ -16850,7 +16854,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="59" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PRSO-6556 - CCRU - KPI template update on 28.10
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/FT PoS 2018.xlsx
+++ b/Projects/CCRU/Data/FT PoS 2018.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="981" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Traditional Trade" sheetId="1" state="visible" r:id="rId2"/>
@@ -43,9 +43,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$166</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Traditional Trade'!$A$1:$AQ$162</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1082,13 +1083,13 @@
     <t xml:space="preserve">Energy Activation</t>
   </si>
   <si>
-    <t xml:space="preserve">RGM Activations: SSD/Juice in Bread/Bakery Zone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RGM Активации: SSD/Сок в зоне Хлеб/Выпечка</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD/Juice in Bread/Bakery Zone</t>
+    <t xml:space="preserve">RGM Activations: SCHWEPPES in ALCO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RGM Активации: SCHWEPPES в алкоголе</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHWEPPES in ALCO</t>
   </si>
   <si>
     <t xml:space="preserve">Promo Displays</t>
@@ -1957,7 +1958,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1968,6 +1969,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -2083,7 +2090,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2212,6 +2219,14 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2224,43 +2239,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2269,10 +2248,42 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2296,11 +2307,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2308,7 +2319,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2420,19 +2431,19 @@
   </sheetPr>
   <dimension ref="A1:AQ167"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="N124" activeCellId="0" sqref="N124"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="G111" activeCellId="0" sqref="G111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.85"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="17.502024291498"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="42.3562753036437"/>
-    <col collapsed="false" hidden="false" max="31" min="9" style="1" width="17.502024291498"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="17.502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="17.502024291498"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="42.6315789473684"/>
+    <col collapsed="false" hidden="false" max="31" min="9" style="1" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="2" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="1025" min="33" style="1" width="17.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="42.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11318,10 +11329,10 @@
         <v>304</v>
       </c>
       <c r="F105" s="12"/>
-      <c r="G105" s="9" t="s">
+      <c r="G105" s="32" t="s">
         <v>317</v>
       </c>
-      <c r="H105" s="12" t="s">
+      <c r="H105" s="32" t="s">
         <v>318</v>
       </c>
       <c r="I105" s="9" t="s">
@@ -11334,7 +11345,7 @@
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
       <c r="N105" s="9"/>
-      <c r="O105" s="12" t="s">
+      <c r="O105" s="33" t="s">
         <v>319</v>
       </c>
       <c r="P105" s="10"/>
@@ -11350,7 +11361,7 @@
       <c r="V105" s="9"/>
       <c r="W105" s="9"/>
       <c r="X105" s="9"/>
-      <c r="Y105" s="12" t="s">
+      <c r="Y105" s="33" t="s">
         <v>319</v>
       </c>
       <c r="Z105" s="9"/>
@@ -11397,10 +11408,10 @@
       <c r="D106" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="E106" s="32" t="s">
+      <c r="E106" s="34" t="s">
         <v>304</v>
       </c>
-      <c r="F106" s="32"/>
+      <c r="F106" s="34"/>
       <c r="G106" s="9" t="s">
         <v>320</v>
       </c>
@@ -11460,7 +11471,7 @@
       <c r="AO106" s="13" t="s">
         <v>322</v>
       </c>
-      <c r="AP106" s="33" t="s">
+      <c r="AP106" s="35" t="s">
         <v>323</v>
       </c>
       <c r="AQ106" s="12"/>
@@ -11529,7 +11540,7 @@
       <c r="AE107" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AF107" s="34" t="n">
+      <c r="AF107" s="36" t="n">
         <v>0</v>
       </c>
       <c r="AG107" s="12"/>
@@ -11621,7 +11632,7 @@
       <c r="AN108" s="12" t="n">
         <v>107</v>
       </c>
-      <c r="AO108" s="35" t="s">
+      <c r="AO108" s="37" t="s">
         <v>335</v>
       </c>
       <c r="AP108" s="12"/>
@@ -11681,7 +11692,7 @@
         <v>339</v>
       </c>
       <c r="Y109" s="12"/>
-      <c r="Z109" s="36" t="s">
+      <c r="Z109" s="38" t="s">
         <v>340</v>
       </c>
       <c r="AA109" s="9"/>
@@ -11719,98 +11730,98 @@
       <c r="AQ109" s="12"/>
     </row>
     <row r="110" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="37" t="n">
+      <c r="A110" s="39" t="n">
         <v>109</v>
       </c>
-      <c r="B110" s="36" t="s">
+      <c r="B110" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="C110" s="36" t="s">
+      <c r="C110" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="D110" s="36" t="s">
+      <c r="D110" s="38" t="s">
         <v>45</v>
       </c>
-      <c r="E110" s="36" t="s">
+      <c r="E110" s="38" t="s">
         <v>233</v>
       </c>
-      <c r="F110" s="36"/>
-      <c r="G110" s="37" t="s">
+      <c r="F110" s="38"/>
+      <c r="G110" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="H110" s="37" t="s">
+      <c r="H110" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="I110" s="37" t="s">
+      <c r="I110" s="39" t="s">
         <v>338</v>
       </c>
-      <c r="J110" s="37"/>
-      <c r="K110" s="37" t="n">
+      <c r="J110" s="39"/>
+      <c r="K110" s="39" t="n">
         <v>0.5</v>
       </c>
-      <c r="L110" s="37" t="n">
+      <c r="L110" s="39" t="n">
         <v>24</v>
       </c>
-      <c r="M110" s="37"/>
-      <c r="N110" s="36" t="s">
+      <c r="M110" s="39"/>
+      <c r="N110" s="38" t="s">
         <v>326</v>
       </c>
-      <c r="O110" s="38" t="s">
+      <c r="O110" s="40" t="s">
         <v>327</v>
       </c>
-      <c r="P110" s="38"/>
-      <c r="Q110" s="38"/>
-      <c r="R110" s="36"/>
-      <c r="S110" s="37" t="s">
+      <c r="P110" s="40"/>
+      <c r="Q110" s="40"/>
+      <c r="R110" s="38"/>
+      <c r="S110" s="39" t="s">
         <v>328</v>
       </c>
-      <c r="T110" s="36"/>
-      <c r="U110" s="36"/>
-      <c r="V110" s="36"/>
-      <c r="W110" s="36"/>
-      <c r="X110" s="37" t="s">
+      <c r="T110" s="38"/>
+      <c r="U110" s="38"/>
+      <c r="V110" s="38"/>
+      <c r="W110" s="38"/>
+      <c r="X110" s="39" t="s">
         <v>339</v>
       </c>
-      <c r="Y110" s="36" t="s">
+      <c r="Y110" s="38" t="s">
         <v>340</v>
       </c>
-      <c r="Z110" s="36"/>
-      <c r="AA110" s="37"/>
-      <c r="AB110" s="36"/>
-      <c r="AC110" s="36"/>
-      <c r="AD110" s="37" t="s">
+      <c r="Z110" s="38"/>
+      <c r="AA110" s="39"/>
+      <c r="AB110" s="38"/>
+      <c r="AC110" s="38"/>
+      <c r="AD110" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="AE110" s="37" t="s">
+      <c r="AE110" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="AF110" s="39" t="n">
+      <c r="AF110" s="41" t="n">
         <v>0</v>
       </c>
-      <c r="AG110" s="37"/>
-      <c r="AH110" s="37"/>
-      <c r="AI110" s="37" t="s">
+      <c r="AG110" s="39"/>
+      <c r="AH110" s="39"/>
+      <c r="AI110" s="39" t="s">
         <v>341</v>
       </c>
-      <c r="AJ110" s="37" t="s">
+      <c r="AJ110" s="39" t="s">
         <v>342</v>
       </c>
-      <c r="AK110" s="37"/>
-      <c r="AL110" s="37"/>
-      <c r="AM110" s="36" t="n">
+      <c r="AK110" s="39"/>
+      <c r="AL110" s="39"/>
+      <c r="AM110" s="38" t="n">
         <v>3</v>
       </c>
-      <c r="AN110" s="36" t="n">
+      <c r="AN110" s="38" t="n">
         <v>165</v>
       </c>
-      <c r="AO110" s="36"/>
-      <c r="AP110" s="36" t="s">
+      <c r="AO110" s="38"/>
+      <c r="AP110" s="38" t="s">
         <v>330</v>
       </c>
-      <c r="AQ110" s="36"/>
+      <c r="AQ110" s="38"/>
     </row>
     <row r="111" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="37" t="n">
+      <c r="A111" s="39" t="n">
         <v>110</v>
       </c>
       <c r="B111" s="12" t="s">
@@ -11893,7 +11904,7 @@
       <c r="AQ111" s="12"/>
     </row>
     <row r="112" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="37" t="n">
+      <c r="A112" s="39" t="n">
         <v>111</v>
       </c>
       <c r="B112" s="12" t="s">
@@ -11925,7 +11936,7 @@
       <c r="L112" s="9"/>
       <c r="M112" s="9"/>
       <c r="N112" s="12"/>
-      <c r="O112" s="40" t="s">
+      <c r="O112" s="42" t="s">
         <v>352</v>
       </c>
       <c r="P112" s="27"/>
@@ -11936,15 +11947,15 @@
       </c>
       <c r="T112" s="12"/>
       <c r="U112" s="12"/>
-      <c r="V112" s="40"/>
+      <c r="V112" s="42"/>
       <c r="W112" s="12"/>
       <c r="X112" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="Y112" s="40" t="s">
+      <c r="Y112" s="42" t="s">
         <v>352</v>
       </c>
-      <c r="Z112" s="40"/>
+      <c r="Z112" s="42"/>
       <c r="AA112" s="9"/>
       <c r="AB112" s="12"/>
       <c r="AC112" s="12"/>
@@ -11974,13 +11985,13 @@
         <v>110</v>
       </c>
       <c r="AO112" s="12"/>
-      <c r="AP112" s="33" t="s">
+      <c r="AP112" s="35" t="s">
         <v>356</v>
       </c>
       <c r="AQ112" s="12"/>
     </row>
     <row r="113" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="37" t="n">
+      <c r="A113" s="39" t="n">
         <v>112</v>
       </c>
       <c r="B113" s="12" t="s">
@@ -12061,13 +12072,13 @@
         <v>111</v>
       </c>
       <c r="AO113" s="12"/>
-      <c r="AP113" s="33" t="s">
+      <c r="AP113" s="35" t="s">
         <v>356</v>
       </c>
       <c r="AQ113" s="12"/>
     </row>
     <row r="114" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="37" t="n">
+      <c r="A114" s="39" t="n">
         <v>113</v>
       </c>
       <c r="B114" s="12" t="s">
@@ -12089,7 +12100,7 @@
       <c r="H114" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="I114" s="41" t="s">
+      <c r="I114" s="43" t="s">
         <v>363</v>
       </c>
       <c r="J114" s="14"/>
@@ -12097,7 +12108,7 @@
       <c r="L114" s="9"/>
       <c r="M114" s="9"/>
       <c r="N114" s="12"/>
-      <c r="O114" s="42"/>
+      <c r="O114" s="44"/>
       <c r="P114" s="27"/>
       <c r="Q114" s="27"/>
       <c r="R114" s="9" t="s">
@@ -12119,22 +12130,22 @@
       <c r="AD114" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="AE114" s="41" t="s">
+      <c r="AE114" s="43" t="s">
         <v>364</v>
       </c>
       <c r="AF114" s="17" t="n">
         <v>0.025</v>
       </c>
-      <c r="AG114" s="37" t="n">
+      <c r="AG114" s="39" t="n">
         <v>0</v>
       </c>
-      <c r="AH114" s="37" t="n">
+      <c r="AH114" s="39" t="n">
         <v>1</v>
       </c>
       <c r="AI114" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="AJ114" s="37" t="s">
+      <c r="AJ114" s="39" t="s">
         <v>365</v>
       </c>
       <c r="AK114" s="9"/>
@@ -12148,13 +12159,13 @@
       <c r="AO114" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="AP114" s="33" t="s">
+      <c r="AP114" s="35" t="s">
         <v>356</v>
       </c>
       <c r="AQ114" s="12"/>
     </row>
     <row r="115" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="37" t="n">
+      <c r="A115" s="39" t="n">
         <v>114</v>
       </c>
       <c r="B115" s="12" t="s">
@@ -12186,7 +12197,7 @@
       <c r="L115" s="9"/>
       <c r="M115" s="9"/>
       <c r="N115" s="12"/>
-      <c r="O115" s="42"/>
+      <c r="O115" s="44"/>
       <c r="P115" s="27"/>
       <c r="Q115" s="27"/>
       <c r="R115" s="9" t="s">
@@ -12198,7 +12209,7 @@
       <c r="V115" s="12"/>
       <c r="W115" s="12"/>
       <c r="X115" s="9"/>
-      <c r="Y115" s="37" t="s">
+      <c r="Y115" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z115" s="12"/>
@@ -12211,7 +12222,7 @@
       <c r="AE115" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="AF115" s="43" t="n">
+      <c r="AF115" s="45" t="n">
         <v>1</v>
       </c>
       <c r="AG115" s="9" t="n">
@@ -12220,10 +12231,10 @@
       <c r="AH115" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AI115" s="37" t="s">
+      <c r="AI115" s="39" t="s">
         <v>370</v>
       </c>
-      <c r="AJ115" s="37"/>
+      <c r="AJ115" s="39"/>
       <c r="AK115" s="9"/>
       <c r="AL115" s="9"/>
       <c r="AM115" s="12" t="n">
@@ -12235,13 +12246,13 @@
       <c r="AO115" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="AP115" s="33" t="s">
+      <c r="AP115" s="35" t="s">
         <v>361</v>
       </c>
       <c r="AQ115" s="12"/>
     </row>
     <row r="116" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="37" t="n">
+      <c r="A116" s="39" t="n">
         <v>115</v>
       </c>
       <c r="B116" s="12" t="s">
@@ -12291,7 +12302,7 @@
       <c r="V116" s="12"/>
       <c r="W116" s="12"/>
       <c r="X116" s="9"/>
-      <c r="Y116" s="37" t="s">
+      <c r="Y116" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z116" s="12"/>
@@ -12310,7 +12321,7 @@
       <c r="AG116" s="9"/>
       <c r="AH116" s="9"/>
       <c r="AI116" s="9"/>
-      <c r="AJ116" s="37"/>
+      <c r="AJ116" s="39"/>
       <c r="AK116" s="9"/>
       <c r="AL116" s="9"/>
       <c r="AM116" s="12" t="n">
@@ -12320,13 +12331,13 @@
         <v>114</v>
       </c>
       <c r="AO116" s="12"/>
-      <c r="AP116" s="33" t="s">
+      <c r="AP116" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ116" s="12"/>
     </row>
     <row r="117" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="37" t="n">
+      <c r="A117" s="39" t="n">
         <v>116</v>
       </c>
       <c r="B117" s="12" t="s">
@@ -12342,10 +12353,10 @@
         <v>304</v>
       </c>
       <c r="F117" s="12"/>
-      <c r="G117" s="44" t="s">
+      <c r="G117" s="46" t="s">
         <v>374</v>
       </c>
-      <c r="H117" s="44" t="s">
+      <c r="H117" s="46" t="s">
         <v>375</v>
       </c>
       <c r="I117" s="14" t="s">
@@ -12357,10 +12368,10 @@
       </c>
       <c r="L117" s="9"/>
       <c r="M117" s="9"/>
-      <c r="N117" s="45" t="s">
+      <c r="N117" s="47" t="s">
         <v>376</v>
       </c>
-      <c r="O117" s="46" t="s">
+      <c r="O117" s="47" t="s">
         <v>377</v>
       </c>
       <c r="P117" s="27"/>
@@ -12376,7 +12387,7 @@
       <c r="V117" s="12"/>
       <c r="W117" s="12"/>
       <c r="X117" s="9"/>
-      <c r="Y117" s="37" t="s">
+      <c r="Y117" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z117" s="12"/>
@@ -12395,7 +12406,7 @@
       <c r="AG117" s="9"/>
       <c r="AH117" s="9"/>
       <c r="AI117" s="9"/>
-      <c r="AJ117" s="37"/>
+      <c r="AJ117" s="39"/>
       <c r="AK117" s="9"/>
       <c r="AL117" s="9"/>
       <c r="AM117" s="12" t="n">
@@ -12405,13 +12416,13 @@
         <v>115</v>
       </c>
       <c r="AO117" s="12"/>
-      <c r="AP117" s="33" t="s">
+      <c r="AP117" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ117" s="12"/>
     </row>
     <row r="118" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="37" t="n">
+      <c r="A118" s="39" t="n">
         <v>117</v>
       </c>
       <c r="B118" s="12" t="s">
@@ -12461,7 +12472,7 @@
       <c r="V118" s="12"/>
       <c r="W118" s="12"/>
       <c r="X118" s="9"/>
-      <c r="Y118" s="37" t="s">
+      <c r="Y118" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z118" s="12"/>
@@ -12480,7 +12491,7 @@
       <c r="AG118" s="9"/>
       <c r="AH118" s="9"/>
       <c r="AI118" s="9"/>
-      <c r="AJ118" s="37"/>
+      <c r="AJ118" s="39"/>
       <c r="AK118" s="9"/>
       <c r="AL118" s="9"/>
       <c r="AM118" s="12" t="n">
@@ -12490,13 +12501,13 @@
         <v>116</v>
       </c>
       <c r="AO118" s="12"/>
-      <c r="AP118" s="33" t="s">
+      <c r="AP118" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ118" s="12"/>
     </row>
     <row r="119" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="37" t="n">
+      <c r="A119" s="39" t="n">
         <v>118</v>
       </c>
       <c r="B119" s="12" t="s">
@@ -12546,7 +12557,7 @@
       <c r="V119" s="12"/>
       <c r="W119" s="12"/>
       <c r="X119" s="9"/>
-      <c r="Y119" s="37" t="s">
+      <c r="Y119" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z119" s="12"/>
@@ -12565,7 +12576,7 @@
       <c r="AG119" s="9"/>
       <c r="AH119" s="9"/>
       <c r="AI119" s="9"/>
-      <c r="AJ119" s="37"/>
+      <c r="AJ119" s="39"/>
       <c r="AK119" s="9"/>
       <c r="AL119" s="9"/>
       <c r="AM119" s="12" t="n">
@@ -12575,13 +12586,13 @@
         <v>117</v>
       </c>
       <c r="AO119" s="12"/>
-      <c r="AP119" s="33" t="s">
+      <c r="AP119" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ119" s="12"/>
     </row>
     <row r="120" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="37" t="n">
+      <c r="A120" s="39" t="n">
         <v>119</v>
       </c>
       <c r="B120" s="12" t="s">
@@ -12597,10 +12608,10 @@
         <v>304</v>
       </c>
       <c r="F120" s="12"/>
-      <c r="G120" s="44" t="s">
+      <c r="G120" s="46" t="s">
         <v>382</v>
       </c>
-      <c r="H120" s="44" t="s">
+      <c r="H120" s="46" t="s">
         <v>383</v>
       </c>
       <c r="I120" s="14" t="s">
@@ -12612,10 +12623,10 @@
       </c>
       <c r="L120" s="9"/>
       <c r="M120" s="9"/>
-      <c r="N120" s="45" t="s">
+      <c r="N120" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="O120" s="47" t="n">
+      <c r="O120" s="48" t="n">
         <v>5449000214744</v>
       </c>
       <c r="P120" s="27"/>
@@ -12631,7 +12642,7 @@
       <c r="V120" s="12"/>
       <c r="W120" s="12"/>
       <c r="X120" s="9"/>
-      <c r="Y120" s="37" t="s">
+      <c r="Y120" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z120" s="12"/>
@@ -12650,7 +12661,7 @@
       <c r="AG120" s="9"/>
       <c r="AH120" s="9"/>
       <c r="AI120" s="9"/>
-      <c r="AJ120" s="37"/>
+      <c r="AJ120" s="39"/>
       <c r="AK120" s="9"/>
       <c r="AL120" s="9"/>
       <c r="AM120" s="12" t="n">
@@ -12660,13 +12671,13 @@
         <v>118</v>
       </c>
       <c r="AO120" s="12"/>
-      <c r="AP120" s="33" t="s">
+      <c r="AP120" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ120" s="12"/>
     </row>
     <row r="121" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="37" t="n">
+      <c r="A121" s="39" t="n">
         <v>120</v>
       </c>
       <c r="B121" s="12" t="s">
@@ -12716,7 +12727,7 @@
       <c r="V121" s="12"/>
       <c r="W121" s="12"/>
       <c r="X121" s="9"/>
-      <c r="Y121" s="37" t="s">
+      <c r="Y121" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z121" s="12"/>
@@ -12735,7 +12746,7 @@
       <c r="AG121" s="9"/>
       <c r="AH121" s="9"/>
       <c r="AI121" s="9"/>
-      <c r="AJ121" s="37"/>
+      <c r="AJ121" s="39"/>
       <c r="AK121" s="9"/>
       <c r="AL121" s="9"/>
       <c r="AM121" s="12" t="n">
@@ -12745,13 +12756,13 @@
         <v>119</v>
       </c>
       <c r="AO121" s="12"/>
-      <c r="AP121" s="33" t="s">
+      <c r="AP121" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ121" s="12"/>
     </row>
     <row r="122" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="37" t="n">
+      <c r="A122" s="39" t="n">
         <v>121</v>
       </c>
       <c r="B122" s="12" t="s">
@@ -12801,7 +12812,7 @@
       <c r="V122" s="12"/>
       <c r="W122" s="12"/>
       <c r="X122" s="9"/>
-      <c r="Y122" s="37" t="s">
+      <c r="Y122" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z122" s="12"/>
@@ -12820,7 +12831,7 @@
       <c r="AG122" s="9"/>
       <c r="AH122" s="9"/>
       <c r="AI122" s="9"/>
-      <c r="AJ122" s="37"/>
+      <c r="AJ122" s="39"/>
       <c r="AK122" s="9"/>
       <c r="AL122" s="9"/>
       <c r="AM122" s="12" t="n">
@@ -12830,13 +12841,13 @@
         <v>120</v>
       </c>
       <c r="AO122" s="12"/>
-      <c r="AP122" s="33" t="s">
+      <c r="AP122" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ122" s="12"/>
     </row>
     <row r="123" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="37" t="n">
+      <c r="A123" s="39" t="n">
         <v>122</v>
       </c>
       <c r="B123" s="12" t="s">
@@ -12886,7 +12897,7 @@
       <c r="V123" s="12"/>
       <c r="W123" s="12"/>
       <c r="X123" s="9"/>
-      <c r="Y123" s="37" t="s">
+      <c r="Y123" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z123" s="12"/>
@@ -12905,7 +12916,7 @@
       <c r="AG123" s="9"/>
       <c r="AH123" s="9"/>
       <c r="AI123" s="9"/>
-      <c r="AJ123" s="37"/>
+      <c r="AJ123" s="39"/>
       <c r="AK123" s="9"/>
       <c r="AL123" s="9"/>
       <c r="AM123" s="12" t="n">
@@ -12915,13 +12926,13 @@
         <v>121</v>
       </c>
       <c r="AO123" s="12"/>
-      <c r="AP123" s="33" t="s">
+      <c r="AP123" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ123" s="12"/>
     </row>
     <row r="124" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="37" t="n">
+      <c r="A124" s="39" t="n">
         <v>123</v>
       </c>
       <c r="B124" s="12" t="s">
@@ -12971,7 +12982,7 @@
       <c r="V124" s="12"/>
       <c r="W124" s="12"/>
       <c r="X124" s="9"/>
-      <c r="Y124" s="37" t="s">
+      <c r="Y124" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z124" s="12"/>
@@ -12990,7 +13001,7 @@
       <c r="AG124" s="9"/>
       <c r="AH124" s="9"/>
       <c r="AI124" s="9"/>
-      <c r="AJ124" s="37"/>
+      <c r="AJ124" s="39"/>
       <c r="AK124" s="9"/>
       <c r="AL124" s="9"/>
       <c r="AM124" s="12" t="n">
@@ -13000,13 +13011,13 @@
         <v>122</v>
       </c>
       <c r="AO124" s="12"/>
-      <c r="AP124" s="33" t="s">
+      <c r="AP124" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ124" s="12"/>
     </row>
     <row r="125" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="37" t="n">
+      <c r="A125" s="39" t="n">
         <v>124</v>
       </c>
       <c r="B125" s="12" t="s">
@@ -13056,7 +13067,7 @@
       <c r="V125" s="12"/>
       <c r="W125" s="12"/>
       <c r="X125" s="9"/>
-      <c r="Y125" s="37" t="s">
+      <c r="Y125" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z125" s="12"/>
@@ -13075,7 +13086,7 @@
       <c r="AG125" s="9"/>
       <c r="AH125" s="9"/>
       <c r="AI125" s="9"/>
-      <c r="AJ125" s="37"/>
+      <c r="AJ125" s="39"/>
       <c r="AK125" s="9"/>
       <c r="AL125" s="9"/>
       <c r="AM125" s="12" t="n">
@@ -13085,13 +13096,13 @@
         <v>123</v>
       </c>
       <c r="AO125" s="12"/>
-      <c r="AP125" s="33" t="s">
+      <c r="AP125" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ125" s="12"/>
     </row>
     <row r="126" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="37" t="n">
+      <c r="A126" s="39" t="n">
         <v>125</v>
       </c>
       <c r="B126" s="12" t="s">
@@ -13141,7 +13152,7 @@
       <c r="V126" s="12"/>
       <c r="W126" s="12"/>
       <c r="X126" s="9"/>
-      <c r="Y126" s="37" t="s">
+      <c r="Y126" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z126" s="12"/>
@@ -13160,7 +13171,7 @@
       <c r="AG126" s="9"/>
       <c r="AH126" s="9"/>
       <c r="AI126" s="9"/>
-      <c r="AJ126" s="37"/>
+      <c r="AJ126" s="39"/>
       <c r="AK126" s="9"/>
       <c r="AL126" s="9"/>
       <c r="AM126" s="12" t="n">
@@ -13170,13 +13181,13 @@
         <v>124</v>
       </c>
       <c r="AO126" s="12"/>
-      <c r="AP126" s="33" t="s">
+      <c r="AP126" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ126" s="12"/>
     </row>
     <row r="127" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="37" t="n">
+      <c r="A127" s="39" t="n">
         <v>126</v>
       </c>
       <c r="B127" s="12" t="s">
@@ -13210,7 +13221,7 @@
       <c r="N127" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="O127" s="48" t="s">
+      <c r="O127" s="49" t="s">
         <v>399</v>
       </c>
       <c r="P127" s="27"/>
@@ -13226,7 +13237,7 @@
       <c r="V127" s="12"/>
       <c r="W127" s="12"/>
       <c r="X127" s="9"/>
-      <c r="Y127" s="37" t="s">
+      <c r="Y127" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z127" s="12"/>
@@ -13245,7 +13256,7 @@
       <c r="AG127" s="9"/>
       <c r="AH127" s="9"/>
       <c r="AI127" s="9"/>
-      <c r="AJ127" s="37"/>
+      <c r="AJ127" s="39"/>
       <c r="AK127" s="9"/>
       <c r="AL127" s="9"/>
       <c r="AM127" s="12" t="n">
@@ -13255,13 +13266,13 @@
         <v>125</v>
       </c>
       <c r="AO127" s="12"/>
-      <c r="AP127" s="33" t="s">
+      <c r="AP127" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ127" s="12"/>
     </row>
     <row r="128" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="37" t="n">
+      <c r="A128" s="39" t="n">
         <v>127</v>
       </c>
       <c r="B128" s="12" t="s">
@@ -13311,7 +13322,7 @@
       <c r="V128" s="12"/>
       <c r="W128" s="12"/>
       <c r="X128" s="9"/>
-      <c r="Y128" s="37" t="s">
+      <c r="Y128" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z128" s="12"/>
@@ -13330,7 +13341,7 @@
       <c r="AG128" s="9"/>
       <c r="AH128" s="9"/>
       <c r="AI128" s="9"/>
-      <c r="AJ128" s="37"/>
+      <c r="AJ128" s="39"/>
       <c r="AK128" s="9"/>
       <c r="AL128" s="9"/>
       <c r="AM128" s="12" t="n">
@@ -13340,13 +13351,13 @@
         <v>126</v>
       </c>
       <c r="AO128" s="12"/>
-      <c r="AP128" s="33" t="s">
+      <c r="AP128" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ128" s="12"/>
     </row>
     <row r="129" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="37" t="n">
+      <c r="A129" s="39" t="n">
         <v>128</v>
       </c>
       <c r="B129" s="12" t="s">
@@ -13396,7 +13407,7 @@
       <c r="V129" s="12"/>
       <c r="W129" s="12"/>
       <c r="X129" s="9"/>
-      <c r="Y129" s="37" t="s">
+      <c r="Y129" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z129" s="12"/>
@@ -13415,7 +13426,7 @@
       <c r="AG129" s="9"/>
       <c r="AH129" s="9"/>
       <c r="AI129" s="9"/>
-      <c r="AJ129" s="37"/>
+      <c r="AJ129" s="39"/>
       <c r="AK129" s="9"/>
       <c r="AL129" s="9"/>
       <c r="AM129" s="12" t="n">
@@ -13425,13 +13436,13 @@
         <v>127</v>
       </c>
       <c r="AO129" s="12"/>
-      <c r="AP129" s="33" t="s">
+      <c r="AP129" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ129" s="12"/>
     </row>
     <row r="130" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="37" t="n">
+      <c r="A130" s="39" t="n">
         <v>129</v>
       </c>
       <c r="B130" s="12" t="s">
@@ -13481,7 +13492,7 @@
       <c r="V130" s="12"/>
       <c r="W130" s="12"/>
       <c r="X130" s="9"/>
-      <c r="Y130" s="37" t="s">
+      <c r="Y130" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z130" s="12"/>
@@ -13500,7 +13511,7 @@
       <c r="AG130" s="9"/>
       <c r="AH130" s="9"/>
       <c r="AI130" s="9"/>
-      <c r="AJ130" s="37"/>
+      <c r="AJ130" s="39"/>
       <c r="AK130" s="9"/>
       <c r="AL130" s="9"/>
       <c r="AM130" s="12" t="n">
@@ -13510,13 +13521,13 @@
         <v>128</v>
       </c>
       <c r="AO130" s="12"/>
-      <c r="AP130" s="33" t="s">
+      <c r="AP130" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ130" s="12"/>
     </row>
     <row r="131" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="37" t="n">
+      <c r="A131" s="39" t="n">
         <v>130</v>
       </c>
       <c r="B131" s="12" t="s">
@@ -13566,7 +13577,7 @@
       <c r="V131" s="12"/>
       <c r="W131" s="12"/>
       <c r="X131" s="9"/>
-      <c r="Y131" s="37" t="s">
+      <c r="Y131" s="39" t="s">
         <v>369</v>
       </c>
       <c r="Z131" s="12"/>
@@ -13585,7 +13596,7 @@
       <c r="AG131" s="9"/>
       <c r="AH131" s="9"/>
       <c r="AI131" s="9"/>
-      <c r="AJ131" s="37"/>
+      <c r="AJ131" s="39"/>
       <c r="AK131" s="9"/>
       <c r="AL131" s="9"/>
       <c r="AM131" s="12" t="n">
@@ -13595,13 +13606,13 @@
         <v>129</v>
       </c>
       <c r="AO131" s="12"/>
-      <c r="AP131" s="33" t="s">
+      <c r="AP131" s="35" t="s">
         <v>367</v>
       </c>
       <c r="AQ131" s="12"/>
     </row>
     <row r="132" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="37" t="n">
+      <c r="A132" s="39" t="n">
         <v>131</v>
       </c>
       <c r="B132" s="12" t="s">
@@ -13633,7 +13644,7 @@
       <c r="L132" s="9"/>
       <c r="M132" s="9"/>
       <c r="N132" s="12"/>
-      <c r="O132" s="42"/>
+      <c r="O132" s="44"/>
       <c r="P132" s="27"/>
       <c r="Q132" s="27"/>
       <c r="R132" s="9" t="s">
@@ -13645,7 +13656,7 @@
       <c r="V132" s="12"/>
       <c r="W132" s="12"/>
       <c r="X132" s="9"/>
-      <c r="Y132" s="37" t="s">
+      <c r="Y132" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z132" s="12"/>
@@ -13658,7 +13669,7 @@
       <c r="AE132" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="AF132" s="43" t="n">
+      <c r="AF132" s="45" t="n">
         <v>0.5</v>
       </c>
       <c r="AG132" s="9" t="n">
@@ -13667,10 +13678,10 @@
       <c r="AH132" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AI132" s="37" t="s">
+      <c r="AI132" s="39" t="s">
         <v>370</v>
       </c>
-      <c r="AJ132" s="37"/>
+      <c r="AJ132" s="39"/>
       <c r="AK132" s="9"/>
       <c r="AL132" s="9"/>
       <c r="AM132" s="12" t="n">
@@ -13682,13 +13693,13 @@
       <c r="AO132" s="13" t="s">
         <v>413</v>
       </c>
-      <c r="AP132" s="33" t="s">
+      <c r="AP132" s="35" t="s">
         <v>361</v>
       </c>
       <c r="AQ132" s="12"/>
     </row>
     <row r="133" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="37" t="n">
+      <c r="A133" s="39" t="n">
         <v>132</v>
       </c>
       <c r="B133" s="12" t="s">
@@ -13738,7 +13749,7 @@
       <c r="V133" s="12"/>
       <c r="W133" s="12"/>
       <c r="X133" s="9"/>
-      <c r="Y133" s="37" t="s">
+      <c r="Y133" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z133" s="12"/>
@@ -13757,7 +13768,7 @@
       <c r="AG133" s="9"/>
       <c r="AH133" s="9"/>
       <c r="AI133" s="9"/>
-      <c r="AJ133" s="37"/>
+      <c r="AJ133" s="39"/>
       <c r="AK133" s="9"/>
       <c r="AL133" s="9"/>
       <c r="AM133" s="12" t="n">
@@ -13767,13 +13778,13 @@
         <v>131</v>
       </c>
       <c r="AO133" s="12"/>
-      <c r="AP133" s="33" t="s">
+      <c r="AP133" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ133" s="12"/>
     </row>
     <row r="134" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="37" t="n">
+      <c r="A134" s="39" t="n">
         <v>133</v>
       </c>
       <c r="B134" s="12" t="s">
@@ -13823,7 +13834,7 @@
       <c r="V134" s="12"/>
       <c r="W134" s="12"/>
       <c r="X134" s="9"/>
-      <c r="Y134" s="37" t="s">
+      <c r="Y134" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z134" s="12"/>
@@ -13842,7 +13853,7 @@
       <c r="AG134" s="9"/>
       <c r="AH134" s="9"/>
       <c r="AI134" s="9"/>
-      <c r="AJ134" s="37"/>
+      <c r="AJ134" s="39"/>
       <c r="AK134" s="9"/>
       <c r="AL134" s="9"/>
       <c r="AM134" s="12" t="n">
@@ -13852,13 +13863,13 @@
         <v>132</v>
       </c>
       <c r="AO134" s="12"/>
-      <c r="AP134" s="33" t="s">
+      <c r="AP134" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ134" s="12"/>
     </row>
     <row r="135" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="37" t="n">
+      <c r="A135" s="39" t="n">
         <v>134</v>
       </c>
       <c r="B135" s="12" t="s">
@@ -13908,7 +13919,7 @@
       <c r="V135" s="12"/>
       <c r="W135" s="12"/>
       <c r="X135" s="9"/>
-      <c r="Y135" s="37" t="s">
+      <c r="Y135" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z135" s="12"/>
@@ -13927,7 +13938,7 @@
       <c r="AG135" s="9"/>
       <c r="AH135" s="9"/>
       <c r="AI135" s="9"/>
-      <c r="AJ135" s="37"/>
+      <c r="AJ135" s="39"/>
       <c r="AK135" s="9"/>
       <c r="AL135" s="9"/>
       <c r="AM135" s="12" t="n">
@@ -13937,13 +13948,13 @@
         <v>133</v>
       </c>
       <c r="AO135" s="12"/>
-      <c r="AP135" s="33" t="s">
+      <c r="AP135" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ135" s="12"/>
     </row>
     <row r="136" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="37" t="n">
+      <c r="A136" s="39" t="n">
         <v>135</v>
       </c>
       <c r="B136" s="12" t="s">
@@ -13993,7 +14004,7 @@
       <c r="V136" s="12"/>
       <c r="W136" s="12"/>
       <c r="X136" s="9"/>
-      <c r="Y136" s="37" t="s">
+      <c r="Y136" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z136" s="12"/>
@@ -14012,7 +14023,7 @@
       <c r="AG136" s="9"/>
       <c r="AH136" s="9"/>
       <c r="AI136" s="9"/>
-      <c r="AJ136" s="37"/>
+      <c r="AJ136" s="39"/>
       <c r="AK136" s="9"/>
       <c r="AL136" s="9"/>
       <c r="AM136" s="12" t="n">
@@ -14022,13 +14033,13 @@
         <v>134</v>
       </c>
       <c r="AO136" s="12"/>
-      <c r="AP136" s="33" t="s">
+      <c r="AP136" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ136" s="12"/>
     </row>
     <row r="137" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="37" t="n">
+      <c r="A137" s="39" t="n">
         <v>136</v>
       </c>
       <c r="B137" s="12" t="s">
@@ -14078,7 +14089,7 @@
       <c r="V137" s="12"/>
       <c r="W137" s="12"/>
       <c r="X137" s="9"/>
-      <c r="Y137" s="37" t="s">
+      <c r="Y137" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z137" s="12"/>
@@ -14097,7 +14108,7 @@
       <c r="AG137" s="9"/>
       <c r="AH137" s="9"/>
       <c r="AI137" s="9"/>
-      <c r="AJ137" s="37"/>
+      <c r="AJ137" s="39"/>
       <c r="AK137" s="9"/>
       <c r="AL137" s="9"/>
       <c r="AM137" s="12" t="n">
@@ -14107,13 +14118,13 @@
         <v>135</v>
       </c>
       <c r="AO137" s="12"/>
-      <c r="AP137" s="33" t="s">
+      <c r="AP137" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ137" s="12"/>
     </row>
     <row r="138" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="37" t="n">
+      <c r="A138" s="39" t="n">
         <v>137</v>
       </c>
       <c r="B138" s="12" t="s">
@@ -14163,7 +14174,7 @@
       <c r="V138" s="12"/>
       <c r="W138" s="12"/>
       <c r="X138" s="9"/>
-      <c r="Y138" s="37" t="s">
+      <c r="Y138" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z138" s="12"/>
@@ -14182,7 +14193,7 @@
       <c r="AG138" s="9"/>
       <c r="AH138" s="9"/>
       <c r="AI138" s="9"/>
-      <c r="AJ138" s="37"/>
+      <c r="AJ138" s="39"/>
       <c r="AK138" s="9"/>
       <c r="AL138" s="9"/>
       <c r="AM138" s="12" t="n">
@@ -14192,13 +14203,13 @@
         <v>136</v>
       </c>
       <c r="AO138" s="12"/>
-      <c r="AP138" s="33" t="s">
+      <c r="AP138" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ138" s="12"/>
     </row>
     <row r="139" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="37" t="n">
+      <c r="A139" s="39" t="n">
         <v>138</v>
       </c>
       <c r="B139" s="12" t="s">
@@ -14248,7 +14259,7 @@
       <c r="V139" s="12"/>
       <c r="W139" s="12"/>
       <c r="X139" s="9"/>
-      <c r="Y139" s="37" t="s">
+      <c r="Y139" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z139" s="12"/>
@@ -14267,7 +14278,7 @@
       <c r="AG139" s="9"/>
       <c r="AH139" s="9"/>
       <c r="AI139" s="9"/>
-      <c r="AJ139" s="37"/>
+      <c r="AJ139" s="39"/>
       <c r="AK139" s="9"/>
       <c r="AL139" s="9"/>
       <c r="AM139" s="12" t="n">
@@ -14277,13 +14288,13 @@
         <v>137</v>
       </c>
       <c r="AO139" s="12"/>
-      <c r="AP139" s="33" t="s">
+      <c r="AP139" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ139" s="12"/>
     </row>
     <row r="140" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="37" t="n">
+      <c r="A140" s="39" t="n">
         <v>139</v>
       </c>
       <c r="B140" s="12" t="s">
@@ -14333,7 +14344,7 @@
       <c r="V140" s="12"/>
       <c r="W140" s="12"/>
       <c r="X140" s="9"/>
-      <c r="Y140" s="37" t="s">
+      <c r="Y140" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z140" s="12"/>
@@ -14352,7 +14363,7 @@
       <c r="AG140" s="9"/>
       <c r="AH140" s="9"/>
       <c r="AI140" s="9"/>
-      <c r="AJ140" s="37"/>
+      <c r="AJ140" s="39"/>
       <c r="AK140" s="9"/>
       <c r="AL140" s="9"/>
       <c r="AM140" s="12" t="n">
@@ -14362,13 +14373,13 @@
         <v>138</v>
       </c>
       <c r="AO140" s="12"/>
-      <c r="AP140" s="33" t="s">
+      <c r="AP140" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ140" s="12"/>
     </row>
     <row r="141" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="37" t="n">
+      <c r="A141" s="39" t="n">
         <v>140</v>
       </c>
       <c r="B141" s="12" t="s">
@@ -14418,7 +14429,7 @@
       <c r="V141" s="12"/>
       <c r="W141" s="12"/>
       <c r="X141" s="9"/>
-      <c r="Y141" s="37" t="s">
+      <c r="Y141" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z141" s="12"/>
@@ -14437,7 +14448,7 @@
       <c r="AG141" s="9"/>
       <c r="AH141" s="9"/>
       <c r="AI141" s="9"/>
-      <c r="AJ141" s="37"/>
+      <c r="AJ141" s="39"/>
       <c r="AK141" s="9"/>
       <c r="AL141" s="9"/>
       <c r="AM141" s="12" t="n">
@@ -14447,13 +14458,13 @@
         <v>139</v>
       </c>
       <c r="AO141" s="12"/>
-      <c r="AP141" s="33" t="s">
+      <c r="AP141" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ141" s="12"/>
     </row>
     <row r="142" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="37" t="n">
+      <c r="A142" s="39" t="n">
         <v>141</v>
       </c>
       <c r="B142" s="12" t="s">
@@ -14503,7 +14514,7 @@
       <c r="V142" s="12"/>
       <c r="W142" s="12"/>
       <c r="X142" s="9"/>
-      <c r="Y142" s="37" t="s">
+      <c r="Y142" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z142" s="12"/>
@@ -14522,7 +14533,7 @@
       <c r="AG142" s="9"/>
       <c r="AH142" s="9"/>
       <c r="AI142" s="9"/>
-      <c r="AJ142" s="37"/>
+      <c r="AJ142" s="39"/>
       <c r="AK142" s="9"/>
       <c r="AL142" s="9"/>
       <c r="AM142" s="12" t="n">
@@ -14532,13 +14543,13 @@
         <v>140</v>
       </c>
       <c r="AO142" s="12"/>
-      <c r="AP142" s="33" t="s">
+      <c r="AP142" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ142" s="12"/>
     </row>
     <row r="143" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="37" t="n">
+      <c r="A143" s="39" t="n">
         <v>142</v>
       </c>
       <c r="B143" s="12" t="s">
@@ -14588,7 +14599,7 @@
       <c r="V143" s="12"/>
       <c r="W143" s="12"/>
       <c r="X143" s="9"/>
-      <c r="Y143" s="37" t="s">
+      <c r="Y143" s="39" t="s">
         <v>412</v>
       </c>
       <c r="Z143" s="12"/>
@@ -14607,7 +14618,7 @@
       <c r="AG143" s="9"/>
       <c r="AH143" s="9"/>
       <c r="AI143" s="9"/>
-      <c r="AJ143" s="37"/>
+      <c r="AJ143" s="39"/>
       <c r="AK143" s="9"/>
       <c r="AL143" s="9"/>
       <c r="AM143" s="12" t="n">
@@ -14617,13 +14628,13 @@
         <v>141</v>
       </c>
       <c r="AO143" s="12"/>
-      <c r="AP143" s="33" t="s">
+      <c r="AP143" s="35" t="s">
         <v>410</v>
       </c>
       <c r="AQ143" s="12"/>
     </row>
     <row r="144" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="37" t="n">
+      <c r="A144" s="39" t="n">
         <v>143</v>
       </c>
       <c r="B144" s="12" t="s">
@@ -14655,7 +14666,7 @@
       <c r="L144" s="9"/>
       <c r="M144" s="9"/>
       <c r="N144" s="12"/>
-      <c r="O144" s="42"/>
+      <c r="O144" s="44"/>
       <c r="P144" s="27"/>
       <c r="Q144" s="27"/>
       <c r="R144" s="9" t="s">
@@ -14667,7 +14678,7 @@
       <c r="V144" s="12"/>
       <c r="W144" s="12"/>
       <c r="X144" s="9"/>
-      <c r="Y144" s="37" t="s">
+      <c r="Y144" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z144" s="12"/>
@@ -14680,7 +14691,7 @@
       <c r="AE144" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="AF144" s="43" t="n">
+      <c r="AF144" s="45" t="n">
         <v>0.5</v>
       </c>
       <c r="AG144" s="9" t="n">
@@ -14689,10 +14700,10 @@
       <c r="AH144" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="AI144" s="37" t="s">
+      <c r="AI144" s="39" t="s">
         <v>370</v>
       </c>
-      <c r="AJ144" s="37"/>
+      <c r="AJ144" s="39"/>
       <c r="AK144" s="9"/>
       <c r="AL144" s="9"/>
       <c r="AM144" s="12" t="n">
@@ -14704,13 +14715,13 @@
       <c r="AO144" s="13" t="s">
         <v>439</v>
       </c>
-      <c r="AP144" s="33" t="s">
+      <c r="AP144" s="35" t="s">
         <v>361</v>
       </c>
       <c r="AQ144" s="12"/>
     </row>
     <row r="145" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="37" t="n">
+      <c r="A145" s="39" t="n">
         <v>144</v>
       </c>
       <c r="B145" s="12" t="s">
@@ -14760,7 +14771,7 @@
       <c r="V145" s="12"/>
       <c r="W145" s="12"/>
       <c r="X145" s="9"/>
-      <c r="Y145" s="37" t="s">
+      <c r="Y145" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z145" s="12"/>
@@ -14779,7 +14790,7 @@
       <c r="AG145" s="9"/>
       <c r="AH145" s="9"/>
       <c r="AI145" s="9"/>
-      <c r="AJ145" s="37"/>
+      <c r="AJ145" s="39"/>
       <c r="AK145" s="9"/>
       <c r="AL145" s="9"/>
       <c r="AM145" s="12" t="n">
@@ -14789,13 +14800,13 @@
         <v>143</v>
       </c>
       <c r="AO145" s="12"/>
-      <c r="AP145" s="33" t="s">
+      <c r="AP145" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ145" s="12"/>
     </row>
     <row r="146" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="37" t="n">
+      <c r="A146" s="39" t="n">
         <v>145</v>
       </c>
       <c r="B146" s="12" t="s">
@@ -14845,7 +14856,7 @@
       <c r="V146" s="12"/>
       <c r="W146" s="12"/>
       <c r="X146" s="9"/>
-      <c r="Y146" s="37" t="s">
+      <c r="Y146" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z146" s="12"/>
@@ -14864,7 +14875,7 @@
       <c r="AG146" s="9"/>
       <c r="AH146" s="9"/>
       <c r="AI146" s="9"/>
-      <c r="AJ146" s="37"/>
+      <c r="AJ146" s="39"/>
       <c r="AK146" s="9"/>
       <c r="AL146" s="9"/>
       <c r="AM146" s="12" t="n">
@@ -14874,13 +14885,13 @@
         <v>144</v>
       </c>
       <c r="AO146" s="12"/>
-      <c r="AP146" s="33" t="s">
+      <c r="AP146" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ146" s="12"/>
     </row>
     <row r="147" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="37" t="n">
+      <c r="A147" s="39" t="n">
         <v>146</v>
       </c>
       <c r="B147" s="12" t="s">
@@ -14930,7 +14941,7 @@
       <c r="V147" s="12"/>
       <c r="W147" s="12"/>
       <c r="X147" s="9"/>
-      <c r="Y147" s="37" t="s">
+      <c r="Y147" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z147" s="12"/>
@@ -14949,7 +14960,7 @@
       <c r="AG147" s="9"/>
       <c r="AH147" s="9"/>
       <c r="AI147" s="9"/>
-      <c r="AJ147" s="37"/>
+      <c r="AJ147" s="39"/>
       <c r="AK147" s="9"/>
       <c r="AL147" s="9"/>
       <c r="AM147" s="12" t="n">
@@ -14959,13 +14970,13 @@
         <v>145</v>
       </c>
       <c r="AO147" s="12"/>
-      <c r="AP147" s="33" t="s">
+      <c r="AP147" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ147" s="12"/>
     </row>
     <row r="148" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="37" t="n">
+      <c r="A148" s="39" t="n">
         <v>147</v>
       </c>
       <c r="B148" s="12" t="s">
@@ -15015,7 +15026,7 @@
       <c r="V148" s="12"/>
       <c r="W148" s="12"/>
       <c r="X148" s="9"/>
-      <c r="Y148" s="37" t="s">
+      <c r="Y148" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z148" s="12"/>
@@ -15034,7 +15045,7 @@
       <c r="AG148" s="9"/>
       <c r="AH148" s="9"/>
       <c r="AI148" s="9"/>
-      <c r="AJ148" s="37"/>
+      <c r="AJ148" s="39"/>
       <c r="AK148" s="9"/>
       <c r="AL148" s="9"/>
       <c r="AM148" s="12" t="n">
@@ -15044,13 +15055,13 @@
         <v>146</v>
       </c>
       <c r="AO148" s="12"/>
-      <c r="AP148" s="33" t="s">
+      <c r="AP148" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ148" s="12"/>
     </row>
     <row r="149" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="37" t="n">
+      <c r="A149" s="39" t="n">
         <v>148</v>
       </c>
       <c r="B149" s="12" t="s">
@@ -15100,7 +15111,7 @@
       <c r="V149" s="12"/>
       <c r="W149" s="12"/>
       <c r="X149" s="9"/>
-      <c r="Y149" s="37" t="s">
+      <c r="Y149" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z149" s="12"/>
@@ -15119,7 +15130,7 @@
       <c r="AG149" s="9"/>
       <c r="AH149" s="9"/>
       <c r="AI149" s="9"/>
-      <c r="AJ149" s="37"/>
+      <c r="AJ149" s="39"/>
       <c r="AK149" s="9"/>
       <c r="AL149" s="9"/>
       <c r="AM149" s="12" t="n">
@@ -15129,13 +15140,13 @@
         <v>147</v>
       </c>
       <c r="AO149" s="12"/>
-      <c r="AP149" s="33" t="s">
+      <c r="AP149" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ149" s="12"/>
     </row>
     <row r="150" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="37" t="n">
+      <c r="A150" s="39" t="n">
         <v>149</v>
       </c>
       <c r="B150" s="12" t="s">
@@ -15185,7 +15196,7 @@
       <c r="V150" s="12"/>
       <c r="W150" s="12"/>
       <c r="X150" s="9"/>
-      <c r="Y150" s="37" t="s">
+      <c r="Y150" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z150" s="12"/>
@@ -15204,7 +15215,7 @@
       <c r="AG150" s="9"/>
       <c r="AH150" s="9"/>
       <c r="AI150" s="9"/>
-      <c r="AJ150" s="37"/>
+      <c r="AJ150" s="39"/>
       <c r="AK150" s="9"/>
       <c r="AL150" s="9"/>
       <c r="AM150" s="12" t="n">
@@ -15214,13 +15225,13 @@
         <v>148</v>
       </c>
       <c r="AO150" s="12"/>
-      <c r="AP150" s="33" t="s">
+      <c r="AP150" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ150" s="12"/>
     </row>
     <row r="151" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="37" t="n">
+      <c r="A151" s="39" t="n">
         <v>150</v>
       </c>
       <c r="B151" s="12" t="s">
@@ -15270,7 +15281,7 @@
       <c r="V151" s="12"/>
       <c r="W151" s="12"/>
       <c r="X151" s="9"/>
-      <c r="Y151" s="37" t="s">
+      <c r="Y151" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z151" s="12"/>
@@ -15289,7 +15300,7 @@
       <c r="AG151" s="9"/>
       <c r="AH151" s="9"/>
       <c r="AI151" s="9"/>
-      <c r="AJ151" s="37"/>
+      <c r="AJ151" s="39"/>
       <c r="AK151" s="9"/>
       <c r="AL151" s="9"/>
       <c r="AM151" s="12" t="n">
@@ -15299,13 +15310,13 @@
         <v>149</v>
       </c>
       <c r="AO151" s="12"/>
-      <c r="AP151" s="33" t="s">
+      <c r="AP151" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ151" s="12"/>
     </row>
     <row r="152" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="37" t="n">
+      <c r="A152" s="39" t="n">
         <v>151</v>
       </c>
       <c r="B152" s="12" t="s">
@@ -15355,7 +15366,7 @@
       <c r="V152" s="12"/>
       <c r="W152" s="12"/>
       <c r="X152" s="9"/>
-      <c r="Y152" s="37" t="s">
+      <c r="Y152" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z152" s="12"/>
@@ -15374,7 +15385,7 @@
       <c r="AG152" s="9"/>
       <c r="AH152" s="9"/>
       <c r="AI152" s="9"/>
-      <c r="AJ152" s="37"/>
+      <c r="AJ152" s="39"/>
       <c r="AK152" s="9"/>
       <c r="AL152" s="9"/>
       <c r="AM152" s="12" t="n">
@@ -15384,13 +15395,13 @@
         <v>150</v>
       </c>
       <c r="AO152" s="12"/>
-      <c r="AP152" s="33" t="s">
+      <c r="AP152" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ152" s="12"/>
     </row>
     <row r="153" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="37" t="n">
+      <c r="A153" s="39" t="n">
         <v>152</v>
       </c>
       <c r="B153" s="12" t="s">
@@ -15440,7 +15451,7 @@
       <c r="V153" s="12"/>
       <c r="W153" s="12"/>
       <c r="X153" s="9"/>
-      <c r="Y153" s="37" t="s">
+      <c r="Y153" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z153" s="12"/>
@@ -15459,7 +15470,7 @@
       <c r="AG153" s="9"/>
       <c r="AH153" s="9"/>
       <c r="AI153" s="9"/>
-      <c r="AJ153" s="37"/>
+      <c r="AJ153" s="39"/>
       <c r="AK153" s="9"/>
       <c r="AL153" s="9"/>
       <c r="AM153" s="12" t="n">
@@ -15469,13 +15480,13 @@
         <v>151</v>
       </c>
       <c r="AO153" s="12"/>
-      <c r="AP153" s="33" t="s">
+      <c r="AP153" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ153" s="12"/>
     </row>
     <row r="154" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A154" s="37" t="n">
+      <c r="A154" s="39" t="n">
         <v>153</v>
       </c>
       <c r="B154" s="12" t="s">
@@ -15525,7 +15536,7 @@
       <c r="V154" s="12"/>
       <c r="W154" s="12"/>
       <c r="X154" s="9"/>
-      <c r="Y154" s="37" t="s">
+      <c r="Y154" s="39" t="s">
         <v>438</v>
       </c>
       <c r="Z154" s="12"/>
@@ -15544,7 +15555,7 @@
       <c r="AG154" s="9"/>
       <c r="AH154" s="9"/>
       <c r="AI154" s="9"/>
-      <c r="AJ154" s="37"/>
+      <c r="AJ154" s="39"/>
       <c r="AK154" s="9"/>
       <c r="AL154" s="9"/>
       <c r="AM154" s="12" t="n">
@@ -15554,13 +15565,13 @@
         <v>152</v>
       </c>
       <c r="AO154" s="12"/>
-      <c r="AP154" s="33" t="s">
+      <c r="AP154" s="35" t="s">
         <v>436</v>
       </c>
       <c r="AQ154" s="12"/>
     </row>
     <row r="155" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="37" t="n">
+      <c r="A155" s="39" t="n">
         <v>154</v>
       </c>
       <c r="B155" s="12" t="s">
@@ -15637,13 +15648,13 @@
         <v>153</v>
       </c>
       <c r="AO155" s="12"/>
-      <c r="AP155" s="33" t="s">
+      <c r="AP155" s="35" t="s">
         <v>356</v>
       </c>
       <c r="AQ155" s="12"/>
     </row>
     <row r="156" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="37" t="n">
+      <c r="A156" s="39" t="n">
         <v>155</v>
       </c>
       <c r="B156" s="12" t="s">
@@ -15655,68 +15666,68 @@
       <c r="D156" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E156" s="49" t="s">
+      <c r="E156" s="50" t="s">
         <v>469</v>
       </c>
-      <c r="F156" s="49" t="s">
+      <c r="F156" s="50" t="s">
         <v>470</v>
       </c>
-      <c r="G156" s="33" t="s">
+      <c r="G156" s="35" t="s">
         <v>308</v>
       </c>
-      <c r="H156" s="50" t="s">
+      <c r="H156" s="51" t="s">
         <v>471</v>
       </c>
-      <c r="I156" s="51" t="s">
+      <c r="I156" s="52" t="s">
         <v>472</v>
       </c>
-      <c r="J156" s="51" t="s">
+      <c r="J156" s="52" t="s">
         <v>473</v>
       </c>
-      <c r="K156" s="51"/>
-      <c r="L156" s="51"/>
+      <c r="K156" s="52"/>
+      <c r="L156" s="52"/>
       <c r="M156" s="21"/>
       <c r="N156" s="21"/>
-      <c r="O156" s="51"/>
-      <c r="P156" s="51"/>
-      <c r="Q156" s="51"/>
-      <c r="R156" s="51"/>
-      <c r="S156" s="51" t="s">
+      <c r="O156" s="52"/>
+      <c r="P156" s="52"/>
+      <c r="Q156" s="52"/>
+      <c r="R156" s="52"/>
+      <c r="S156" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="T156" s="51"/>
-      <c r="U156" s="51"/>
-      <c r="V156" s="51"/>
-      <c r="W156" s="51"/>
-      <c r="X156" s="51"/>
-      <c r="Y156" s="51"/>
-      <c r="Z156" s="51"/>
-      <c r="AA156" s="51"/>
-      <c r="AB156" s="51"/>
-      <c r="AC156" s="51"/>
-      <c r="AD156" s="51"/>
-      <c r="AE156" s="51"/>
-      <c r="AF156" s="52" t="n">
+      <c r="T156" s="52"/>
+      <c r="U156" s="52"/>
+      <c r="V156" s="52"/>
+      <c r="W156" s="52"/>
+      <c r="X156" s="52"/>
+      <c r="Y156" s="52"/>
+      <c r="Z156" s="52"/>
+      <c r="AA156" s="52"/>
+      <c r="AB156" s="52"/>
+      <c r="AC156" s="52"/>
+      <c r="AD156" s="52"/>
+      <c r="AE156" s="52"/>
+      <c r="AF156" s="53" t="n">
         <v>0</v>
       </c>
-      <c r="AG156" s="51"/>
-      <c r="AH156" s="51"/>
-      <c r="AI156" s="51"/>
-      <c r="AJ156" s="51"/>
-      <c r="AK156" s="51"/>
-      <c r="AL156" s="51"/>
-      <c r="AM156" s="51"/>
+      <c r="AG156" s="52"/>
+      <c r="AH156" s="52"/>
+      <c r="AI156" s="52"/>
+      <c r="AJ156" s="52"/>
+      <c r="AK156" s="52"/>
+      <c r="AL156" s="52"/>
+      <c r="AM156" s="52"/>
       <c r="AN156" s="12" t="n">
         <v>154</v>
       </c>
-      <c r="AO156" s="51" t="n">
+      <c r="AO156" s="52" t="n">
         <v>101</v>
       </c>
-      <c r="AP156" s="51"/>
-      <c r="AQ156" s="51"/>
+      <c r="AP156" s="52"/>
+      <c r="AQ156" s="52"/>
     </row>
     <row r="157" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="37" t="n">
+      <c r="A157" s="39" t="n">
         <v>156</v>
       </c>
       <c r="B157" s="12" t="s">
@@ -15728,66 +15739,66 @@
       <c r="D157" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E157" s="49" t="s">
+      <c r="E157" s="50" t="s">
         <v>475</v>
       </c>
-      <c r="F157" s="49" t="s">
+      <c r="F157" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="G157" s="49" t="s">
+      <c r="G157" s="50" t="s">
         <v>356</v>
       </c>
-      <c r="H157" s="50"/>
-      <c r="I157" s="51" t="s">
+      <c r="H157" s="51"/>
+      <c r="I157" s="52" t="s">
         <v>477</v>
       </c>
-      <c r="J157" s="51" t="s">
+      <c r="J157" s="52" t="s">
         <v>478</v>
       </c>
-      <c r="K157" s="51"/>
-      <c r="L157" s="51"/>
+      <c r="K157" s="52"/>
+      <c r="L157" s="52"/>
       <c r="M157" s="21"/>
       <c r="N157" s="21"/>
-      <c r="O157" s="51"/>
-      <c r="P157" s="51"/>
-      <c r="Q157" s="51"/>
-      <c r="R157" s="51"/>
-      <c r="S157" s="51" t="s">
+      <c r="O157" s="52"/>
+      <c r="P157" s="52"/>
+      <c r="Q157" s="52"/>
+      <c r="R157" s="52"/>
+      <c r="S157" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="T157" s="51"/>
-      <c r="U157" s="51"/>
-      <c r="V157" s="51"/>
-      <c r="W157" s="51"/>
-      <c r="X157" s="51"/>
-      <c r="Y157" s="51"/>
-      <c r="Z157" s="51"/>
-      <c r="AA157" s="51"/>
-      <c r="AB157" s="51"/>
-      <c r="AC157" s="51"/>
-      <c r="AD157" s="51"/>
-      <c r="AE157" s="51"/>
-      <c r="AF157" s="52" t="n">
+      <c r="T157" s="52"/>
+      <c r="U157" s="52"/>
+      <c r="V157" s="52"/>
+      <c r="W157" s="52"/>
+      <c r="X157" s="52"/>
+      <c r="Y157" s="52"/>
+      <c r="Z157" s="52"/>
+      <c r="AA157" s="52"/>
+      <c r="AB157" s="52"/>
+      <c r="AC157" s="52"/>
+      <c r="AD157" s="52"/>
+      <c r="AE157" s="52"/>
+      <c r="AF157" s="53" t="n">
         <v>0</v>
       </c>
-      <c r="AG157" s="51"/>
-      <c r="AH157" s="51"/>
-      <c r="AI157" s="51"/>
-      <c r="AJ157" s="51"/>
-      <c r="AK157" s="51"/>
-      <c r="AL157" s="51"/>
-      <c r="AM157" s="51"/>
+      <c r="AG157" s="52"/>
+      <c r="AH157" s="52"/>
+      <c r="AI157" s="52"/>
+      <c r="AJ157" s="52"/>
+      <c r="AK157" s="52"/>
+      <c r="AL157" s="52"/>
+      <c r="AM157" s="52"/>
       <c r="AN157" s="12" t="n">
         <v>155</v>
       </c>
       <c r="AO157" s="21" t="s">
         <v>479</v>
       </c>
-      <c r="AP157" s="51"/>
-      <c r="AQ157" s="51"/>
+      <c r="AP157" s="52"/>
+      <c r="AQ157" s="52"/>
     </row>
     <row r="158" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="37" t="n">
+      <c r="A158" s="39" t="n">
         <v>157</v>
       </c>
       <c r="B158" s="12" t="s">
@@ -15799,68 +15810,68 @@
       <c r="D158" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E158" s="49" t="s">
+      <c r="E158" s="50" t="s">
         <v>480</v>
       </c>
-      <c r="F158" s="49" t="s">
+      <c r="F158" s="50" t="s">
         <v>481</v>
       </c>
-      <c r="G158" s="49" t="s">
+      <c r="G158" s="50" t="s">
         <v>323</v>
       </c>
-      <c r="H158" s="50" t="s">
+      <c r="H158" s="51" t="s">
         <v>482</v>
       </c>
-      <c r="I158" s="51" t="s">
+      <c r="I158" s="52" t="s">
         <v>472</v>
       </c>
-      <c r="J158" s="51" t="s">
+      <c r="J158" s="52" t="s">
         <v>478</v>
       </c>
-      <c r="K158" s="51"/>
-      <c r="L158" s="51"/>
+      <c r="K158" s="52"/>
+      <c r="L158" s="52"/>
       <c r="M158" s="21"/>
       <c r="N158" s="21"/>
-      <c r="O158" s="51"/>
-      <c r="P158" s="51"/>
-      <c r="Q158" s="51"/>
-      <c r="R158" s="51"/>
-      <c r="S158" s="51" t="s">
+      <c r="O158" s="52"/>
+      <c r="P158" s="52"/>
+      <c r="Q158" s="52"/>
+      <c r="R158" s="52"/>
+      <c r="S158" s="52" t="s">
         <v>474</v>
       </c>
-      <c r="T158" s="51"/>
-      <c r="U158" s="51"/>
-      <c r="V158" s="51"/>
-      <c r="W158" s="51"/>
-      <c r="X158" s="51"/>
-      <c r="Y158" s="51"/>
-      <c r="Z158" s="51"/>
-      <c r="AA158" s="51"/>
-      <c r="AB158" s="51"/>
-      <c r="AC158" s="51"/>
-      <c r="AD158" s="51"/>
-      <c r="AE158" s="51"/>
-      <c r="AF158" s="52" t="n">
+      <c r="T158" s="52"/>
+      <c r="U158" s="52"/>
+      <c r="V158" s="52"/>
+      <c r="W158" s="52"/>
+      <c r="X158" s="52"/>
+      <c r="Y158" s="52"/>
+      <c r="Z158" s="52"/>
+      <c r="AA158" s="52"/>
+      <c r="AB158" s="52"/>
+      <c r="AC158" s="52"/>
+      <c r="AD158" s="52"/>
+      <c r="AE158" s="52"/>
+      <c r="AF158" s="53" t="n">
         <v>0</v>
       </c>
-      <c r="AG158" s="51"/>
-      <c r="AH158" s="51"/>
-      <c r="AI158" s="51"/>
-      <c r="AJ158" s="51"/>
-      <c r="AK158" s="51"/>
-      <c r="AL158" s="51"/>
-      <c r="AM158" s="51"/>
+      <c r="AG158" s="52"/>
+      <c r="AH158" s="52"/>
+      <c r="AI158" s="52"/>
+      <c r="AJ158" s="52"/>
+      <c r="AK158" s="52"/>
+      <c r="AL158" s="52"/>
+      <c r="AM158" s="52"/>
       <c r="AN158" s="12" t="n">
         <v>156</v>
       </c>
-      <c r="AO158" s="51" t="n">
+      <c r="AO158" s="52" t="n">
         <v>105</v>
       </c>
-      <c r="AP158" s="51"/>
-      <c r="AQ158" s="51"/>
+      <c r="AP158" s="52"/>
+      <c r="AQ158" s="52"/>
     </row>
     <row r="159" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="37" t="n">
+      <c r="A159" s="39" t="n">
         <v>158</v>
       </c>
       <c r="B159" s="12" t="s">
@@ -15872,70 +15883,70 @@
       <c r="D159" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E159" s="49" t="s">
+      <c r="E159" s="50" t="s">
         <v>483</v>
       </c>
-      <c r="F159" s="49" t="s">
+      <c r="F159" s="50" t="s">
         <v>484</v>
       </c>
-      <c r="G159" s="49" t="s">
+      <c r="G159" s="50" t="s">
         <v>485</v>
       </c>
-      <c r="H159" s="51"/>
+      <c r="H159" s="52"/>
       <c r="I159" s="21" t="s">
         <v>486</v>
       </c>
       <c r="J159" s="21" t="s">
         <v>478</v>
       </c>
-      <c r="K159" s="51"/>
-      <c r="L159" s="51"/>
+      <c r="K159" s="52"/>
+      <c r="L159" s="52"/>
       <c r="M159" s="21"/>
       <c r="N159" s="21"/>
-      <c r="O159" s="51" t="s">
+      <c r="O159" s="52" t="s">
         <v>487</v>
       </c>
-      <c r="P159" s="51"/>
-      <c r="Q159" s="51"/>
-      <c r="R159" s="51"/>
-      <c r="S159" s="51" t="s">
+      <c r="P159" s="52"/>
+      <c r="Q159" s="52"/>
+      <c r="R159" s="52"/>
+      <c r="S159" s="52" t="s">
         <v>488</v>
       </c>
-      <c r="T159" s="51"/>
-      <c r="U159" s="51"/>
-      <c r="V159" s="51"/>
-      <c r="W159" s="51"/>
-      <c r="X159" s="53" t="s">
+      <c r="T159" s="52"/>
+      <c r="U159" s="52"/>
+      <c r="V159" s="52"/>
+      <c r="W159" s="52"/>
+      <c r="X159" s="54" t="s">
         <v>339</v>
       </c>
-      <c r="Y159" s="54" t="s">
+      <c r="Y159" s="55" t="s">
         <v>489</v>
       </c>
-      <c r="Z159" s="51"/>
-      <c r="AA159" s="51"/>
-      <c r="AB159" s="51"/>
-      <c r="AC159" s="51"/>
-      <c r="AD159" s="51"/>
-      <c r="AE159" s="51"/>
-      <c r="AF159" s="55" t="n">
+      <c r="Z159" s="52"/>
+      <c r="AA159" s="52"/>
+      <c r="AB159" s="52"/>
+      <c r="AC159" s="52"/>
+      <c r="AD159" s="52"/>
+      <c r="AE159" s="52"/>
+      <c r="AF159" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AG159" s="51"/>
-      <c r="AH159" s="51"/>
-      <c r="AI159" s="51"/>
-      <c r="AJ159" s="51"/>
-      <c r="AK159" s="51"/>
-      <c r="AL159" s="51"/>
-      <c r="AM159" s="51"/>
+      <c r="AG159" s="52"/>
+      <c r="AH159" s="52"/>
+      <c r="AI159" s="52"/>
+      <c r="AJ159" s="52"/>
+      <c r="AK159" s="52"/>
+      <c r="AL159" s="52"/>
+      <c r="AM159" s="52"/>
       <c r="AN159" s="12" t="n">
         <v>157</v>
       </c>
-      <c r="AO159" s="51"/>
-      <c r="AP159" s="51"/>
-      <c r="AQ159" s="51"/>
+      <c r="AO159" s="52"/>
+      <c r="AP159" s="52"/>
+      <c r="AQ159" s="52"/>
     </row>
     <row r="160" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="37" t="n">
+      <c r="A160" s="39" t="n">
         <v>159</v>
       </c>
       <c r="B160" s="12" t="s">
@@ -15947,68 +15958,68 @@
       <c r="D160" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E160" s="49" t="s">
+      <c r="E160" s="50" t="s">
         <v>490</v>
       </c>
-      <c r="F160" s="49" t="s">
+      <c r="F160" s="50" t="s">
         <v>491</v>
       </c>
-      <c r="G160" s="49" t="s">
+      <c r="G160" s="50" t="s">
         <v>492</v>
       </c>
-      <c r="H160" s="51"/>
+      <c r="H160" s="52"/>
       <c r="I160" s="21" t="s">
         <v>493</v>
       </c>
       <c r="J160" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="K160" s="51"/>
-      <c r="L160" s="51"/>
+      <c r="K160" s="52"/>
+      <c r="L160" s="52"/>
       <c r="M160" s="21"/>
       <c r="N160" s="21"/>
-      <c r="O160" s="51" t="s">
+      <c r="O160" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="P160" s="51"/>
-      <c r="Q160" s="51"/>
-      <c r="R160" s="51"/>
-      <c r="S160" s="51" t="s">
+      <c r="P160" s="52"/>
+      <c r="Q160" s="52"/>
+      <c r="R160" s="52"/>
+      <c r="S160" s="52" t="s">
         <v>488</v>
       </c>
-      <c r="T160" s="51"/>
-      <c r="U160" s="51"/>
-      <c r="V160" s="51"/>
-      <c r="W160" s="51"/>
-      <c r="X160" s="51"/>
+      <c r="T160" s="52"/>
+      <c r="U160" s="52"/>
+      <c r="V160" s="52"/>
+      <c r="W160" s="52"/>
+      <c r="X160" s="52"/>
       <c r="Y160" s="21" t="s">
         <v>495</v>
       </c>
-      <c r="Z160" s="51"/>
-      <c r="AA160" s="51"/>
-      <c r="AB160" s="51"/>
-      <c r="AC160" s="51"/>
-      <c r="AD160" s="51"/>
-      <c r="AE160" s="51"/>
-      <c r="AF160" s="55" t="n">
+      <c r="Z160" s="52"/>
+      <c r="AA160" s="52"/>
+      <c r="AB160" s="52"/>
+      <c r="AC160" s="52"/>
+      <c r="AD160" s="52"/>
+      <c r="AE160" s="52"/>
+      <c r="AF160" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AG160" s="51"/>
-      <c r="AH160" s="51"/>
-      <c r="AI160" s="51"/>
-      <c r="AJ160" s="51"/>
-      <c r="AK160" s="51"/>
-      <c r="AL160" s="51"/>
-      <c r="AM160" s="51"/>
+      <c r="AG160" s="52"/>
+      <c r="AH160" s="52"/>
+      <c r="AI160" s="52"/>
+      <c r="AJ160" s="52"/>
+      <c r="AK160" s="52"/>
+      <c r="AL160" s="52"/>
+      <c r="AM160" s="52"/>
       <c r="AN160" s="12" t="n">
         <v>158</v>
       </c>
-      <c r="AO160" s="51"/>
-      <c r="AP160" s="51"/>
-      <c r="AQ160" s="51"/>
+      <c r="AO160" s="52"/>
+      <c r="AP160" s="52"/>
+      <c r="AQ160" s="52"/>
     </row>
     <row r="161" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="37" t="n">
+      <c r="A161" s="39" t="n">
         <v>160</v>
       </c>
       <c r="B161" s="12" t="s">
@@ -16020,68 +16031,68 @@
       <c r="D161" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E161" s="49" t="s">
+      <c r="E161" s="50" t="s">
         <v>496</v>
       </c>
-      <c r="F161" s="49" t="s">
+      <c r="F161" s="50" t="s">
         <v>497</v>
       </c>
-      <c r="G161" s="49" t="s">
+      <c r="G161" s="50" t="s">
         <v>498</v>
       </c>
-      <c r="H161" s="51"/>
+      <c r="H161" s="52"/>
       <c r="I161" s="21" t="s">
         <v>493</v>
       </c>
       <c r="J161" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="K161" s="51"/>
-      <c r="L161" s="51"/>
+      <c r="K161" s="52"/>
+      <c r="L161" s="52"/>
       <c r="M161" s="21"/>
       <c r="N161" s="21"/>
-      <c r="O161" s="51" t="s">
+      <c r="O161" s="52" t="s">
         <v>499</v>
       </c>
-      <c r="P161" s="51"/>
-      <c r="Q161" s="51"/>
-      <c r="R161" s="51"/>
-      <c r="S161" s="51" t="s">
+      <c r="P161" s="52"/>
+      <c r="Q161" s="52"/>
+      <c r="R161" s="52"/>
+      <c r="S161" s="52" t="s">
         <v>488</v>
       </c>
-      <c r="T161" s="51"/>
-      <c r="U161" s="51"/>
-      <c r="V161" s="51"/>
-      <c r="W161" s="51"/>
-      <c r="X161" s="51"/>
+      <c r="T161" s="52"/>
+      <c r="U161" s="52"/>
+      <c r="V161" s="52"/>
+      <c r="W161" s="52"/>
+      <c r="X161" s="52"/>
       <c r="Y161" s="21" t="s">
         <v>495</v>
       </c>
-      <c r="Z161" s="51"/>
-      <c r="AA161" s="51"/>
-      <c r="AB161" s="51"/>
-      <c r="AC161" s="51"/>
-      <c r="AD161" s="51"/>
-      <c r="AE161" s="51"/>
-      <c r="AF161" s="55" t="n">
+      <c r="Z161" s="52"/>
+      <c r="AA161" s="52"/>
+      <c r="AB161" s="52"/>
+      <c r="AC161" s="52"/>
+      <c r="AD161" s="52"/>
+      <c r="AE161" s="52"/>
+      <c r="AF161" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AG161" s="51"/>
-      <c r="AH161" s="51"/>
-      <c r="AI161" s="51"/>
-      <c r="AJ161" s="51"/>
-      <c r="AK161" s="51"/>
-      <c r="AL161" s="51"/>
-      <c r="AM161" s="51"/>
+      <c r="AG161" s="52"/>
+      <c r="AH161" s="52"/>
+      <c r="AI161" s="52"/>
+      <c r="AJ161" s="52"/>
+      <c r="AK161" s="52"/>
+      <c r="AL161" s="52"/>
+      <c r="AM161" s="52"/>
       <c r="AN161" s="12" t="n">
         <v>159</v>
       </c>
-      <c r="AO161" s="51"/>
-      <c r="AP161" s="51"/>
-      <c r="AQ161" s="51"/>
+      <c r="AO161" s="52"/>
+      <c r="AP161" s="52"/>
+      <c r="AQ161" s="52"/>
     </row>
     <row r="162" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="37" t="n">
+      <c r="A162" s="39" t="n">
         <v>161</v>
       </c>
       <c r="B162" s="12" t="s">
@@ -16093,68 +16104,68 @@
       <c r="D162" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E162" s="49" t="s">
+      <c r="E162" s="50" t="s">
         <v>500</v>
       </c>
-      <c r="F162" s="49" t="s">
+      <c r="F162" s="50" t="s">
         <v>501</v>
       </c>
-      <c r="G162" s="49" t="s">
+      <c r="G162" s="50" t="s">
         <v>502</v>
       </c>
-      <c r="H162" s="51"/>
+      <c r="H162" s="52"/>
       <c r="I162" s="21" t="s">
         <v>493</v>
       </c>
       <c r="J162" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="K162" s="51"/>
-      <c r="L162" s="51"/>
+      <c r="K162" s="52"/>
+      <c r="L162" s="52"/>
       <c r="M162" s="21"/>
       <c r="N162" s="21"/>
-      <c r="O162" s="51" t="s">
+      <c r="O162" s="52" t="s">
         <v>503</v>
       </c>
-      <c r="P162" s="51"/>
-      <c r="Q162" s="51"/>
-      <c r="R162" s="51"/>
-      <c r="S162" s="51" t="s">
+      <c r="P162" s="52"/>
+      <c r="Q162" s="52"/>
+      <c r="R162" s="52"/>
+      <c r="S162" s="52" t="s">
         <v>488</v>
       </c>
-      <c r="T162" s="51"/>
-      <c r="U162" s="51"/>
-      <c r="V162" s="51"/>
-      <c r="W162" s="51"/>
-      <c r="X162" s="51"/>
+      <c r="T162" s="52"/>
+      <c r="U162" s="52"/>
+      <c r="V162" s="52"/>
+      <c r="W162" s="52"/>
+      <c r="X162" s="52"/>
       <c r="Y162" s="21" t="s">
         <v>495</v>
       </c>
-      <c r="Z162" s="51"/>
-      <c r="AA162" s="51"/>
-      <c r="AB162" s="51"/>
-      <c r="AC162" s="51"/>
-      <c r="AD162" s="51"/>
-      <c r="AE162" s="51"/>
-      <c r="AF162" s="55" t="n">
+      <c r="Z162" s="52"/>
+      <c r="AA162" s="52"/>
+      <c r="AB162" s="52"/>
+      <c r="AC162" s="52"/>
+      <c r="AD162" s="52"/>
+      <c r="AE162" s="52"/>
+      <c r="AF162" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AG162" s="51"/>
-      <c r="AH162" s="51"/>
-      <c r="AI162" s="51"/>
-      <c r="AJ162" s="51"/>
-      <c r="AK162" s="51"/>
+      <c r="AG162" s="52"/>
+      <c r="AH162" s="52"/>
+      <c r="AI162" s="52"/>
+      <c r="AJ162" s="52"/>
+      <c r="AK162" s="52"/>
       <c r="AL162" s="12"/>
-      <c r="AM162" s="51"/>
+      <c r="AM162" s="52"/>
       <c r="AN162" s="12" t="n">
         <v>160</v>
       </c>
-      <c r="AO162" s="51"/>
-      <c r="AP162" s="51"/>
-      <c r="AQ162" s="51"/>
+      <c r="AO162" s="52"/>
+      <c r="AP162" s="52"/>
+      <c r="AQ162" s="52"/>
     </row>
     <row r="163" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="37" t="n">
+      <c r="A163" s="39" t="n">
         <v>162</v>
       </c>
       <c r="B163" s="12" t="s">
@@ -16166,16 +16177,16 @@
       <c r="D163" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E163" s="49" t="s">
+      <c r="E163" s="50" t="s">
         <v>504</v>
       </c>
-      <c r="F163" s="49" t="s">
+      <c r="F163" s="50" t="s">
         <v>505</v>
       </c>
-      <c r="G163" s="49" t="s">
+      <c r="G163" s="50" t="s">
         <v>506</v>
       </c>
-      <c r="H163" s="51" t="s">
+      <c r="H163" s="52" t="s">
         <v>246</v>
       </c>
       <c r="I163" s="21" t="s">
@@ -16184,54 +16195,54 @@
       <c r="J163" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="K163" s="51"/>
-      <c r="L163" s="51"/>
+      <c r="K163" s="52"/>
+      <c r="L163" s="52"/>
       <c r="M163" s="21"/>
       <c r="N163" s="21"/>
       <c r="O163" s="21" t="s">
         <v>508</v>
       </c>
-      <c r="P163" s="51"/>
-      <c r="Q163" s="51"/>
-      <c r="R163" s="51"/>
-      <c r="S163" s="51" t="s">
+      <c r="P163" s="52"/>
+      <c r="Q163" s="52"/>
+      <c r="R163" s="52"/>
+      <c r="S163" s="52" t="s">
         <v>488</v>
       </c>
-      <c r="T163" s="51"/>
-      <c r="U163" s="51"/>
-      <c r="V163" s="51"/>
-      <c r="W163" s="51"/>
-      <c r="X163" s="51"/>
+      <c r="T163" s="52"/>
+      <c r="U163" s="52"/>
+      <c r="V163" s="52"/>
+      <c r="W163" s="52"/>
+      <c r="X163" s="52"/>
       <c r="Y163" s="21" t="s">
         <v>509</v>
       </c>
-      <c r="Z163" s="51"/>
-      <c r="AA163" s="51"/>
-      <c r="AB163" s="51"/>
-      <c r="AC163" s="51"/>
-      <c r="AD163" s="51"/>
-      <c r="AE163" s="51"/>
-      <c r="AF163" s="55" t="n">
+      <c r="Z163" s="52"/>
+      <c r="AA163" s="52"/>
+      <c r="AB163" s="52"/>
+      <c r="AC163" s="52"/>
+      <c r="AD163" s="52"/>
+      <c r="AE163" s="52"/>
+      <c r="AF163" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AG163" s="51"/>
-      <c r="AH163" s="51"/>
-      <c r="AI163" s="51"/>
-      <c r="AJ163" s="51"/>
-      <c r="AK163" s="51"/>
-      <c r="AL163" s="51"/>
-      <c r="AM163" s="51"/>
+      <c r="AG163" s="52"/>
+      <c r="AH163" s="52"/>
+      <c r="AI163" s="52"/>
+      <c r="AJ163" s="52"/>
+      <c r="AK163" s="52"/>
+      <c r="AL163" s="52"/>
+      <c r="AM163" s="52"/>
       <c r="AN163" s="12" t="n">
         <v>161</v>
       </c>
-      <c r="AO163" s="51" t="n">
+      <c r="AO163" s="52" t="n">
         <v>83</v>
       </c>
-      <c r="AP163" s="51"/>
-      <c r="AQ163" s="51"/>
+      <c r="AP163" s="52"/>
+      <c r="AQ163" s="52"/>
     </row>
     <row r="164" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="37" t="n">
+      <c r="A164" s="39" t="n">
         <v>163</v>
       </c>
       <c r="B164" s="12" t="s">
@@ -16243,16 +16254,16 @@
       <c r="D164" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E164" s="49" t="s">
+      <c r="E164" s="50" t="s">
         <v>504</v>
       </c>
-      <c r="F164" s="49" t="s">
+      <c r="F164" s="50" t="s">
         <v>505</v>
       </c>
-      <c r="G164" s="49" t="s">
+      <c r="G164" s="50" t="s">
         <v>506</v>
       </c>
-      <c r="H164" s="51" t="s">
+      <c r="H164" s="52" t="s">
         <v>274</v>
       </c>
       <c r="I164" s="21" t="s">
@@ -16261,54 +16272,54 @@
       <c r="J164" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="K164" s="51"/>
-      <c r="L164" s="51"/>
+      <c r="K164" s="52"/>
+      <c r="L164" s="52"/>
       <c r="M164" s="21"/>
       <c r="N164" s="21"/>
       <c r="O164" s="21" t="s">
         <v>508</v>
       </c>
-      <c r="P164" s="51"/>
-      <c r="Q164" s="51"/>
-      <c r="R164" s="51"/>
-      <c r="S164" s="51" t="s">
+      <c r="P164" s="52"/>
+      <c r="Q164" s="52"/>
+      <c r="R164" s="52"/>
+      <c r="S164" s="52" t="s">
         <v>488</v>
       </c>
-      <c r="T164" s="51"/>
-      <c r="U164" s="51"/>
-      <c r="V164" s="51"/>
-      <c r="W164" s="51"/>
-      <c r="X164" s="51"/>
+      <c r="T164" s="52"/>
+      <c r="U164" s="52"/>
+      <c r="V164" s="52"/>
+      <c r="W164" s="52"/>
+      <c r="X164" s="52"/>
       <c r="Y164" s="21" t="s">
         <v>510</v>
       </c>
-      <c r="Z164" s="51"/>
-      <c r="AA164" s="51"/>
-      <c r="AB164" s="51"/>
-      <c r="AC164" s="51"/>
-      <c r="AD164" s="51"/>
-      <c r="AE164" s="51"/>
-      <c r="AF164" s="55" t="n">
+      <c r="Z164" s="52"/>
+      <c r="AA164" s="52"/>
+      <c r="AB164" s="52"/>
+      <c r="AC164" s="52"/>
+      <c r="AD164" s="52"/>
+      <c r="AE164" s="52"/>
+      <c r="AF164" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AG164" s="51"/>
-      <c r="AH164" s="51"/>
-      <c r="AI164" s="51"/>
-      <c r="AJ164" s="51"/>
-      <c r="AK164" s="51"/>
-      <c r="AL164" s="51"/>
-      <c r="AM164" s="51"/>
+      <c r="AG164" s="52"/>
+      <c r="AH164" s="52"/>
+      <c r="AI164" s="52"/>
+      <c r="AJ164" s="52"/>
+      <c r="AK164" s="52"/>
+      <c r="AL164" s="52"/>
+      <c r="AM164" s="52"/>
       <c r="AN164" s="12" t="n">
         <v>162</v>
       </c>
-      <c r="AO164" s="51" t="n">
+      <c r="AO164" s="52" t="n">
         <v>91</v>
       </c>
-      <c r="AP164" s="51"/>
-      <c r="AQ164" s="51"/>
+      <c r="AP164" s="52"/>
+      <c r="AQ164" s="52"/>
     </row>
     <row r="165" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="37" t="n">
+      <c r="A165" s="39" t="n">
         <v>164</v>
       </c>
       <c r="B165" s="12" t="s">
@@ -16320,16 +16331,16 @@
       <c r="D165" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E165" s="49" t="s">
+      <c r="E165" s="50" t="s">
         <v>504</v>
       </c>
-      <c r="F165" s="49" t="s">
+      <c r="F165" s="50" t="s">
         <v>505</v>
       </c>
-      <c r="G165" s="49" t="s">
+      <c r="G165" s="50" t="s">
         <v>506</v>
       </c>
-      <c r="H165" s="51" t="s">
+      <c r="H165" s="52" t="s">
         <v>265</v>
       </c>
       <c r="I165" s="21" t="s">
@@ -16338,54 +16349,54 @@
       <c r="J165" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="K165" s="51"/>
-      <c r="L165" s="51"/>
+      <c r="K165" s="52"/>
+      <c r="L165" s="52"/>
       <c r="M165" s="21"/>
       <c r="N165" s="21"/>
       <c r="O165" s="21" t="s">
         <v>508</v>
       </c>
-      <c r="P165" s="51"/>
-      <c r="Q165" s="51"/>
-      <c r="R165" s="51"/>
-      <c r="S165" s="51" t="s">
+      <c r="P165" s="52"/>
+      <c r="Q165" s="52"/>
+      <c r="R165" s="52"/>
+      <c r="S165" s="52" t="s">
         <v>488</v>
       </c>
-      <c r="T165" s="51"/>
-      <c r="U165" s="51"/>
-      <c r="V165" s="51"/>
-      <c r="W165" s="51"/>
-      <c r="X165" s="51"/>
+      <c r="T165" s="52"/>
+      <c r="U165" s="52"/>
+      <c r="V165" s="52"/>
+      <c r="W165" s="52"/>
+      <c r="X165" s="52"/>
       <c r="Y165" s="21" t="s">
         <v>511</v>
       </c>
-      <c r="Z165" s="51"/>
-      <c r="AA165" s="51"/>
-      <c r="AB165" s="51"/>
-      <c r="AC165" s="51"/>
-      <c r="AD165" s="51"/>
-      <c r="AE165" s="51"/>
-      <c r="AF165" s="55" t="n">
+      <c r="Z165" s="52"/>
+      <c r="AA165" s="52"/>
+      <c r="AB165" s="52"/>
+      <c r="AC165" s="52"/>
+      <c r="AD165" s="52"/>
+      <c r="AE165" s="52"/>
+      <c r="AF165" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AG165" s="51"/>
-      <c r="AH165" s="51"/>
-      <c r="AI165" s="51"/>
-      <c r="AJ165" s="51"/>
-      <c r="AK165" s="51"/>
-      <c r="AL165" s="51"/>
-      <c r="AM165" s="51"/>
+      <c r="AG165" s="52"/>
+      <c r="AH165" s="52"/>
+      <c r="AI165" s="52"/>
+      <c r="AJ165" s="52"/>
+      <c r="AK165" s="52"/>
+      <c r="AL165" s="52"/>
+      <c r="AM165" s="52"/>
       <c r="AN165" s="12" t="n">
         <v>163</v>
       </c>
-      <c r="AO165" s="51" t="n">
+      <c r="AO165" s="52" t="n">
         <v>88</v>
       </c>
-      <c r="AP165" s="51"/>
-      <c r="AQ165" s="51"/>
+      <c r="AP165" s="52"/>
+      <c r="AQ165" s="52"/>
     </row>
     <row r="166" customFormat="false" ht="30.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A166" s="37" t="n">
+      <c r="A166" s="39" t="n">
         <v>165</v>
       </c>
       <c r="B166" s="12" t="s">
@@ -16397,16 +16408,16 @@
       <c r="D166" s="23" t="s">
         <v>468</v>
       </c>
-      <c r="E166" s="49" t="s">
+      <c r="E166" s="50" t="s">
         <v>504</v>
       </c>
-      <c r="F166" s="49" t="s">
+      <c r="F166" s="50" t="s">
         <v>505</v>
       </c>
-      <c r="G166" s="49" t="s">
+      <c r="G166" s="50" t="s">
         <v>506</v>
       </c>
-      <c r="H166" s="51" t="s">
+      <c r="H166" s="52" t="s">
         <v>289</v>
       </c>
       <c r="I166" s="21" t="s">
@@ -16415,51 +16426,51 @@
       <c r="J166" s="21" t="s">
         <v>494</v>
       </c>
-      <c r="K166" s="51"/>
-      <c r="L166" s="51"/>
+      <c r="K166" s="52"/>
+      <c r="L166" s="52"/>
       <c r="M166" s="21"/>
       <c r="N166" s="21"/>
       <c r="O166" s="21" t="s">
         <v>508</v>
       </c>
-      <c r="P166" s="51"/>
-      <c r="Q166" s="51"/>
-      <c r="R166" s="51"/>
-      <c r="S166" s="51" t="s">
+      <c r="P166" s="52"/>
+      <c r="Q166" s="52"/>
+      <c r="R166" s="52"/>
+      <c r="S166" s="52" t="s">
         <v>488</v>
       </c>
-      <c r="T166" s="51"/>
-      <c r="U166" s="51"/>
-      <c r="V166" s="51"/>
-      <c r="W166" s="51"/>
-      <c r="X166" s="51"/>
+      <c r="T166" s="52"/>
+      <c r="U166" s="52"/>
+      <c r="V166" s="52"/>
+      <c r="W166" s="52"/>
+      <c r="X166" s="52"/>
       <c r="Y166" s="21" t="s">
         <v>512</v>
       </c>
-      <c r="Z166" s="51"/>
-      <c r="AA166" s="51"/>
-      <c r="AB166" s="51"/>
-      <c r="AC166" s="51"/>
-      <c r="AD166" s="51"/>
-      <c r="AE166" s="51"/>
-      <c r="AF166" s="55" t="n">
+      <c r="Z166" s="52"/>
+      <c r="AA166" s="52"/>
+      <c r="AB166" s="52"/>
+      <c r="AC166" s="52"/>
+      <c r="AD166" s="52"/>
+      <c r="AE166" s="52"/>
+      <c r="AF166" s="56" t="n">
         <v>0</v>
       </c>
-      <c r="AG166" s="51"/>
-      <c r="AH166" s="51"/>
-      <c r="AI166" s="51"/>
-      <c r="AJ166" s="51"/>
-      <c r="AK166" s="51"/>
-      <c r="AL166" s="51"/>
-      <c r="AM166" s="51"/>
+      <c r="AG166" s="52"/>
+      <c r="AH166" s="52"/>
+      <c r="AI166" s="52"/>
+      <c r="AJ166" s="52"/>
+      <c r="AK166" s="52"/>
+      <c r="AL166" s="52"/>
+      <c r="AM166" s="52"/>
       <c r="AN166" s="12" t="n">
         <v>164</v>
       </c>
-      <c r="AO166" s="51" t="n">
+      <c r="AO166" s="52" t="n">
         <v>96</v>
       </c>
-      <c r="AP166" s="51"/>
-      <c r="AQ166" s="51"/>
+      <c r="AP166" s="52"/>
+      <c r="AQ166" s="52"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -16519,16 +16530,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="57" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="180" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="57" t="s">
         <v>355</v>
       </c>
     </row>
@@ -16556,7 +16567,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16593,7 +16604,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16630,7 +16641,7 @@
       <c r="A7" s="0" t="s">
         <v>519</v>
       </c>
-      <c r="C7" s="57" t="s">
+      <c r="C7" s="58" t="s">
         <v>520</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -16639,10 +16650,10 @@
       <c r="F7" s="0" t="s">
         <v>521</v>
       </c>
-      <c r="H7" s="57"/>
+      <c r="H7" s="58"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="58" t="s">
         <v>10</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -16651,13 +16662,13 @@
       <c r="F8" s="0" t="s">
         <v>522</v>
       </c>
-      <c r="H8" s="57"/>
+      <c r="H8" s="58"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="57"/>
+      <c r="A10" s="58"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="58" t="s">
         <v>520</v>
       </c>
       <c r="B11" s="0" t="n">
@@ -16668,7 +16679,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="0" t="n">
@@ -16682,21 +16693,21 @@
       <c r="A15" s="0" t="s">
         <v>525</v>
       </c>
-      <c r="E15" s="57"/>
-      <c r="H15" s="57"/>
+      <c r="E15" s="58"/>
+      <c r="H15" s="58"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E16" s="57"/>
-      <c r="H16" s="57"/>
+      <c r="E16" s="58"/>
+      <c r="H16" s="58"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="58" t="s">
         <v>520</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="58" t="s">
         <v>520</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -16707,13 +16718,13 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="57" t="s">
+      <c r="A19" s="58" t="s">
         <v>10</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="58" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -16724,16 +16735,16 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="58" t="s">
         <v>528</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="59" t="s">
         <v>529</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="58" t="s">
         <v>528</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="59" t="s">
         <v>530</v>
       </c>
     </row>
@@ -16748,31 +16759,31 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G25" s="57" t="s">
+      <c r="G25" s="58" t="s">
         <v>520</v>
       </c>
-      <c r="H25" s="59" t="s">
+      <c r="H25" s="60" t="s">
         <v>533</v>
       </c>
-      <c r="J25" s="57"/>
+      <c r="J25" s="58"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G26" s="57" t="s">
+      <c r="G26" s="58" t="s">
         <v>10</v>
       </c>
       <c r="H26" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="J26" s="57"/>
+      <c r="J26" s="58"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="57" t="s">
+      <c r="B28" s="58" t="s">
         <v>520</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="60" t="s">
         <v>533</v>
       </c>
-      <c r="D28" s="57" t="s">
+      <c r="D28" s="58" t="s">
         <v>520</v>
       </c>
       <c r="E28" s="0" t="n">
@@ -16783,13 +16794,13 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="57" t="s">
+      <c r="B29" s="58" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="D29" s="57" t="s">
+      <c r="D29" s="58" t="s">
         <v>10</v>
       </c>
       <c r="E29" s="0" t="n">
@@ -16828,52 +16839,52 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="61" t="s">
+      <c r="D1" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="61" t="s">
+      <c r="F1" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="62" t="s">
         <v>537</v>
       </c>
-      <c r="H1" s="61" t="s">
+      <c r="H1" s="62" t="s">
         <v>538</v>
       </c>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="62" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="61" t="s">
+      <c r="K1" s="62" t="s">
         <v>539</v>
       </c>
-      <c r="L1" s="61" t="s">
+      <c r="L1" s="62" t="s">
         <v>36</v>
       </c>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="62" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="63" t="s">
         <v>540</v>
       </c>
     </row>

</xml_diff>